<commit_message>
Ik ben begonnen met de assetlist maken
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
   <si>
     <t>ID Code</t>
   </si>
@@ -166,16 +166,22 @@
     <t>|</t>
   </si>
   <si>
-    <t>Weapon_HandPistol_1</t>
-  </si>
-  <si>
     <t>Weapon_Shotgun_2</t>
   </si>
   <si>
-    <t>Weapon_Knife_3</t>
+    <t>Weapon_Revolver_1</t>
   </si>
   <si>
-    <t>Weapon_Harpoon_4</t>
+    <t>Weapon_CeremicBlade_3</t>
+  </si>
+  <si>
+    <t>Weapon_AssaultRifle_4</t>
+  </si>
+  <si>
+    <t>Weapon_HarpoonGun_5</t>
+  </si>
+  <si>
+    <t>Weapon_Grenades_6</t>
   </si>
 </sst>
 </file>
@@ -640,10 +646,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Goed" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutraal" xfId="3" builtinId="28"/>
-    <cellStyle name="Ongeldig" xfId="2" builtinId="27"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -666,9 +672,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -706,7 +712,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -778,7 +784,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -954,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1342,7 +1348,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>5</v>
@@ -1389,7 +1395,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>5</v>
@@ -1520,8 +1526,12 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -1572,8 +1582,12 @@
       </c>
     </row>
     <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="35"/>
+      <c r="A20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>

</xml_diff>

<commit_message>
Script map toegevoegd & PSD files in ieder verdieping toegevoegd & Excel consistentie aangepast
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -325,19 +325,19 @@
     <t>???</t>
   </si>
   <si>
-    <t>| AbstractEnemy | AIEnemy | Turret | Roomba | MechanicalArms | LiveStockEnemy | Dogs | Cows | Chickens | Oyster | Plants</t>
-  </si>
-  <si>
-    <t>| PackManager | AbstractPack | StimPack | MedicalPack | AmmoPack | GrenadePack | KeyCards | LootManager | InfoManager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">| Movement | CameraControl | Health | SoundManager | HUDManager | AIShipManager | GameManager | SurvivorManager </t>
-  </si>
-  <si>
-    <t xml:space="preserve">| CodeBreaker | ExplodingBarrel | Lights | WeaponManager | AbstractWeapons | MeleeWeapon | Shotgun | Pistol | HarpoonGun </t>
-  </si>
-  <si>
-    <t>| FlareGun | AssaultRifle | AbstractGrenades | FragGrenades | StunGrenades | SmokeGrenades | AbstractMines</t>
+    <t>| PackManager | AbstractPack | StimPack | MedicalPack | AmmoPack | GrenadePack | KeyCards | LootManager | InfoManager |</t>
+  </si>
+  <si>
+    <t>| AbstractEnemy | AIEnemy | Turret | Roomba | MechanicalArms | LiveStockEnemy | Dogs | Cows | Chickens | Oyster | Plants |</t>
+  </si>
+  <si>
+    <t>| Movement | CameraControl | Health | SoundManager | HUDManager | AIShipManager | GameManager | SurvivorManager |</t>
+  </si>
+  <si>
+    <t>| CodeBreaker | ExplodingBarrel | Lights | WeaponManager | AbstractWeapons | MeleeWeapon | Shotgun | Pistol | HarpoonGun |</t>
+  </si>
+  <si>
+    <t>| FlareGun | AssaultRifle | AbstractGrenades | FragGrenades | StunGrenades | SmokeGrenades | AbstractMines |</t>
   </si>
 </sst>
 </file>
@@ -633,7 +633,7 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -796,7 +796,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1116,8 +1115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,7 +1212,7 @@
       <c r="G2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="59" t="s">
+      <c r="H2" s="58" t="s">
         <v>23</v>
       </c>
       <c r="I2" s="10" t="s">
@@ -1270,10 +1269,10 @@
       <c r="G3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="59" t="s">
+      <c r="H3" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="58" t="s">
+      <c r="I3" s="10" t="s">
         <v>48</v>
       </c>
       <c r="J3" s="11"/>
@@ -1309,10 +1308,10 @@
       <c r="G4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="59" t="s">
+      <c r="H4" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="58" t="s">
+      <c r="I4" s="10" t="s">
         <v>48</v>
       </c>
       <c r="J4" s="11"/>
@@ -1348,10 +1347,10 @@
       <c r="G5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="58" t="s">
+      <c r="I5" s="10" t="s">
         <v>48</v>
       </c>
       <c r="J5" s="11"/>
@@ -1387,10 +1386,10 @@
       <c r="G6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="59" t="s">
+      <c r="H6" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="58" t="s">
+      <c r="I6" s="10" t="s">
         <v>48</v>
       </c>
       <c r="J6" s="11"/>
@@ -1426,10 +1425,10 @@
       <c r="G7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="59" t="s">
+      <c r="H7" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="58" t="s">
+      <c r="I7" s="10" t="s">
         <v>48</v>
       </c>
       <c r="J7" s="11"/>
@@ -1465,10 +1464,10 @@
       <c r="G8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="59" t="s">
+      <c r="H8" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="I8" s="58" t="s">
+      <c r="I8" s="10" t="s">
         <v>48</v>
       </c>
       <c r="J8" s="11"/>
@@ -1491,11 +1490,11 @@
       <c r="G9" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="H9" s="59" t="s">
+      <c r="H9" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="I9" s="58" t="s">
-        <v>103</v>
+      <c r="I9" s="10" t="s">
+        <v>102</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="31"/>
@@ -1522,11 +1521,11 @@
         <v>12</v>
       </c>
       <c r="G10" s="9"/>
-      <c r="H10" s="59" t="s">
+      <c r="H10" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="I10" s="58" t="s">
-        <v>102</v>
+      <c r="I10" s="10" t="s">
+        <v>103</v>
       </c>
       <c r="J10" s="11"/>
       <c r="K10" s="31"/>
@@ -1546,10 +1545,10 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="59" t="s">
+      <c r="H11" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="I11" s="58" t="s">
+      <c r="I11" s="10" t="s">
         <v>104</v>
       </c>
       <c r="J11" s="11"/>
@@ -1574,10 +1573,10 @@
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="59" t="s">
+      <c r="H12" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="I12" s="58" t="s">
+      <c r="I12" s="10" t="s">
         <v>105</v>
       </c>
       <c r="J12" s="11"/>
@@ -1595,10 +1594,10 @@
       <c r="A13" s="5"/>
       <c r="B13" s="35"/>
       <c r="G13" s="9"/>
-      <c r="H13" s="59" t="s">
+      <c r="H13" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="I13" s="58" t="s">
+      <c r="I13" s="10" t="s">
         <v>106</v>
       </c>
       <c r="J13" s="11"/>

</xml_diff>

<commit_message>
Added all assets so far
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="175">
   <si>
     <t>ID Code</t>
   </si>
@@ -154,9 +154,6 @@
     <t>Sprint 9 (20-06 t/m 03-07)</t>
   </si>
   <si>
-    <t>F. Level</t>
-  </si>
-  <si>
     <t>G. HUD Elementen</t>
   </si>
   <si>
@@ -319,9 +316,6 @@
     <t>???</t>
   </si>
   <si>
-    <t>| AbstractEnemy | AIEnemy | Turret | Roomba | MechanicalArms | LiveStockEnemy | Dogs | Cows | Chickens | Oyster | Plants</t>
-  </si>
-  <si>
     <t>| PackManager | AbstractPack | StimPack | MedicalPack | AmmoPack | GrenadePack | KeyCards | LootManager | InfoManager</t>
   </si>
   <si>
@@ -394,9 +388,6 @@
     <t>| BionicLeftArm | RightArm</t>
   </si>
   <si>
-    <t>| MutatedDog | MutatedChicken | Turret | Roomba| Camera | Xenomorph | Plant</t>
-  </si>
-  <si>
     <t>StaticEnviroment_Boxes_1</t>
   </si>
   <si>
@@ -539,6 +530,18 @@
   </si>
   <si>
     <t>HUD_</t>
+  </si>
+  <si>
+    <t>| MutatedDog | MutatedChicken | Turret | Roomba| Camera | Xenomorph | Plant | AIMainFrame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">| AbstractEnemy | AIEnemy | Turret | Roomba | MechanicalArms | LiveStockEnemy | Dogs | Cows | Chickens | Oyster | </t>
+  </si>
+  <si>
+    <t>| Boxes | Corpses | GarbageBin | PropogandePosters | CryoPods | OperatingTable | Plants | OverGrowth | BrokenGlass | DogHouse | ToolBox | Welder | Grinder | Hammer | SconicScrewDriver |  Generator | FusionCore | TelePorter | Computer | AssemblyLine | Fighter | Drone | MinningShip | SpaceSuit | BrokenTurrets | Desks | Chairs | FloodLights| Tires | Warhead | WarheadTrolley | MoonBuggy | Servers | SecurityGates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">| MedPack | StimPack | KeyCards | LorePDA | Barrel | FireExtinguisher | Doors | Boxes | WeaponLockers </t>
   </si>
 </sst>
 </file>
@@ -1317,8 +1320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T721"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A147" sqref="A147"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,7 +1334,7 @@
     <col min="6" max="6" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="121" style="3" customWidth="1"/>
+    <col min="9" max="9" width="255.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" style="3" customWidth="1"/>
     <col min="11" max="11" width="28.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="19" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
@@ -1418,7 +1421,7 @@
         <v>23</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J2" s="11"/>
       <c r="K2" s="12" t="s">
@@ -1475,7 +1478,7 @@
         <v>24</v>
       </c>
       <c r="I3" s="58" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J3" s="11"/>
       <c r="K3" s="16"/>
@@ -1514,7 +1517,7 @@
         <v>25</v>
       </c>
       <c r="I4" s="58" t="s">
-        <v>125</v>
+        <v>171</v>
       </c>
       <c r="J4" s="11"/>
       <c r="K4" s="21"/>
@@ -1553,7 +1556,7 @@
         <v>26</v>
       </c>
       <c r="I5" s="58" t="s">
-        <v>47</v>
+        <v>173</v>
       </c>
       <c r="J5" s="11"/>
       <c r="K5" s="21"/>
@@ -1592,7 +1595,7 @@
         <v>27</v>
       </c>
       <c r="I6" s="58" t="s">
-        <v>47</v>
+        <v>174</v>
       </c>
       <c r="J6" s="11"/>
       <c r="K6" s="21"/>
@@ -1628,10 +1631,10 @@
         <v>28</v>
       </c>
       <c r="H7" s="59" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="I7" s="58" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J7" s="11"/>
       <c r="K7" s="31"/>
@@ -1667,10 +1670,10 @@
         <v>29</v>
       </c>
       <c r="H8" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="58" t="s">
         <v>46</v>
-      </c>
-      <c r="I8" s="58" t="s">
-        <v>47</v>
       </c>
       <c r="J8" s="11"/>
       <c r="K8" s="31"/>
@@ -1690,13 +1693,13 @@
         <v>8</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H9" s="59" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I9" s="58" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="31"/>
@@ -1711,7 +1714,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>5</v>
@@ -1724,10 +1727,10 @@
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="59" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I10" s="58" t="s">
-        <v>100</v>
+        <v>172</v>
       </c>
       <c r="J10" s="11"/>
       <c r="K10" s="31"/>
@@ -1763,7 +1766,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>5</v>
@@ -1773,10 +1776,10 @@
       <c r="E12" s="8"/>
       <c r="G12" s="9"/>
       <c r="H12" s="59" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I12" s="58" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J12" s="11"/>
       <c r="K12" s="31"/>
@@ -1811,7 +1814,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>5</v>
@@ -1821,10 +1824,10 @@
       <c r="E14" s="8"/>
       <c r="G14" s="9"/>
       <c r="H14" s="59" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I14" s="58" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J14" s="11"/>
       <c r="K14" s="31"/>
@@ -1859,17 +1862,17 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>5</v>
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="59" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I16" s="58" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J16" s="11"/>
       <c r="K16" s="31"/>
@@ -1901,7 +1904,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>5</v>
@@ -1911,10 +1914,10 @@
       <c r="E18" s="8"/>
       <c r="G18" s="9"/>
       <c r="H18" s="59" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I18" s="58" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J18" s="11"/>
       <c r="K18" s="31"/>
@@ -1949,7 +1952,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>5</v>
@@ -1993,7 +1996,7 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>5</v>
@@ -2037,7 +2040,7 @@
     </row>
     <row r="24" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>5</v>
@@ -2084,7 +2087,7 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>5</v>
@@ -2159,7 +2162,7 @@
     </row>
     <row r="29" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>5</v>
@@ -2210,7 +2213,7 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>5</v>
@@ -2235,7 +2238,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>5</v>
@@ -2253,7 +2256,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>5</v>
@@ -2271,7 +2274,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>5</v>
@@ -2289,7 +2292,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="35" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>5</v>
@@ -2307,7 +2310,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>5</v>
@@ -2325,7 +2328,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>5</v>
@@ -2343,7 +2346,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>5</v>
@@ -2361,7 +2364,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>5</v>
@@ -2386,7 +2389,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="35" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>5</v>
@@ -2404,7 +2407,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>5</v>
@@ -2422,7 +2425,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>5</v>
@@ -2440,7 +2443,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>5</v>
@@ -2458,7 +2461,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>5</v>
@@ -2476,7 +2479,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="35" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>5</v>
@@ -2494,7 +2497,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>5</v>
@@ -2512,7 +2515,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>5</v>
@@ -2530,7 +2533,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>5</v>
@@ -2548,7 +2551,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>5</v>
@@ -2566,7 +2569,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="35" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>5</v>
@@ -2584,7 +2587,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>5</v>
@@ -2602,7 +2605,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>5</v>
@@ -2620,7 +2623,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>5</v>
@@ -2638,7 +2641,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>5</v>
@@ -2656,7 +2659,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="35" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>5</v>
@@ -2674,7 +2677,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>5</v>
@@ -2692,7 +2695,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>5</v>
@@ -2710,7 +2713,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>5</v>
@@ -2728,7 +2731,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B89" s="6" t="s">
         <v>5</v>
@@ -2746,7 +2749,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="35" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B91" s="6" t="s">
         <v>5</v>
@@ -2764,7 +2767,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>5</v>
@@ -2782,7 +2785,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B95" s="6" t="s">
         <v>5</v>
@@ -2800,7 +2803,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B97" s="6" t="s">
         <v>5</v>
@@ -2818,7 +2821,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B99" s="6" t="s">
         <v>5</v>
@@ -2836,7 +2839,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="35" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B101" s="6" t="s">
         <v>5</v>
@@ -2854,7 +2857,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B103" s="6" t="s">
         <v>5</v>
@@ -2872,7 +2875,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B105" s="6" t="s">
         <v>5</v>
@@ -2890,7 +2893,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B107" s="6" t="s">
         <v>5</v>
@@ -2908,7 +2911,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="35" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B109" s="6" t="s">
         <v>5</v>
@@ -2926,7 +2929,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B111" s="6" t="s">
         <v>5</v>
@@ -2944,7 +2947,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B113" s="6" t="s">
         <v>5</v>
@@ -2962,7 +2965,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B115" s="6" t="s">
         <v>5</v>
@@ -2980,7 +2983,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B117" s="6" t="s">
         <v>5</v>
@@ -2998,7 +3001,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="35" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B119" s="6" t="s">
         <v>5</v>
@@ -3016,7 +3019,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B121" s="6" t="s">
         <v>5</v>
@@ -3041,7 +3044,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="35" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>5</v>
@@ -3059,7 +3062,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>5</v>
@@ -3077,7 +3080,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B128" s="6" t="s">
         <v>5</v>
@@ -3095,7 +3098,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>5</v>
@@ -3113,7 +3116,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>5</v>
@@ -3131,7 +3134,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="35" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B134" s="6" t="s">
         <v>5</v>
@@ -3149,7 +3152,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B136" s="6" t="s">
         <v>5</v>
@@ -3167,7 +3170,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B138" s="6" t="s">
         <v>5</v>
@@ -3185,7 +3188,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B140" s="6" t="s">
         <v>5</v>
@@ -3210,7 +3213,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B143" s="6" t="s">
         <v>5</v>
@@ -3235,7 +3238,7 @@
     </row>
     <row r="146" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A146" s="35" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B146" s="6" t="s">
         <v>5</v>
@@ -3352,16 +3355,16 @@
     </row>
     <row r="161" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B161" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C161" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D161" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D161" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E161" s="8">
         <v>8</v>
@@ -3373,16 +3376,16 @@
     </row>
     <row r="162" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B162" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C162" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D162" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D162" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E162" s="8">
         <v>8</v>
@@ -3421,16 +3424,16 @@
     </row>
     <row r="163" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B163" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C163" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D163" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D163" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E163" s="8">
         <v>6</v>
@@ -3450,16 +3453,16 @@
     </row>
     <row r="164" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B164" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C164" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D164" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D164" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E164" s="8">
         <v>7</v>
@@ -3479,16 +3482,16 @@
     </row>
     <row r="165" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A165" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B165" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C165" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D165" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D165" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E165" s="8">
         <v>8</v>
@@ -3509,16 +3512,16 @@
     </row>
     <row r="166" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B166" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C166" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D166" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D166" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E166" s="8">
         <v>7</v>
@@ -3536,16 +3539,16 @@
     </row>
     <row r="167" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B167" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C167" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D167" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D167" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E167" s="8">
         <v>7</v>
@@ -3563,16 +3566,16 @@
     </row>
     <row r="168" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B168" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C168" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D168" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D168" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E168" s="8">
         <v>7</v>
@@ -3590,16 +3593,16 @@
     </row>
     <row r="169" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B169" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C169" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D169" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D169" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E169" s="8">
         <v>4</v>
@@ -3643,16 +3646,16 @@
     </row>
     <row r="171" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B171" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C171" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D171" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D171" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E171" s="8">
         <v>8</v>
@@ -3679,16 +3682,16 @@
     </row>
     <row r="172" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B172" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C172" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D172" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D172" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E172" s="8">
         <v>7</v>
@@ -3706,16 +3709,16 @@
     </row>
     <row r="173" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B173" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C173" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D173" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D173" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E173" s="8">
         <v>6</v>
@@ -3726,16 +3729,16 @@
     </row>
     <row r="174" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B174" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C174" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D174" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D174" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E174" s="8">
         <v>6</v>
@@ -3756,16 +3759,16 @@
     </row>
     <row r="175" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A175" s="35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B175" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C175" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D175" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D175" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E175" s="8">
         <v>6</v>
@@ -3786,16 +3789,16 @@
     </row>
     <row r="176" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B176" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C176" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D176" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D176" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E176" s="8">
         <v>7</v>
@@ -3816,16 +3819,16 @@
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B177" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C177" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D177" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D177" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E177" s="8">
         <v>6</v>
@@ -3835,16 +3838,16 @@
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B178" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C178" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D178" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D178" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E178" s="8">
         <v>6</v>
@@ -3854,16 +3857,16 @@
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B179" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C179" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D179" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D179" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E179" s="8">
         <v>6</v>
@@ -3871,16 +3874,16 @@
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B180" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C180" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D180" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D180" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E180" s="8">
         <v>4</v>
@@ -3888,16 +3891,16 @@
     </row>
     <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B181" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C181" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D181" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D181" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E181" s="8">
         <v>4</v>
@@ -3912,16 +3915,16 @@
     </row>
     <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B183" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C183" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D183" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D183" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E183" s="8">
         <v>10</v>
@@ -3929,16 +3932,16 @@
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B184" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C184" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D184" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D184" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E184" s="8">
         <v>10</v>
@@ -3946,16 +3949,16 @@
     </row>
     <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B185" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C185" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D185" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D185" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E185" s="8">
         <v>9</v>
@@ -3970,16 +3973,16 @@
     </row>
     <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B187" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C187" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D187" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D187" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E187" s="8">
         <v>7</v>
@@ -3987,16 +3990,16 @@
     </row>
     <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B188" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C188" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D188" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D188" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E188" s="8">
         <v>8</v>
@@ -4004,16 +4007,16 @@
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B189" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C189" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D189" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D189" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E189" s="8">
         <v>9</v>
@@ -4021,16 +4024,16 @@
     </row>
     <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B190" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C190" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D190" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D190" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E190" s="8">
         <v>10</v>
@@ -4038,16 +4041,16 @@
     </row>
     <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B191" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C191" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D191" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D191" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E191" s="8">
         <v>7</v>
@@ -4055,16 +4058,16 @@
     </row>
     <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B192" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C192" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D192" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D192" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E192" s="8">
         <v>4</v>
@@ -4072,16 +4075,16 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B193" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C193" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D193" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D193" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E193" s="8">
         <v>4</v>
@@ -4089,16 +4092,16 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B194" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C194" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D194" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D194" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E194" s="8">
         <v>4</v>
@@ -4113,16 +4116,16 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B196" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C196" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D196" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D196" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E196" s="8">
         <v>5</v>
@@ -4137,16 +4140,16 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B198" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C198" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D198" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D198" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E198" s="8">
         <v>6</v>
@@ -4154,16 +4157,16 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B199" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C199" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D199" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D199" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E199" s="8">
         <v>5</v>
@@ -4171,16 +4174,16 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B200" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C200" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D200" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D200" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E200" s="8">
         <v>5</v>
@@ -4188,16 +4191,16 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B201" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C201" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D201" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D201" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E201" s="8">
         <v>5</v>
@@ -4205,16 +4208,16 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B202" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C202" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D202" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D202" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E202" s="8">
         <v>4</v>
@@ -4229,16 +4232,16 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B204" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C204" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D204" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D204" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E204" s="8">
         <v>10</v>
@@ -4246,16 +4249,16 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B205" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C205" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D205" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D205" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E205" s="8">
         <v>10</v>
@@ -4263,16 +4266,16 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B206" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C206" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D206" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D206" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E206" s="8">
         <v>9</v>
@@ -4280,16 +4283,16 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B207" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C207" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D207" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D207" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E207" s="8">
         <v>7</v>
@@ -4297,16 +4300,16 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B208" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C208" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D208" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D208" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E208" s="8">
         <v>7</v>
@@ -4314,16 +4317,16 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B209" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C209" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D209" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D209" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E209" s="8">
         <v>7</v>
@@ -4331,16 +4334,16 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B210" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C210" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D210" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D210" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E210" s="8">
         <v>9</v>
@@ -4348,16 +4351,16 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B211" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C211" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D211" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D211" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E211" s="8">
         <v>9</v>
@@ -4365,16 +4368,16 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B212" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C212" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D212" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D212" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E212" s="8">
         <v>8</v>
@@ -4382,16 +4385,16 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B213" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C213" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D213" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D213" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E213" s="8">
         <v>8</v>
@@ -4399,16 +4402,16 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B214" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C214" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D214" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D214" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E214" s="8">
         <v>7</v>
@@ -4416,16 +4419,16 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B215" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C215" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D215" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D215" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E215" s="8">
         <v>7</v>
@@ -4433,16 +4436,16 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B216" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C216" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D216" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="D216" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E216" s="8">
         <v>6</v>

</xml_diff>

<commit_message>
Laatste Update Asset List DONE !!
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -2102,8 +2102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1027"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O42" sqref="O42"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2116,7 +2116,7 @@
     <col min="6" max="6" width="16.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.28515625" style="46" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="156.7109375" style="46" customWidth="1"/>
+    <col min="9" max="9" width="166.5703125" style="46" customWidth="1"/>
     <col min="10" max="10" width="28.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="34.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="33.7109375" style="3" bestFit="1" customWidth="1"/>
@@ -3187,36 +3187,15 @@
         <v>10</v>
       </c>
       <c r="G23" s="9"/>
-      <c r="J23" s="10">
-        <v>2363</v>
-      </c>
-      <c r="K23" s="35">
-        <v>263</v>
-      </c>
-      <c r="L23" s="35">
-        <v>263</v>
-      </c>
-      <c r="M23" s="35">
-        <v>261</v>
-      </c>
-      <c r="N23" s="35">
-        <v>259</v>
-      </c>
-      <c r="O23" s="35">
-        <v>256</v>
-      </c>
-      <c r="P23" s="35">
-        <v>260</v>
-      </c>
-      <c r="Q23" s="35">
-        <v>262</v>
-      </c>
-      <c r="R23" s="35">
-        <v>264</v>
-      </c>
-      <c r="S23" s="3">
-        <v>264</v>
-      </c>
+      <c r="J23" s="10"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="35"/>
+      <c r="O23" s="35"/>
+      <c r="P23" s="35"/>
+      <c r="Q23" s="35"/>
+      <c r="R23" s="35"/>
       <c r="T23" s="73">
         <f>T20+T21+T22</f>
         <v>0</v>
@@ -3699,36 +3678,10 @@
       <c r="E36" s="8">
         <v>10</v>
       </c>
-      <c r="J36" s="10">
-        <v>2330</v>
-      </c>
-      <c r="K36" s="35">
-        <v>260</v>
-      </c>
-      <c r="L36" s="35">
-        <v>260</v>
-      </c>
-      <c r="M36" s="3">
-        <v>260</v>
-      </c>
-      <c r="N36" s="3">
-        <v>260</v>
-      </c>
-      <c r="O36" s="3">
-        <v>260</v>
-      </c>
-      <c r="P36" s="3">
-        <v>260</v>
-      </c>
-      <c r="Q36" s="3">
-        <v>260</v>
-      </c>
-      <c r="R36" s="35">
-        <v>260</v>
-      </c>
-      <c r="S36" s="3">
-        <v>250</v>
-      </c>
+      <c r="J36" s="10"/>
+      <c r="K36" s="35"/>
+      <c r="L36" s="35"/>
+      <c r="R36" s="35"/>
       <c r="T36" s="71">
         <f>T34+T35</f>
         <v>0</v>

</xml_diff>

<commit_message>
Presentatie & Uren Registratie
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -2102,21 +2102,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1027"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q42" sqref="Q42"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" style="46" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="166.5703125" style="46" customWidth="1"/>
+    <col min="1" max="1" width="42.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="46" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="164.7109375" style="46" customWidth="1"/>
     <col min="10" max="10" width="28.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="34.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="33.7109375" style="3" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Asset list punten update & Bug gefixed in weapon switch tijdens aimen
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -1559,7 +1559,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1783,6 +1783,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2103,7 +2106,7 @@
   <dimension ref="A1:U1027"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3463,7 +3466,7 @@
         <v>9</v>
       </c>
       <c r="J30" s="10"/>
-      <c r="K30" s="50" t="s">
+      <c r="K30" s="79" t="s">
         <v>242</v>
       </c>
       <c r="L30" s="52" t="s">
@@ -3551,7 +3554,7 @@
         <v>9</v>
       </c>
       <c r="J32" s="1"/>
-      <c r="K32" s="34" t="s">
+      <c r="K32" s="79" t="s">
         <v>250</v>
       </c>
       <c r="L32" s="52" t="s">
@@ -3648,7 +3651,9 @@
       <c r="J35" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="K35" s="37"/>
+      <c r="K35" s="37">
+        <v>20</v>
+      </c>
       <c r="L35" s="37"/>
       <c r="M35" s="37"/>
       <c r="N35" s="37"/>
@@ -3659,7 +3664,7 @@
       <c r="S35" s="37"/>
       <c r="T35" s="72">
         <f>K35+L35+M35+N35+O35+P35+Q35+R35+S35</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3684,7 +3689,7 @@
       <c r="R36" s="35"/>
       <c r="T36" s="71">
         <f>T34+T35</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="U36" s="71" t="s">
         <v>374</v>

</xml_diff>

<commit_message>
Nieuwe Script officiel toegevoegd
UnlockWeapon is nu officieel deel van onze scripts
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$A$1:$E$672</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$A$1:$E$673</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1831" uniqueCount="403">
   <si>
     <t>ID Code</t>
   </si>
@@ -640,9 +640,6 @@
     <t>Enemy_AIMainFrame_9</t>
   </si>
   <si>
-    <t>| PackManager | AbstractPack | StimPack | MedicalPack | AmmoPack | GrenadePack | KeyCards | LootManager | InfoManager |</t>
-  </si>
-  <si>
     <t>| AbstractEnemy | AIEnemy | Turret | Roomba | LiveStockEnemy | Dogs | Chickens | Camera | Proxy | Plants |</t>
   </si>
   <si>
@@ -1223,6 +1220,12 @@
   </si>
   <si>
     <t>HUD_StartScreen_25 (9)</t>
+  </si>
+  <si>
+    <t>Items_UnlockWeapon</t>
+  </si>
+  <si>
+    <t>| PackManager | AbstractPack | StimPack | MedicalPack | AmmoPack | GrenadePack | KeyCards | LootManager | InfoManager |UnlockWeapon |</t>
   </si>
 </sst>
 </file>
@@ -2103,10 +2106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U1027"/>
+  <dimension ref="A1:U1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2157,7 +2160,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I1" s="46" t="s">
         <v>30</v>
@@ -2216,7 +2219,7 @@
         <v>22</v>
       </c>
       <c r="I2" s="47" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="57" t="s">
@@ -2273,35 +2276,35 @@
         <v>23</v>
       </c>
       <c r="I3" s="47" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J3" s="10"/>
       <c r="K3" s="32" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L3" s="74" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="M3" s="74" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="N3" s="78" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="P3" s="51" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="R3" s="51" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="S3" s="78" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -2330,35 +2333,35 @@
         <v>24</v>
       </c>
       <c r="I4" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N4" s="52" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P4" s="50" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="R4" s="50" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="S4" s="52" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -2387,35 +2390,35 @@
         <v>25</v>
       </c>
       <c r="I5" s="47" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L5" s="69" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="N5" s="52" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P5" s="52" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Q5" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="R5" s="52" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="S5" s="50" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -2444,35 +2447,35 @@
         <v>25</v>
       </c>
       <c r="I6" s="47" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="23" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L6" s="69" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="N6" s="52" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P6" s="50" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="R6" s="50" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="S6" s="50" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -2501,35 +2504,35 @@
         <v>25</v>
       </c>
       <c r="I7" s="47" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="23" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L7" s="69" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="N7" s="52" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O7" s="69" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="P7" s="52" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="R7" s="50" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="S7" s="50" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -2558,35 +2561,35 @@
         <v>26</v>
       </c>
       <c r="I8" s="47" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L8" s="69" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="N8" s="58" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="O8" s="69" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="P8" s="50" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="R8" s="50" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="S8" s="50" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -2603,35 +2606,35 @@
         <v>27</v>
       </c>
       <c r="I9" s="47" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="23" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L9" s="69" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="N9" s="56" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="O9" s="69" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="P9" s="50" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q9" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="R9" s="50" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="S9" s="50" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -2658,35 +2661,35 @@
         <v>27</v>
       </c>
       <c r="I10" s="47" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="69" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L10" s="77" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="N10" s="56" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="P10" s="50" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="Q10" s="69" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="R10" s="50" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="S10" s="50" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -2711,33 +2714,33 @@
         <v>41</v>
       </c>
       <c r="I11" s="47" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="23"/>
       <c r="L11" s="14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="M11" s="68" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="N11" s="52" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="P11" s="50" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="Q11" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R11" s="50" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="S11" s="50" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -2761,33 +2764,33 @@
         <v>41</v>
       </c>
       <c r="I12" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="23"/>
       <c r="L12" s="14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="M12" s="69" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N12" s="56" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O12" s="69" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="P12" s="52" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="Q12" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="R12" s="50" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="S12" s="52" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -2811,33 +2814,33 @@
         <v>41</v>
       </c>
       <c r="I13" s="47" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="23"/>
       <c r="L13" s="14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M13" s="69" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="N13" s="52" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O13" s="14" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="P13" s="50" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Q13" s="14" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="R13" s="50" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="S13" s="52" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -2858,34 +2861,34 @@
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="47" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I14" s="47" t="s">
-        <v>207</v>
+        <v>402</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="23"/>
       <c r="L14" s="23"/>
       <c r="M14" s="69" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N14" s="34" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="O14" s="69" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="P14" s="50" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="Q14" s="14" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="R14" s="50" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="S14" s="50" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -2906,26 +2909,26 @@
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="47" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I15" s="47" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="23"/>
       <c r="L15" s="23"/>
       <c r="M15" s="69" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="N15" s="50" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="P15" s="34"/>
       <c r="R15" s="50" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="S15" s="50" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -2946,21 +2949,21 @@
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="47" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I16" s="47" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="23"/>
       <c r="L16" s="23"/>
       <c r="M16" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N16" s="52"/>
       <c r="P16" s="34"/>
       <c r="R16" s="50" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="S16" s="34"/>
     </row>
@@ -2972,10 +2975,10 @@
       <c r="E17" s="8"/>
       <c r="G17" s="9"/>
       <c r="H17" s="47" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I17" s="47" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="23"/>
@@ -2985,7 +2988,7 @@
       <c r="P17" s="52"/>
       <c r="Q17" s="15"/>
       <c r="R17" s="50" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="S17" s="34"/>
     </row>
@@ -3007,10 +3010,10 @@
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="47" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I18" s="47" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="23"/>
@@ -3040,10 +3043,10 @@
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="47" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I19" s="47" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="29"/>
@@ -3077,10 +3080,10 @@
       </c>
       <c r="G20" s="9"/>
       <c r="H20" s="47" t="s">
+        <v>221</v>
+      </c>
+      <c r="I20" s="47" t="s">
         <v>222</v>
-      </c>
-      <c r="I20" s="47" t="s">
-        <v>223</v>
       </c>
       <c r="J20" s="60" t="s">
         <v>19</v>
@@ -3117,10 +3120,10 @@
       </c>
       <c r="G21" s="9"/>
       <c r="H21" s="47" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I21" s="47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J21" s="61" t="s">
         <v>17</v>
@@ -3204,7 +3207,7 @@
         <v>0</v>
       </c>
       <c r="U23" s="71" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3281,31 +3284,31 @@
       <c r="G26" s="9"/>
       <c r="J26" s="10"/>
       <c r="K26" s="57" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L26" s="57" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M26" s="57" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N26" s="57" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="O26" s="57" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P26" s="57" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Q26" s="57" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="R26" s="57" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="S26" s="57" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="T26" s="63"/>
     </row>
@@ -3328,31 +3331,31 @@
       <c r="G27" s="9"/>
       <c r="J27" s="10"/>
       <c r="K27" s="50" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L27" s="50" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M27" s="58" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N27" s="50" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O27" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="P27" s="51" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q27" s="54" t="s">
+        <v>272</v>
+      </c>
+      <c r="R27" s="51" t="s">
         <v>273</v>
       </c>
-      <c r="R27" s="51" t="s">
-        <v>274</v>
-      </c>
       <c r="S27" s="54" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T27" s="63"/>
     </row>
@@ -3375,31 +3378,31 @@
       <c r="G28" s="9"/>
       <c r="H28" s="48"/>
       <c r="K28" s="52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L28" s="50" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M28" s="50" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N28" s="50" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O28" s="26" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="P28" s="56" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Q28" s="52" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="R28" s="50" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="S28" s="50" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="T28" s="63"/>
     </row>
@@ -3421,31 +3424,31 @@
       </c>
       <c r="J29" s="10"/>
       <c r="K29" s="50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L29" s="52" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M29" s="50" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N29" s="56" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="O29" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="P29" s="50" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Q29" s="56" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="R29" s="50" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="S29" s="50" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="T29" s="63"/>
     </row>
@@ -3467,29 +3470,29 @@
       </c>
       <c r="J30" s="10"/>
       <c r="K30" s="79" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L30" s="52" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="M30" s="50" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N30" s="50" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="O30" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P30" s="50" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Q30" s="50"/>
       <c r="R30" s="50" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="S30" s="50" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="T30" s="63"/>
     </row>
@@ -3511,29 +3514,29 @@
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="52" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L31" s="52" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M31" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N31" s="52" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="O31" s="28" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="P31" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Q31" s="52"/>
       <c r="R31" s="50" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="S31" s="52" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T31" s="63"/>
     </row>
@@ -3555,23 +3558,23 @@
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="79" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L32" s="52" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M32" s="50" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N32" s="52" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="O32" s="28"/>
       <c r="P32" s="52"/>
       <c r="Q32" s="52"/>
       <c r="R32" s="50"/>
       <c r="S32" s="52" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="T32" s="63"/>
     </row>
@@ -3586,14 +3589,14 @@
       <c r="L33" s="53"/>
       <c r="M33" s="55"/>
       <c r="N33" s="53" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="O33" s="44"/>
       <c r="P33" s="53"/>
       <c r="Q33" s="53"/>
       <c r="R33" s="55"/>
       <c r="S33" s="53" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="T33" s="63" t="s">
         <v>31</v>
@@ -3692,7 +3695,7 @@
         <v>20</v>
       </c>
       <c r="U36" s="71" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -11312,7 +11315,7 @@
     </row>
     <row r="497" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A497" s="27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B497" s="6" t="s">
         <v>5</v>
@@ -11330,7 +11333,7 @@
     </row>
     <row r="498" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A498" s="27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B498" s="18" t="s">
         <v>10</v>
@@ -12632,34 +12635,34 @@
       <c r="H589" s="49"/>
     </row>
     <row r="590" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A590" s="27"/>
-      <c r="B590" s="27"/>
-      <c r="C590" s="7"/>
-      <c r="D590" s="8"/>
-      <c r="E590" s="8"/>
+      <c r="A590" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="B590" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C590" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D590" s="8">
+        <v>20</v>
+      </c>
+      <c r="E590" s="8">
+        <v>2</v>
+      </c>
       <c r="H590" s="49"/>
     </row>
     <row r="591" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A591" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B591" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C591" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D591" s="8">
-        <v>30</v>
-      </c>
-      <c r="E591" s="8">
-        <v>8</v>
-      </c>
+      <c r="A591" s="27"/>
+      <c r="B591" s="27"/>
+      <c r="C591" s="7"/>
+      <c r="D591" s="8"/>
+      <c r="E591" s="8"/>
       <c r="H591" s="49"/>
     </row>
     <row r="592" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A592" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B592" s="25" t="s">
         <v>11</v>
@@ -12668,16 +12671,16 @@
         <v>89</v>
       </c>
       <c r="D592" s="8">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E592" s="8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H592" s="49"/>
     </row>
     <row r="593" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A593" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B593" s="25" t="s">
         <v>11</v>
@@ -12686,16 +12689,16 @@
         <v>89</v>
       </c>
       <c r="D593" s="8">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E593" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H593" s="49"/>
     </row>
     <row r="594" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A594" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B594" s="25" t="s">
         <v>11</v>
@@ -12704,15 +12707,16 @@
         <v>89</v>
       </c>
       <c r="D594" s="8">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="E594" s="8">
         <v>6</v>
       </c>
+      <c r="H594" s="49"/>
     </row>
     <row r="595" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A595" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B595" s="25" t="s">
         <v>11</v>
@@ -12721,15 +12725,15 @@
         <v>89</v>
       </c>
       <c r="D595" s="8">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E595" s="8">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="596" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A596" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B596" s="25" t="s">
         <v>11</v>
@@ -12738,15 +12742,15 @@
         <v>89</v>
       </c>
       <c r="D596" s="8">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="E596" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="597" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A597" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B597" s="25" t="s">
         <v>11</v>
@@ -12755,7 +12759,7 @@
         <v>89</v>
       </c>
       <c r="D597" s="8">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E597" s="8">
         <v>6</v>
@@ -12763,7 +12767,7 @@
     </row>
     <row r="598" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A598" s="5" t="s">
-        <v>209</v>
+        <v>62</v>
       </c>
       <c r="B598" s="25" t="s">
         <v>11</v>
@@ -12772,15 +12776,15 @@
         <v>89</v>
       </c>
       <c r="D598" s="8">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E598" s="8">
         <v>6</v>
       </c>
     </row>
     <row r="599" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A599" s="4" t="s">
-        <v>210</v>
+      <c r="A599" s="5" t="s">
+        <v>208</v>
       </c>
       <c r="B599" s="25" t="s">
         <v>11</v>
@@ -12789,15 +12793,15 @@
         <v>89</v>
       </c>
       <c r="D599" s="8">
-        <v>80</v>
-      </c>
-      <c r="E599" s="3">
+        <v>50</v>
+      </c>
+      <c r="E599" s="8">
         <v>6</v>
       </c>
     </row>
     <row r="600" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A600" s="5" t="s">
-        <v>63</v>
+      <c r="A600" s="4" t="s">
+        <v>209</v>
       </c>
       <c r="B600" s="25" t="s">
         <v>11</v>
@@ -12806,39 +12810,39 @@
         <v>89</v>
       </c>
       <c r="D600" s="8">
+        <v>80</v>
+      </c>
+      <c r="E600" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="601" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A601" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B601" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C601" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D601" s="8">
         <v>60</v>
       </c>
-      <c r="E600" s="8">
+      <c r="E601" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="601" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A601" s="5"/>
-      <c r="B601" s="27"/>
-      <c r="C601" s="7"/>
-      <c r="D601" s="8"/>
-      <c r="E601" s="8"/>
-    </row>
     <row r="602" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A602" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B602" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C602" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D602" s="8">
-        <v>70</v>
-      </c>
-      <c r="E602" s="8">
-        <v>10</v>
-      </c>
+      <c r="A602" s="5"/>
+      <c r="B602" s="27"/>
+      <c r="C602" s="7"/>
+      <c r="D602" s="8"/>
+      <c r="E602" s="8"/>
     </row>
     <row r="603" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A603" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B603" s="25" t="s">
         <v>11</v>
@@ -12847,15 +12851,15 @@
         <v>89</v>
       </c>
       <c r="D603" s="8">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="E603" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="604" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A604" s="27" t="s">
-        <v>66</v>
+      <c r="A604" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="B604" s="25" t="s">
         <v>11</v>
@@ -12864,15 +12868,15 @@
         <v>89</v>
       </c>
       <c r="D604" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E604" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="605" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A605" s="27" t="s">
-        <v>211</v>
+        <v>66</v>
       </c>
       <c r="B605" s="25" t="s">
         <v>11</v>
@@ -12881,33 +12885,32 @@
         <v>89</v>
       </c>
       <c r="D605" s="8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E605" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="607" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A607" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B607" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="606" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A606" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="B606" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C607" s="7" t="s">
+      <c r="C606" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D607" s="8">
-        <v>30</v>
-      </c>
-      <c r="E607" s="8">
-        <v>7</v>
-      </c>
-      <c r="H607" s="49"/>
+      <c r="D606" s="8">
+        <v>10</v>
+      </c>
+      <c r="E606" s="8">
+        <v>10</v>
+      </c>
     </row>
     <row r="608" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A608" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B608" s="25" t="s">
         <v>11</v>
@@ -12916,16 +12919,16 @@
         <v>89</v>
       </c>
       <c r="D608" s="8">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="E608" s="8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H608" s="49"/>
     </row>
     <row r="609" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A609" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B609" s="25" t="s">
         <v>11</v>
@@ -12934,16 +12937,16 @@
         <v>89</v>
       </c>
       <c r="D609" s="8">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="E609" s="8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H609" s="49"/>
     </row>
     <row r="610" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A610" s="27" t="s">
-        <v>70</v>
+      <c r="A610" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="B610" s="25" t="s">
         <v>11</v>
@@ -12952,16 +12955,16 @@
         <v>89</v>
       </c>
       <c r="D610" s="8">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E610" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H610" s="49"/>
     </row>
     <row r="611" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A611" s="5" t="s">
-        <v>71</v>
+      <c r="A611" s="27" t="s">
+        <v>70</v>
       </c>
       <c r="B611" s="25" t="s">
         <v>11</v>
@@ -12970,16 +12973,16 @@
         <v>89</v>
       </c>
       <c r="D611" s="8">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="E611" s="8">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H611" s="49"/>
     </row>
     <row r="612" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A612" s="5" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="B612" s="25" t="s">
         <v>11</v>
@@ -12988,16 +12991,16 @@
         <v>89</v>
       </c>
       <c r="D612" s="8">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E612" s="8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H612" s="49"/>
     </row>
     <row r="613" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A613" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B613" s="25" t="s">
         <v>11</v>
@@ -13015,7 +13018,7 @@
     </row>
     <row r="614" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A614" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B614" s="25" t="s">
         <v>11</v>
@@ -13029,60 +13032,60 @@
       <c r="E614" s="8">
         <v>4</v>
       </c>
+      <c r="H614" s="49"/>
     </row>
     <row r="615" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A615" s="5"/>
-      <c r="B615" s="27"/>
-      <c r="C615" s="7"/>
-      <c r="D615" s="8"/>
-      <c r="E615" s="8"/>
+      <c r="A615" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B615" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C615" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D615" s="8">
+        <v>40</v>
+      </c>
+      <c r="E615" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="616" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A616" s="5" t="s">
+      <c r="A616" s="5"/>
+      <c r="B616" s="27"/>
+      <c r="C616" s="7"/>
+      <c r="D616" s="8"/>
+      <c r="E616" s="8"/>
+    </row>
+    <row r="617" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A617" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B616" s="25" t="s">
+      <c r="B617" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C616" s="7" t="s">
+      <c r="C617" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D616" s="8">
+      <c r="D617" s="8">
         <v>70</v>
       </c>
-      <c r="E616" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="617" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A617" s="5"/>
-      <c r="B617" s="27"/>
-      <c r="C617" s="7"/>
-      <c r="D617" s="8"/>
-      <c r="E617" s="8"/>
-      <c r="F617" s="43"/>
+      <c r="E617" s="8">
+        <v>5</v>
+      </c>
     </row>
     <row r="618" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A618" s="5" t="s">
+      <c r="A618" s="5"/>
+      <c r="B618" s="27"/>
+      <c r="C618" s="7"/>
+      <c r="D618" s="8"/>
+      <c r="E618" s="8"/>
+      <c r="F618" s="43"/>
+    </row>
+    <row r="619" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A619" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="B618" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C618" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D618" s="8">
-        <v>30</v>
-      </c>
-      <c r="E618" s="8">
-        <v>6</v>
-      </c>
-      <c r="F618" s="43"/>
-    </row>
-    <row r="619" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A619" s="27" t="s">
-        <v>73</v>
       </c>
       <c r="B619" s="25" t="s">
         <v>11</v>
@@ -13094,12 +13097,13 @@
         <v>30</v>
       </c>
       <c r="E619" s="8">
-        <v>5</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F619" s="43"/>
     </row>
     <row r="620" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A620" s="27" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="B620" s="25" t="s">
         <v>11</v>
@@ -13108,7 +13112,7 @@
         <v>89</v>
       </c>
       <c r="D620" s="8">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E620" s="8">
         <v>5</v>
@@ -13116,7 +13120,7 @@
     </row>
     <row r="621" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A621" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B621" s="25" t="s">
         <v>11</v>
@@ -13132,8 +13136,8 @@
       </c>
     </row>
     <row r="622" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A622" s="5" t="s">
-        <v>74</v>
+      <c r="A622" s="27" t="s">
+        <v>92</v>
       </c>
       <c r="B622" s="25" t="s">
         <v>11</v>
@@ -13142,39 +13146,39 @@
         <v>89</v>
       </c>
       <c r="D622" s="8">
+        <v>40</v>
+      </c>
+      <c r="E622" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="623" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A623" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B623" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C623" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D623" s="8">
         <v>20</v>
       </c>
-      <c r="E622" s="8">
+      <c r="E623" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="623" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A623" s="5"/>
-      <c r="B623" s="27"/>
-      <c r="C623" s="7"/>
-      <c r="D623" s="8"/>
-      <c r="E623" s="8"/>
-    </row>
     <row r="624" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A624" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B624" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C624" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D624" s="8">
-        <v>60</v>
-      </c>
-      <c r="E624" s="8">
-        <v>10</v>
-      </c>
+      <c r="A624" s="5"/>
+      <c r="B624" s="27"/>
+      <c r="C624" s="7"/>
+      <c r="D624" s="8"/>
+      <c r="E624" s="8"/>
     </row>
     <row r="625" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A625" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B625" s="25" t="s">
         <v>11</v>
@@ -13183,15 +13187,15 @@
         <v>89</v>
       </c>
       <c r="D625" s="8">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="E625" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A626" s="27" t="s">
-        <v>77</v>
+      <c r="A626" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="B626" s="25" t="s">
         <v>11</v>
@@ -13200,15 +13204,15 @@
         <v>89</v>
       </c>
       <c r="D626" s="8">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E626" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="627" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A627" s="5" t="s">
-        <v>78</v>
+      <c r="A627" s="27" t="s">
+        <v>77</v>
       </c>
       <c r="B627" s="25" t="s">
         <v>11</v>
@@ -13217,15 +13221,15 @@
         <v>89</v>
       </c>
       <c r="D627" s="8">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E627" s="8">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="628" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A628" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B628" s="25" t="s">
         <v>11</v>
@@ -13242,7 +13246,7 @@
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A629" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B629" s="25" t="s">
         <v>11</v>
@@ -13251,7 +13255,7 @@
         <v>89</v>
       </c>
       <c r="D629" s="8">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E629" s="8">
         <v>7</v>
@@ -13259,7 +13263,7 @@
     </row>
     <row r="630" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A630" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B630" s="25" t="s">
         <v>11</v>
@@ -13268,15 +13272,15 @@
         <v>89</v>
       </c>
       <c r="D630" s="8">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E630" s="8">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="631" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A631" s="27" t="s">
-        <v>82</v>
+      <c r="A631" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="B631" s="25" t="s">
         <v>11</v>
@@ -13285,15 +13289,15 @@
         <v>89</v>
       </c>
       <c r="D631" s="8">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E631" s="8">
         <v>9</v>
       </c>
     </row>
     <row r="632" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A632" s="5" t="s">
-        <v>83</v>
+      <c r="A632" s="27" t="s">
+        <v>82</v>
       </c>
       <c r="B632" s="25" t="s">
         <v>11</v>
@@ -13302,15 +13306,15 @@
         <v>89</v>
       </c>
       <c r="D632" s="8">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="E632" s="8">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="633" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A633" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B633" s="25" t="s">
         <v>11</v>
@@ -13319,7 +13323,7 @@
         <v>89</v>
       </c>
       <c r="D633" s="8">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="E633" s="8">
         <v>8</v>
@@ -13327,7 +13331,7 @@
     </row>
     <row r="634" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A634" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B634" s="25" t="s">
         <v>11</v>
@@ -13336,15 +13340,15 @@
         <v>89</v>
       </c>
       <c r="D634" s="8">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="E634" s="8">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="635" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A635" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B635" s="25" t="s">
         <v>11</v>
@@ -13361,7 +13365,7 @@
     </row>
     <row r="636" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A636" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B636" s="25" t="s">
         <v>11</v>
@@ -13373,21 +13377,34 @@
         <v>70</v>
       </c>
       <c r="E636" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="637" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A637" s="4"/>
-      <c r="B637" s="4"/>
-      <c r="C637" s="7"/>
+      <c r="A637" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B637" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C637" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="D637" s="8">
-        <f>SUM(D581:D636)</f>
-        <v>2330</v>
+        <v>70</v>
+      </c>
+      <c r="E637" s="8">
+        <v>6</v>
       </c>
     </row>
     <row r="638" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A638" s="5"/>
-      <c r="B638" s="27"/>
+      <c r="A638" s="4"/>
+      <c r="B638" s="4"/>
+      <c r="C638" s="7"/>
+      <c r="D638" s="8">
+        <f>SUM(D581:D637)</f>
+        <v>2350</v>
+      </c>
     </row>
     <row r="639" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A639" s="5"/>
@@ -13402,11 +13419,11 @@
       <c r="B641" s="27"/>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A642" s="27"/>
+      <c r="A642" s="5"/>
       <c r="B642" s="27"/>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A643" s="5"/>
+      <c r="A643" s="27"/>
       <c r="B643" s="27"/>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.25">
@@ -13438,11 +13455,11 @@
       <c r="B650" s="27"/>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A651" s="27"/>
+      <c r="A651" s="5"/>
       <c r="B651" s="27"/>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A652" s="5"/>
+      <c r="A652" s="27"/>
       <c r="B652" s="27"/>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.25">
@@ -13458,11 +13475,11 @@
       <c r="B655" s="27"/>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A656" s="27"/>
+      <c r="A656" s="5"/>
       <c r="B656" s="27"/>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A657" s="5"/>
+      <c r="A657" s="27"/>
       <c r="B657" s="27"/>
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.25">
@@ -13478,11 +13495,11 @@
       <c r="B660" s="27"/>
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A661" s="27"/>
+      <c r="A661" s="5"/>
       <c r="B661" s="27"/>
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A662" s="5"/>
+      <c r="A662" s="27"/>
       <c r="B662" s="27"/>
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.25">
@@ -13498,11 +13515,11 @@
       <c r="B665" s="27"/>
     </row>
     <row r="666" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A666" s="27"/>
+      <c r="A666" s="5"/>
       <c r="B666" s="27"/>
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A667" s="5"/>
+      <c r="A667" s="27"/>
       <c r="B667" s="27"/>
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.25">
@@ -13518,11 +13535,11 @@
       <c r="B670" s="27"/>
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A671" s="27"/>
+      <c r="A671" s="5"/>
       <c r="B671" s="27"/>
     </row>
     <row r="672" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A672" s="5"/>
+      <c r="A672" s="27"/>
       <c r="B672" s="27"/>
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.25">
@@ -13538,11 +13555,11 @@
       <c r="B675" s="27"/>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A676" s="27"/>
+      <c r="A676" s="5"/>
       <c r="B676" s="27"/>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A677" s="5"/>
+      <c r="A677" s="27"/>
       <c r="B677" s="27"/>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.25">
@@ -13558,11 +13575,11 @@
       <c r="B680" s="27"/>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A681" s="27"/>
+      <c r="A681" s="5"/>
       <c r="B681" s="27"/>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A682" s="5"/>
+      <c r="A682" s="27"/>
       <c r="B682" s="27"/>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.25">
@@ -13578,11 +13595,11 @@
       <c r="B685" s="27"/>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A686" s="27"/>
+      <c r="A686" s="5"/>
       <c r="B686" s="27"/>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A687" s="5"/>
+      <c r="A687" s="27"/>
       <c r="B687" s="27"/>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.25">
@@ -13598,11 +13615,11 @@
       <c r="B690" s="27"/>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A691" s="27"/>
+      <c r="A691" s="5"/>
       <c r="B691" s="27"/>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A692" s="5"/>
+      <c r="A692" s="27"/>
       <c r="B692" s="27"/>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.25">
@@ -13622,11 +13639,11 @@
       <c r="B696" s="27"/>
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A697" s="27"/>
+      <c r="A697" s="5"/>
       <c r="B697" s="27"/>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A698" s="5"/>
+      <c r="A698" s="27"/>
       <c r="B698" s="27"/>
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.25">
@@ -13642,11 +13659,11 @@
       <c r="B701" s="27"/>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A702" s="27"/>
+      <c r="A702" s="5"/>
       <c r="B702" s="27"/>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A703" s="5"/>
+      <c r="A703" s="27"/>
       <c r="B703" s="27"/>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.25">
@@ -13662,11 +13679,11 @@
       <c r="B706" s="27"/>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A707" s="27"/>
+      <c r="A707" s="5"/>
       <c r="B707" s="27"/>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A708" s="5"/>
+      <c r="A708" s="27"/>
       <c r="B708" s="27"/>
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.25">
@@ -13682,11 +13699,11 @@
       <c r="B711" s="27"/>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A712" s="27"/>
+      <c r="A712" s="5"/>
       <c r="B712" s="27"/>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A713" s="5"/>
+      <c r="A713" s="27"/>
       <c r="B713" s="27"/>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.25">
@@ -13702,11 +13719,11 @@
       <c r="B716" s="27"/>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A717" s="27"/>
+      <c r="A717" s="5"/>
       <c r="B717" s="27"/>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A718" s="5"/>
+      <c r="A718" s="27"/>
       <c r="B718" s="27"/>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.25">
@@ -13722,11 +13739,11 @@
       <c r="B721" s="27"/>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A722" s="27"/>
+      <c r="A722" s="5"/>
       <c r="B722" s="27"/>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A723" s="5"/>
+      <c r="A723" s="27"/>
       <c r="B723" s="27"/>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.25">
@@ -13742,12 +13759,12 @@
       <c r="B726" s="27"/>
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A727" s="8"/>
-      <c r="B727" s="8"/>
+      <c r="A727" s="5"/>
+      <c r="B727" s="27"/>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A728" s="5"/>
-      <c r="B728" s="27"/>
+      <c r="A728" s="8"/>
+      <c r="B728" s="8"/>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A729" s="5"/>
@@ -13778,11 +13795,11 @@
       <c r="B735" s="27"/>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A736" s="27"/>
+      <c r="A736" s="5"/>
       <c r="B736" s="27"/>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A737" s="5"/>
+      <c r="A737" s="27"/>
       <c r="B737" s="27"/>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.25">
@@ -13814,11 +13831,11 @@
       <c r="B744" s="27"/>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A745" s="27"/>
+      <c r="A745" s="5"/>
       <c r="B745" s="27"/>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A746" s="5"/>
+      <c r="A746" s="27"/>
       <c r="B746" s="27"/>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.25">
@@ -13850,11 +13867,11 @@
       <c r="B753" s="27"/>
     </row>
     <row r="754" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A754" s="27"/>
+      <c r="A754" s="5"/>
       <c r="B754" s="27"/>
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A755" s="5"/>
+      <c r="A755" s="27"/>
       <c r="B755" s="27"/>
     </row>
     <row r="756" spans="1:2" x14ac:dyDescent="0.25">
@@ -13886,11 +13903,11 @@
       <c r="B762" s="27"/>
     </row>
     <row r="763" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A763" s="27"/>
+      <c r="A763" s="5"/>
       <c r="B763" s="27"/>
     </row>
     <row r="764" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A764" s="5"/>
+      <c r="A764" s="27"/>
       <c r="B764" s="27"/>
     </row>
     <row r="765" spans="1:2" x14ac:dyDescent="0.25">
@@ -13922,11 +13939,11 @@
       <c r="B771" s="27"/>
     </row>
     <row r="772" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A772" s="27"/>
+      <c r="A772" s="5"/>
       <c r="B772" s="27"/>
     </row>
     <row r="773" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A773" s="5"/>
+      <c r="A773" s="27"/>
       <c r="B773" s="27"/>
     </row>
     <row r="774" spans="1:2" x14ac:dyDescent="0.25">
@@ -13942,11 +13959,11 @@
       <c r="B776" s="27"/>
     </row>
     <row r="777" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A777" s="27"/>
+      <c r="A777" s="5"/>
       <c r="B777" s="27"/>
     </row>
     <row r="778" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A778" s="5"/>
+      <c r="A778" s="27"/>
       <c r="B778" s="27"/>
     </row>
     <row r="779" spans="1:2" x14ac:dyDescent="0.25">
@@ -13962,11 +13979,11 @@
       <c r="B781" s="27"/>
     </row>
     <row r="782" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A782" s="27"/>
+      <c r="A782" s="5"/>
       <c r="B782" s="27"/>
     </row>
     <row r="783" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A783" s="5"/>
+      <c r="A783" s="27"/>
       <c r="B783" s="27"/>
     </row>
     <row r="784" spans="1:2" x14ac:dyDescent="0.25">
@@ -13982,11 +13999,11 @@
       <c r="B786" s="27"/>
     </row>
     <row r="787" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A787" s="27"/>
+      <c r="A787" s="5"/>
       <c r="B787" s="27"/>
     </row>
     <row r="788" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A788" s="5"/>
+      <c r="A788" s="27"/>
       <c r="B788" s="27"/>
     </row>
     <row r="789" spans="1:2" x14ac:dyDescent="0.25">
@@ -14002,11 +14019,11 @@
       <c r="B791" s="27"/>
     </row>
     <row r="792" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A792" s="27"/>
+      <c r="A792" s="5"/>
       <c r="B792" s="27"/>
     </row>
     <row r="793" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A793" s="5"/>
+      <c r="A793" s="27"/>
       <c r="B793" s="27"/>
     </row>
     <row r="794" spans="1:2" x14ac:dyDescent="0.25">
@@ -14022,11 +14039,11 @@
       <c r="B796" s="27"/>
     </row>
     <row r="797" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A797" s="27"/>
+      <c r="A797" s="5"/>
       <c r="B797" s="27"/>
     </row>
     <row r="798" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A798" s="5"/>
+      <c r="A798" s="27"/>
       <c r="B798" s="27"/>
     </row>
     <row r="799" spans="1:2" x14ac:dyDescent="0.25">
@@ -14042,11 +14059,11 @@
       <c r="B801" s="27"/>
     </row>
     <row r="802" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A802" s="27"/>
+      <c r="A802" s="5"/>
       <c r="B802" s="27"/>
     </row>
     <row r="803" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A803" s="5"/>
+      <c r="A803" s="27"/>
       <c r="B803" s="27"/>
     </row>
     <row r="804" spans="1:2" x14ac:dyDescent="0.25">
@@ -14062,11 +14079,11 @@
       <c r="B806" s="27"/>
     </row>
     <row r="807" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A807" s="27"/>
+      <c r="A807" s="5"/>
       <c r="B807" s="27"/>
     </row>
     <row r="808" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A808" s="5"/>
+      <c r="A808" s="27"/>
       <c r="B808" s="27"/>
     </row>
     <row r="809" spans="1:2" x14ac:dyDescent="0.25">
@@ -14082,11 +14099,11 @@
       <c r="B811" s="27"/>
     </row>
     <row r="812" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A812" s="27"/>
+      <c r="A812" s="5"/>
       <c r="B812" s="27"/>
     </row>
     <row r="813" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A813" s="5"/>
+      <c r="A813" s="27"/>
       <c r="B813" s="27"/>
     </row>
     <row r="814" spans="1:2" x14ac:dyDescent="0.25">
@@ -14102,11 +14119,11 @@
       <c r="B816" s="27"/>
     </row>
     <row r="817" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A817" s="27"/>
+      <c r="A817" s="5"/>
       <c r="B817" s="27"/>
     </row>
     <row r="818" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A818" s="5"/>
+      <c r="A818" s="27"/>
       <c r="B818" s="27"/>
     </row>
     <row r="819" spans="1:2" x14ac:dyDescent="0.25">
@@ -14126,11 +14143,11 @@
       <c r="B822" s="27"/>
     </row>
     <row r="823" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A823" s="27"/>
+      <c r="A823" s="5"/>
       <c r="B823" s="27"/>
     </row>
     <row r="824" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A824" s="5"/>
+      <c r="A824" s="27"/>
       <c r="B824" s="27"/>
     </row>
     <row r="825" spans="1:2" x14ac:dyDescent="0.25">
@@ -14146,11 +14163,11 @@
       <c r="B827" s="27"/>
     </row>
     <row r="828" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A828" s="27"/>
+      <c r="A828" s="5"/>
       <c r="B828" s="27"/>
     </row>
     <row r="829" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A829" s="5"/>
+      <c r="A829" s="27"/>
       <c r="B829" s="27"/>
     </row>
     <row r="830" spans="1:2" x14ac:dyDescent="0.25">
@@ -14170,11 +14187,11 @@
       <c r="B833" s="27"/>
     </row>
     <row r="834" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A834" s="27"/>
+      <c r="A834" s="5"/>
       <c r="B834" s="27"/>
     </row>
     <row r="835" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A835" s="5"/>
+      <c r="A835" s="27"/>
       <c r="B835" s="27"/>
     </row>
     <row r="836" spans="1:2" x14ac:dyDescent="0.25">
@@ -14194,12 +14211,12 @@
       <c r="B839" s="27"/>
     </row>
     <row r="840" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A840" s="8"/>
-      <c r="B840" s="8"/>
+      <c r="A840" s="5"/>
+      <c r="B840" s="27"/>
     </row>
     <row r="841" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A841" s="5"/>
-      <c r="B841" s="27"/>
+      <c r="A841" s="8"/>
+      <c r="B841" s="8"/>
     </row>
     <row r="842" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A842" s="5"/>
@@ -14214,11 +14231,11 @@
       <c r="B844" s="27"/>
     </row>
     <row r="845" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A845" s="27"/>
+      <c r="A845" s="5"/>
       <c r="B845" s="27"/>
     </row>
     <row r="846" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A846" s="5"/>
+      <c r="A846" s="27"/>
       <c r="B846" s="27"/>
     </row>
     <row r="847" spans="1:2" x14ac:dyDescent="0.25">
@@ -14234,11 +14251,11 @@
       <c r="B849" s="27"/>
     </row>
     <row r="850" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A850" s="27"/>
+      <c r="A850" s="5"/>
       <c r="B850" s="27"/>
     </row>
     <row r="851" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A851" s="5"/>
+      <c r="A851" s="27"/>
       <c r="B851" s="27"/>
     </row>
     <row r="852" spans="1:2" x14ac:dyDescent="0.25">
@@ -14254,11 +14271,11 @@
       <c r="B854" s="27"/>
     </row>
     <row r="855" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A855" s="27"/>
+      <c r="A855" s="5"/>
       <c r="B855" s="27"/>
     </row>
     <row r="856" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A856" s="5"/>
+      <c r="A856" s="27"/>
       <c r="B856" s="27"/>
     </row>
     <row r="857" spans="1:2" x14ac:dyDescent="0.25">
@@ -14274,11 +14291,11 @@
       <c r="B859" s="27"/>
     </row>
     <row r="860" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A860" s="27"/>
+      <c r="A860" s="5"/>
       <c r="B860" s="27"/>
     </row>
     <row r="861" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A861" s="5"/>
+      <c r="A861" s="27"/>
       <c r="B861" s="27"/>
     </row>
     <row r="862" spans="1:2" x14ac:dyDescent="0.25">
@@ -14294,11 +14311,11 @@
       <c r="B864" s="27"/>
     </row>
     <row r="865" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A865" s="27"/>
+      <c r="A865" s="5"/>
       <c r="B865" s="27"/>
     </row>
     <row r="866" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A866" s="5"/>
+      <c r="A866" s="27"/>
       <c r="B866" s="27"/>
     </row>
     <row r="867" spans="1:2" x14ac:dyDescent="0.25">
@@ -14306,11 +14323,11 @@
       <c r="B867" s="27"/>
     </row>
     <row r="868" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A868" s="27"/>
+      <c r="A868" s="5"/>
       <c r="B868" s="27"/>
     </row>
     <row r="869" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A869" s="5"/>
+      <c r="A869" s="27"/>
       <c r="B869" s="27"/>
     </row>
     <row r="870" spans="1:2" x14ac:dyDescent="0.25">
@@ -14318,11 +14335,11 @@
       <c r="B870" s="27"/>
     </row>
     <row r="871" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A871" s="27"/>
+      <c r="A871" s="5"/>
       <c r="B871" s="27"/>
     </row>
     <row r="872" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A872" s="5"/>
+      <c r="A872" s="27"/>
       <c r="B872" s="27"/>
     </row>
     <row r="873" spans="1:2" x14ac:dyDescent="0.25">
@@ -14330,11 +14347,11 @@
       <c r="B873" s="27"/>
     </row>
     <row r="874" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A874" s="27"/>
+      <c r="A874" s="5"/>
       <c r="B874" s="27"/>
     </row>
     <row r="875" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A875" s="5"/>
+      <c r="A875" s="27"/>
       <c r="B875" s="27"/>
     </row>
     <row r="876" spans="1:2" x14ac:dyDescent="0.25">
@@ -14342,11 +14359,11 @@
       <c r="B876" s="27"/>
     </row>
     <row r="877" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A877" s="27"/>
+      <c r="A877" s="5"/>
       <c r="B877" s="27"/>
     </row>
     <row r="878" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A878" s="5"/>
+      <c r="A878" s="27"/>
       <c r="B878" s="27"/>
     </row>
     <row r="879" spans="1:2" x14ac:dyDescent="0.25">
@@ -14354,11 +14371,11 @@
       <c r="B879" s="27"/>
     </row>
     <row r="880" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A880" s="27"/>
+      <c r="A880" s="5"/>
       <c r="B880" s="27"/>
     </row>
     <row r="881" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A881" s="5"/>
+      <c r="A881" s="27"/>
       <c r="B881" s="27"/>
     </row>
     <row r="882" spans="1:2" x14ac:dyDescent="0.25">
@@ -14366,11 +14383,11 @@
       <c r="B882" s="27"/>
     </row>
     <row r="883" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A883" s="27"/>
+      <c r="A883" s="5"/>
       <c r="B883" s="27"/>
     </row>
     <row r="884" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A884" s="5"/>
+      <c r="A884" s="27"/>
       <c r="B884" s="27"/>
     </row>
     <row r="885" spans="1:2" x14ac:dyDescent="0.25">
@@ -14378,11 +14395,11 @@
       <c r="B885" s="27"/>
     </row>
     <row r="886" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A886" s="27"/>
+      <c r="A886" s="5"/>
       <c r="B886" s="27"/>
     </row>
     <row r="887" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A887" s="5"/>
+      <c r="A887" s="27"/>
       <c r="B887" s="27"/>
     </row>
     <row r="888" spans="1:2" x14ac:dyDescent="0.25">
@@ -14390,11 +14407,11 @@
       <c r="B888" s="27"/>
     </row>
     <row r="889" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A889" s="27"/>
+      <c r="A889" s="5"/>
       <c r="B889" s="27"/>
     </row>
     <row r="890" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A890" s="5"/>
+      <c r="A890" s="27"/>
       <c r="B890" s="27"/>
     </row>
     <row r="891" spans="1:2" x14ac:dyDescent="0.25">
@@ -14402,11 +14419,11 @@
       <c r="B891" s="27"/>
     </row>
     <row r="892" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A892" s="27"/>
+      <c r="A892" s="5"/>
       <c r="B892" s="27"/>
     </row>
     <row r="893" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A893" s="5"/>
+      <c r="A893" s="27"/>
       <c r="B893" s="27"/>
     </row>
     <row r="894" spans="1:2" x14ac:dyDescent="0.25">
@@ -14414,11 +14431,11 @@
       <c r="B894" s="27"/>
     </row>
     <row r="895" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A895" s="27"/>
+      <c r="A895" s="5"/>
       <c r="B895" s="27"/>
     </row>
     <row r="896" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A896" s="5"/>
+      <c r="A896" s="27"/>
       <c r="B896" s="27"/>
     </row>
     <row r="897" spans="1:2" x14ac:dyDescent="0.25">
@@ -14426,11 +14443,11 @@
       <c r="B897" s="27"/>
     </row>
     <row r="898" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A898" s="27"/>
+      <c r="A898" s="5"/>
       <c r="B898" s="27"/>
     </row>
     <row r="899" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A899" s="5"/>
+      <c r="A899" s="27"/>
       <c r="B899" s="27"/>
     </row>
     <row r="900" spans="1:2" x14ac:dyDescent="0.25">
@@ -14438,11 +14455,11 @@
       <c r="B900" s="27"/>
     </row>
     <row r="901" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A901" s="27"/>
+      <c r="A901" s="5"/>
       <c r="B901" s="27"/>
     </row>
     <row r="902" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A902" s="5"/>
+      <c r="A902" s="27"/>
       <c r="B902" s="27"/>
     </row>
     <row r="903" spans="1:2" x14ac:dyDescent="0.25">
@@ -14450,11 +14467,11 @@
       <c r="B903" s="27"/>
     </row>
     <row r="904" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A904" s="27"/>
+      <c r="A904" s="5"/>
       <c r="B904" s="27"/>
     </row>
     <row r="905" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A905" s="5"/>
+      <c r="A905" s="27"/>
       <c r="B905" s="27"/>
     </row>
     <row r="906" spans="1:2" x14ac:dyDescent="0.25">
@@ -14462,35 +14479,35 @@
       <c r="B906" s="27"/>
     </row>
     <row r="907" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A907" s="27"/>
+      <c r="A907" s="5"/>
       <c r="B907" s="27"/>
     </row>
     <row r="908" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A908" s="5"/>
+      <c r="A908" s="27"/>
       <c r="B908" s="27"/>
     </row>
     <row r="909" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A909" s="27"/>
+      <c r="A909" s="5"/>
       <c r="B909" s="27"/>
     </row>
     <row r="910" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A910" s="5"/>
+      <c r="A910" s="27"/>
       <c r="B910" s="27"/>
     </row>
     <row r="911" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A911" s="27"/>
+      <c r="A911" s="5"/>
       <c r="B911" s="27"/>
     </row>
     <row r="912" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A912" s="5"/>
+      <c r="A912" s="27"/>
       <c r="B912" s="27"/>
     </row>
     <row r="913" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A913" s="27"/>
+      <c r="A913" s="5"/>
       <c r="B913" s="27"/>
     </row>
     <row r="914" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A914" s="5"/>
+      <c r="A914" s="27"/>
       <c r="B914" s="27"/>
     </row>
     <row r="915" spans="1:2" x14ac:dyDescent="0.25">
@@ -14498,11 +14515,11 @@
       <c r="B915" s="27"/>
     </row>
     <row r="916" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A916" s="27"/>
+      <c r="A916" s="5"/>
       <c r="B916" s="27"/>
     </row>
     <row r="917" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A917" s="5"/>
+      <c r="A917" s="27"/>
       <c r="B917" s="27"/>
     </row>
     <row r="918" spans="1:2" x14ac:dyDescent="0.25">
@@ -14538,11 +14555,11 @@
       <c r="B925" s="27"/>
     </row>
     <row r="926" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A926" s="27"/>
+      <c r="A926" s="5"/>
       <c r="B926" s="27"/>
     </row>
     <row r="927" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A927" s="5"/>
+      <c r="A927" s="27"/>
       <c r="B927" s="27"/>
     </row>
     <row r="928" spans="1:2" x14ac:dyDescent="0.25">
@@ -14566,12 +14583,12 @@
       <c r="B932" s="27"/>
     </row>
     <row r="933" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A933" s="8"/>
-      <c r="B933" s="8"/>
+      <c r="A933" s="5"/>
+      <c r="B933" s="27"/>
     </row>
     <row r="934" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A934" s="5"/>
-      <c r="B934" s="27"/>
+      <c r="A934" s="8"/>
+      <c r="B934" s="8"/>
     </row>
     <row r="935" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A935" s="5"/>
@@ -14606,11 +14623,11 @@
       <c r="B942" s="27"/>
     </row>
     <row r="943" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A943" s="27"/>
+      <c r="A943" s="5"/>
       <c r="B943" s="27"/>
     </row>
     <row r="944" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A944" s="5"/>
+      <c r="A944" s="27"/>
       <c r="B944" s="27"/>
     </row>
     <row r="945" spans="1:2" x14ac:dyDescent="0.25">
@@ -14646,11 +14663,11 @@
       <c r="B952" s="27"/>
     </row>
     <row r="953" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A953" s="27"/>
+      <c r="A953" s="5"/>
       <c r="B953" s="27"/>
     </row>
     <row r="954" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A954" s="5"/>
+      <c r="A954" s="27"/>
       <c r="B954" s="27"/>
     </row>
     <row r="955" spans="1:2" x14ac:dyDescent="0.25">
@@ -14706,11 +14723,11 @@
       <c r="B967" s="27"/>
     </row>
     <row r="968" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A968" s="27"/>
+      <c r="A968" s="5"/>
       <c r="B968" s="27"/>
     </row>
     <row r="969" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A969" s="5"/>
+      <c r="A969" s="27"/>
       <c r="B969" s="27"/>
     </row>
     <row r="970" spans="1:2" x14ac:dyDescent="0.25">
@@ -14734,14 +14751,18 @@
       <c r="B974" s="27"/>
     </row>
     <row r="975" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A975" s="27"/>
+      <c r="A975" s="5"/>
       <c r="B975" s="27"/>
     </row>
-    <row r="1027" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1027" s="5"/>
+    <row r="976" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A976" s="27"/>
+      <c r="B976" s="27"/>
+    </row>
+    <row r="1028" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1028" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E672"/>
+  <autoFilter ref="A1:E673"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Name of project change & update asset list
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -2111,8 +2111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3626,7 +3626,9 @@
       <c r="J34" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="K34" s="31"/>
+      <c r="K34" s="31">
+        <v>20</v>
+      </c>
       <c r="L34" s="31"/>
       <c r="M34" s="31"/>
       <c r="N34" s="31"/>
@@ -3637,7 +3639,7 @@
       <c r="S34" s="31"/>
       <c r="T34" s="64">
         <f>K34+L34+M34+N34+O34+P34+Q34+R34+S34</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3697,7 +3699,7 @@
       <c r="R36" s="35"/>
       <c r="T36" s="71">
         <f>T34+T35</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="U36" s="71" t="s">
         <v>373</v>

</xml_diff>

<commit_message>
08-03-2016 Uren Registratie & Aseet List Update & Input in word
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1832" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1838" uniqueCount="404">
   <si>
     <t>ID Code</t>
   </si>
@@ -733,9 +733,6 @@
     <t>Player_Movement (70)</t>
   </si>
   <si>
-    <t>Game_GameManager (100)</t>
-  </si>
-  <si>
     <t>Weapons_WeaponManager (60)</t>
   </si>
   <si>
@@ -1229,13 +1226,16 @@
   </si>
   <si>
     <t>Items_UnlockWeapon (20)</t>
+  </si>
+  <si>
+    <t>Game_GameManager (15)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1281,14 +1281,6 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1565,7 +1557,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1687,23 +1679,12 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1731,7 +1712,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1752,9 +1733,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1767,13 +1745,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1791,8 +1763,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2112,7 +2096,7 @@
   <dimension ref="A1:U1028"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2124,8 +2108,8 @@
     <col min="5" max="5" width="10.85546875" style="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" style="46" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="164.7109375" style="46" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="164.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="28.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="34.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="33.7109375" style="3" bestFit="1" customWidth="1"/>
@@ -2162,37 +2146,37 @@
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="59" t="s">
+      <c r="K1" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="59" t="s">
+      <c r="M1" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="59" t="s">
+      <c r="N1" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="59" t="s">
+      <c r="O1" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="59" t="s">
+      <c r="P1" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="59" t="s">
+      <c r="Q1" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="59" t="s">
+      <c r="R1" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="S1" s="59" t="s">
+      <c r="S1" s="54" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2218,38 +2202,38 @@
       <c r="G2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="47" t="s">
+      <c r="H2" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="47" t="s">
+      <c r="I2" s="71" t="s">
         <v>228</v>
       </c>
       <c r="J2" s="10"/>
-      <c r="K2" s="57" t="s">
+      <c r="K2" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="76" t="s">
+      <c r="L2" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="76" t="s">
+      <c r="M2" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="76" t="s">
+      <c r="N2" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="57" t="s">
+      <c r="O2" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="57" t="s">
+      <c r="P2" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="57" t="s">
+      <c r="Q2" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="76" t="s">
+      <c r="R2" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="76" t="s">
+      <c r="S2" s="68" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2275,39 +2259,39 @@
       <c r="G3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="71" t="s">
         <v>229</v>
       </c>
       <c r="J3" s="10"/>
       <c r="K3" s="32" t="s">
-        <v>289</v>
-      </c>
-      <c r="L3" s="74" t="s">
-        <v>297</v>
-      </c>
-      <c r="M3" s="74" t="s">
-        <v>398</v>
-      </c>
-      <c r="N3" s="78" t="s">
-        <v>311</v>
+        <v>288</v>
+      </c>
+      <c r="L3" s="66" t="s">
+        <v>296</v>
+      </c>
+      <c r="M3" s="66" t="s">
+        <v>397</v>
+      </c>
+      <c r="N3" s="70" t="s">
+        <v>310</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="P3" s="51" t="s">
-        <v>336</v>
+        <v>327</v>
+      </c>
+      <c r="P3" s="46" t="s">
+        <v>335</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>349</v>
-      </c>
-      <c r="R3" s="51" t="s">
-        <v>341</v>
-      </c>
-      <c r="S3" s="78" t="s">
-        <v>378</v>
+        <v>348</v>
+      </c>
+      <c r="R3" s="46" t="s">
+        <v>340</v>
+      </c>
+      <c r="S3" s="70" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -2332,39 +2316,39 @@
       <c r="G4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="47" t="s">
+      <c r="H4" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="47" t="s">
+      <c r="I4" s="71" t="s">
         <v>230</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="N4" s="52" t="s">
-        <v>312</v>
+        <v>301</v>
+      </c>
+      <c r="N4" s="47" t="s">
+        <v>311</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>329</v>
-      </c>
-      <c r="P4" s="50" t="s">
-        <v>337</v>
+        <v>328</v>
+      </c>
+      <c r="P4" s="45" t="s">
+        <v>336</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>350</v>
-      </c>
-      <c r="R4" s="50" t="s">
-        <v>342</v>
-      </c>
-      <c r="S4" s="52" t="s">
-        <v>382</v>
+        <v>349</v>
+      </c>
+      <c r="R4" s="45" t="s">
+        <v>341</v>
+      </c>
+      <c r="S4" s="47" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -2389,39 +2373,39 @@
       <c r="G5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="47" t="s">
+      <c r="I5" s="71" t="s">
         <v>234</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="14" t="s">
-        <v>291</v>
-      </c>
-      <c r="L5" s="69" t="s">
-        <v>299</v>
+        <v>290</v>
+      </c>
+      <c r="L5" s="63" t="s">
+        <v>298</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>303</v>
-      </c>
-      <c r="N5" s="52" t="s">
-        <v>313</v>
+        <v>302</v>
+      </c>
+      <c r="N5" s="47" t="s">
+        <v>312</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>330</v>
-      </c>
-      <c r="P5" s="52" t="s">
-        <v>338</v>
+        <v>329</v>
+      </c>
+      <c r="P5" s="47" t="s">
+        <v>337</v>
       </c>
       <c r="Q5" s="10" t="s">
-        <v>351</v>
-      </c>
-      <c r="R5" s="52" t="s">
-        <v>367</v>
-      </c>
-      <c r="S5" s="50" t="s">
-        <v>383</v>
+        <v>350</v>
+      </c>
+      <c r="R5" s="47" t="s">
+        <v>366</v>
+      </c>
+      <c r="S5" s="45" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -2446,39 +2430,39 @@
       <c r="G6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="47" t="s">
+      <c r="H6" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="71" t="s">
         <v>224</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="23" t="s">
-        <v>296</v>
-      </c>
-      <c r="L6" s="69" t="s">
-        <v>300</v>
+        <v>295</v>
+      </c>
+      <c r="L6" s="63" t="s">
+        <v>299</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>304</v>
-      </c>
-      <c r="N6" s="52" t="s">
-        <v>315</v>
+        <v>303</v>
+      </c>
+      <c r="N6" s="47" t="s">
+        <v>314</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>331</v>
-      </c>
-      <c r="P6" s="50" t="s">
-        <v>339</v>
+        <v>330</v>
+      </c>
+      <c r="P6" s="45" t="s">
+        <v>338</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="R6" s="50" t="s">
-        <v>368</v>
-      </c>
-      <c r="S6" s="50" t="s">
-        <v>384</v>
+        <v>351</v>
+      </c>
+      <c r="R6" s="45" t="s">
+        <v>367</v>
+      </c>
+      <c r="S6" s="45" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -2503,39 +2487,39 @@
       <c r="G7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="47" t="s">
+      <c r="H7" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="47" t="s">
+      <c r="I7" s="71" t="s">
         <v>225</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="23" t="s">
-        <v>293</v>
-      </c>
-      <c r="L7" s="69" t="s">
-        <v>301</v>
+        <v>292</v>
+      </c>
+      <c r="L7" s="63" t="s">
+        <v>300</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>305</v>
-      </c>
-      <c r="N7" s="52" t="s">
-        <v>316</v>
-      </c>
-      <c r="O7" s="69" t="s">
-        <v>322</v>
-      </c>
-      <c r="P7" s="52" t="s">
-        <v>340</v>
+        <v>304</v>
+      </c>
+      <c r="N7" s="47" t="s">
+        <v>315</v>
+      </c>
+      <c r="O7" s="63" t="s">
+        <v>321</v>
+      </c>
+      <c r="P7" s="47" t="s">
+        <v>339</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>353</v>
-      </c>
-      <c r="R7" s="50" t="s">
-        <v>369</v>
-      </c>
-      <c r="S7" s="50" t="s">
-        <v>385</v>
+        <v>352</v>
+      </c>
+      <c r="R7" s="45" t="s">
+        <v>368</v>
+      </c>
+      <c r="S7" s="45" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -2560,39 +2544,39 @@
       <c r="G8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="47" t="s">
+      <c r="I8" s="71" t="s">
         <v>231</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="23" t="s">
-        <v>294</v>
-      </c>
-      <c r="L8" s="69" t="s">
-        <v>394</v>
+        <v>293</v>
+      </c>
+      <c r="L8" s="63" t="s">
+        <v>393</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>361</v>
-      </c>
-      <c r="N8" s="58" t="s">
-        <v>317</v>
-      </c>
-      <c r="O8" s="69" t="s">
-        <v>323</v>
-      </c>
-      <c r="P8" s="50" t="s">
-        <v>356</v>
+        <v>360</v>
+      </c>
+      <c r="N8" s="53" t="s">
+        <v>316</v>
+      </c>
+      <c r="O8" s="63" t="s">
+        <v>322</v>
+      </c>
+      <c r="P8" s="45" t="s">
+        <v>355</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>354</v>
-      </c>
-      <c r="R8" s="50" t="s">
-        <v>370</v>
-      </c>
-      <c r="S8" s="50" t="s">
-        <v>386</v>
+        <v>353</v>
+      </c>
+      <c r="R8" s="45" t="s">
+        <v>369</v>
+      </c>
+      <c r="S8" s="45" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -2605,39 +2589,39 @@
       <c r="G9" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="H9" s="47" t="s">
+      <c r="H9" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="47" t="s">
+      <c r="I9" s="71" t="s">
         <v>226</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="23" t="s">
-        <v>295</v>
-      </c>
-      <c r="L9" s="69" t="s">
-        <v>396</v>
+        <v>294</v>
+      </c>
+      <c r="L9" s="63" t="s">
+        <v>395</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>306</v>
-      </c>
-      <c r="N9" s="56" t="s">
-        <v>318</v>
-      </c>
-      <c r="O9" s="69" t="s">
-        <v>320</v>
-      </c>
-      <c r="P9" s="50" t="s">
-        <v>357</v>
+        <v>305</v>
+      </c>
+      <c r="N9" s="51" t="s">
+        <v>317</v>
+      </c>
+      <c r="O9" s="63" t="s">
+        <v>319</v>
+      </c>
+      <c r="P9" s="45" t="s">
+        <v>356</v>
       </c>
       <c r="Q9" s="10" t="s">
-        <v>355</v>
-      </c>
-      <c r="R9" s="50" t="s">
-        <v>374</v>
-      </c>
-      <c r="S9" s="50" t="s">
-        <v>387</v>
+        <v>354</v>
+      </c>
+      <c r="R9" s="45" t="s">
+        <v>373</v>
+      </c>
+      <c r="S9" s="45" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -2660,39 +2644,39 @@
         <v>12</v>
       </c>
       <c r="G10" s="9"/>
-      <c r="H10" s="47" t="s">
+      <c r="H10" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="47" t="s">
+      <c r="I10" s="71" t="s">
         <v>227</v>
       </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="69" t="s">
-        <v>395</v>
-      </c>
-      <c r="L10" s="77" t="s">
-        <v>397</v>
+      <c r="K10" s="63" t="s">
+        <v>394</v>
+      </c>
+      <c r="L10" s="69" t="s">
+        <v>396</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>307</v>
-      </c>
-      <c r="N10" s="56" t="s">
-        <v>319</v>
+        <v>306</v>
+      </c>
+      <c r="N10" s="51" t="s">
+        <v>318</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>332</v>
-      </c>
-      <c r="P10" s="50" t="s">
-        <v>358</v>
-      </c>
-      <c r="Q10" s="69" t="s">
-        <v>362</v>
-      </c>
-      <c r="R10" s="50" t="s">
-        <v>375</v>
-      </c>
-      <c r="S10" s="50" t="s">
-        <v>388</v>
+        <v>331</v>
+      </c>
+      <c r="P10" s="45" t="s">
+        <v>357</v>
+      </c>
+      <c r="Q10" s="63" t="s">
+        <v>361</v>
+      </c>
+      <c r="R10" s="45" t="s">
+        <v>374</v>
+      </c>
+      <c r="S10" s="45" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -2713,37 +2697,37 @@
       </c>
       <c r="F11" s="27"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="47" t="s">
+      <c r="I11" s="71" t="s">
         <v>232</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="23"/>
       <c r="L11" s="14" t="s">
-        <v>399</v>
-      </c>
-      <c r="M11" s="68" t="s">
-        <v>308</v>
-      </c>
-      <c r="N11" s="52" t="s">
-        <v>321</v>
+        <v>398</v>
+      </c>
+      <c r="M11" s="62" t="s">
+        <v>307</v>
+      </c>
+      <c r="N11" s="47" t="s">
+        <v>320</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>333</v>
-      </c>
-      <c r="P11" s="50" t="s">
-        <v>347</v>
+        <v>332</v>
+      </c>
+      <c r="P11" s="45" t="s">
+        <v>346</v>
       </c>
       <c r="Q11" s="14" t="s">
-        <v>363</v>
-      </c>
-      <c r="R11" s="50" t="s">
-        <v>376</v>
-      </c>
-      <c r="S11" s="50" t="s">
-        <v>389</v>
+        <v>362</v>
+      </c>
+      <c r="R11" s="45" t="s">
+        <v>375</v>
+      </c>
+      <c r="S11" s="45" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -2763,37 +2747,37 @@
         <v>10</v>
       </c>
       <c r="G12" s="9"/>
-      <c r="H12" s="47" t="s">
+      <c r="H12" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="47" t="s">
-        <v>287</v>
+      <c r="I12" s="71" t="s">
+        <v>286</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="23"/>
       <c r="L12" s="14" t="s">
-        <v>400</v>
-      </c>
-      <c r="M12" s="69" t="s">
-        <v>309</v>
-      </c>
-      <c r="N12" s="56" t="s">
-        <v>326</v>
-      </c>
-      <c r="O12" s="69" t="s">
-        <v>334</v>
-      </c>
-      <c r="P12" s="52" t="s">
-        <v>348</v>
+        <v>399</v>
+      </c>
+      <c r="M12" s="63" t="s">
+        <v>308</v>
+      </c>
+      <c r="N12" s="51" t="s">
+        <v>325</v>
+      </c>
+      <c r="O12" s="63" t="s">
+        <v>333</v>
+      </c>
+      <c r="P12" s="47" t="s">
+        <v>347</v>
       </c>
       <c r="Q12" s="14" t="s">
-        <v>364</v>
-      </c>
-      <c r="R12" s="50" t="s">
-        <v>344</v>
-      </c>
-      <c r="S12" s="52" t="s">
-        <v>390</v>
+        <v>363</v>
+      </c>
+      <c r="R12" s="45" t="s">
+        <v>343</v>
+      </c>
+      <c r="S12" s="47" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -2813,37 +2797,37 @@
         <v>10</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="47" t="s">
+      <c r="H13" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="I13" s="47" t="s">
-        <v>288</v>
+      <c r="I13" s="71" t="s">
+        <v>287</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="23"/>
       <c r="L13" s="14" t="s">
-        <v>292</v>
-      </c>
-      <c r="M13" s="69" t="s">
-        <v>310</v>
-      </c>
-      <c r="N13" s="52" t="s">
-        <v>325</v>
+        <v>291</v>
+      </c>
+      <c r="M13" s="63" t="s">
+        <v>309</v>
+      </c>
+      <c r="N13" s="47" t="s">
+        <v>324</v>
       </c>
       <c r="O13" s="14" t="s">
-        <v>335</v>
-      </c>
-      <c r="P13" s="50" t="s">
-        <v>343</v>
+        <v>334</v>
+      </c>
+      <c r="P13" s="45" t="s">
+        <v>342</v>
       </c>
       <c r="Q13" s="14" t="s">
-        <v>365</v>
-      </c>
-      <c r="R13" s="50" t="s">
-        <v>377</v>
-      </c>
-      <c r="S13" s="52" t="s">
-        <v>392</v>
+        <v>364</v>
+      </c>
+      <c r="R13" s="45" t="s">
+        <v>376</v>
+      </c>
+      <c r="S13" s="47" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -2863,35 +2847,35 @@
         <v>10</v>
       </c>
       <c r="G14" s="9"/>
-      <c r="H14" s="47" t="s">
+      <c r="H14" s="71" t="s">
         <v>215</v>
       </c>
-      <c r="I14" s="47" t="s">
-        <v>402</v>
+      <c r="I14" s="71" t="s">
+        <v>401</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="23"/>
       <c r="L14" s="23"/>
-      <c r="M14" s="69" t="s">
-        <v>314</v>
+      <c r="M14" s="63" t="s">
+        <v>313</v>
       </c>
       <c r="N14" s="34" t="s">
-        <v>327</v>
-      </c>
-      <c r="O14" s="69" t="s">
-        <v>346</v>
-      </c>
-      <c r="P14" s="50" t="s">
+        <v>326</v>
+      </c>
+      <c r="O14" s="63" t="s">
         <v>345</v>
       </c>
+      <c r="P14" s="45" t="s">
+        <v>344</v>
+      </c>
       <c r="Q14" s="14" t="s">
-        <v>366</v>
-      </c>
-      <c r="R14" s="50" t="s">
-        <v>393</v>
-      </c>
-      <c r="S14" s="50" t="s">
-        <v>391</v>
+        <v>365</v>
+      </c>
+      <c r="R14" s="45" t="s">
+        <v>392</v>
+      </c>
+      <c r="S14" s="45" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -2911,27 +2895,27 @@
         <v>10</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="47" t="s">
+      <c r="H15" s="71" t="s">
         <v>216</v>
       </c>
-      <c r="I15" s="47" t="s">
+      <c r="I15" s="71" t="s">
         <v>207</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="23"/>
       <c r="L15" s="23"/>
-      <c r="M15" s="69" t="s">
-        <v>360</v>
-      </c>
-      <c r="N15" s="50" t="s">
-        <v>324</v>
+      <c r="M15" s="63" t="s">
+        <v>359</v>
+      </c>
+      <c r="N15" s="45" t="s">
+        <v>323</v>
       </c>
       <c r="P15" s="34"/>
-      <c r="R15" s="50" t="s">
-        <v>379</v>
-      </c>
-      <c r="S15" s="50" t="s">
-        <v>371</v>
+      <c r="R15" s="45" t="s">
+        <v>378</v>
+      </c>
+      <c r="S15" s="45" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -2951,22 +2935,22 @@
         <v>10</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="71" t="s">
         <v>217</v>
       </c>
-      <c r="I16" s="47" t="s">
+      <c r="I16" s="71" t="s">
         <v>211</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="23"/>
       <c r="L16" s="23"/>
       <c r="M16" s="14" t="s">
-        <v>359</v>
-      </c>
-      <c r="N16" s="52"/>
+        <v>358</v>
+      </c>
+      <c r="N16" s="47"/>
       <c r="P16" s="34"/>
-      <c r="R16" s="50" t="s">
-        <v>380</v>
+      <c r="R16" s="45" t="s">
+        <v>379</v>
       </c>
       <c r="S16" s="34"/>
     </row>
@@ -2977,21 +2961,21 @@
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="47" t="s">
+      <c r="H17" s="71" t="s">
         <v>218</v>
       </c>
-      <c r="I17" s="47" t="s">
+      <c r="I17" s="71" t="s">
         <v>212</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="23"/>
       <c r="L17" s="23"/>
       <c r="M17" s="14"/>
-      <c r="N17" s="52"/>
-      <c r="P17" s="52"/>
+      <c r="N17" s="47"/>
+      <c r="P17" s="47"/>
       <c r="Q17" s="15"/>
-      <c r="R17" s="50" t="s">
-        <v>381</v>
+      <c r="R17" s="45" t="s">
+        <v>380</v>
       </c>
       <c r="S17" s="34"/>
     </row>
@@ -3012,18 +2996,18 @@
         <v>10</v>
       </c>
       <c r="G18" s="9"/>
-      <c r="H18" s="47" t="s">
+      <c r="H18" s="71" t="s">
         <v>219</v>
       </c>
-      <c r="I18" s="47" t="s">
+      <c r="I18" s="71" t="s">
         <v>213</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="23"/>
-      <c r="L18" s="69"/>
+      <c r="L18" s="63"/>
       <c r="M18" s="14"/>
-      <c r="N18" s="52"/>
-      <c r="P18" s="52"/>
+      <c r="N18" s="47"/>
+      <c r="P18" s="47"/>
       <c r="Q18" s="15"/>
       <c r="R18" s="34"/>
       <c r="S18" s="34"/>
@@ -3045,23 +3029,23 @@
         <v>10</v>
       </c>
       <c r="G19" s="9"/>
-      <c r="H19" s="47" t="s">
+      <c r="H19" s="71" t="s">
         <v>220</v>
       </c>
-      <c r="I19" s="47" t="s">
+      <c r="I19" s="71" t="s">
         <v>214</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="29"/>
-      <c r="L19" s="70"/>
-      <c r="M19" s="75"/>
-      <c r="N19" s="53"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="67"/>
+      <c r="N19" s="48"/>
       <c r="O19" s="30"/>
-      <c r="P19" s="53"/>
+      <c r="P19" s="48"/>
       <c r="Q19" s="15"/>
-      <c r="R19" s="55"/>
+      <c r="R19" s="50"/>
       <c r="S19" s="37"/>
-      <c r="T19" s="63" t="s">
+      <c r="T19" s="58" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3082,13 +3066,13 @@
         <v>10</v>
       </c>
       <c r="G20" s="9"/>
-      <c r="H20" s="47" t="s">
+      <c r="H20" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="I20" s="47" t="s">
+      <c r="I20" s="71" t="s">
         <v>222</v>
       </c>
-      <c r="J20" s="60" t="s">
+      <c r="J20" s="55" t="s">
         <v>19</v>
       </c>
       <c r="K20" s="32"/>
@@ -3100,7 +3084,7 @@
       <c r="Q20" s="33"/>
       <c r="R20" s="34"/>
       <c r="S20" s="36"/>
-      <c r="T20" s="60">
+      <c r="T20" s="55">
         <f>K20+L20+M20+N20+O20+P20+Q20+R20+S20</f>
         <v>0</v>
       </c>
@@ -3122,13 +3106,13 @@
         <v>10</v>
       </c>
       <c r="G21" s="9"/>
-      <c r="H21" s="47" t="s">
+      <c r="H21" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="I21" s="47" t="s">
+      <c r="I21" s="71" t="s">
         <v>223</v>
       </c>
-      <c r="J21" s="61" t="s">
+      <c r="J21" s="56" t="s">
         <v>17</v>
       </c>
       <c r="K21" s="23"/>
@@ -3140,7 +3124,7 @@
       <c r="Q21" s="35"/>
       <c r="R21" s="34"/>
       <c r="S21" s="36"/>
-      <c r="T21" s="61">
+      <c r="T21" s="56">
         <f>K21+L21+M21+N21+O21+P21+Q21+R21+S21</f>
         <v>0</v>
       </c>
@@ -3162,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="G22" s="9"/>
-      <c r="J22" s="62" t="s">
+      <c r="J22" s="57" t="s">
         <v>18</v>
       </c>
       <c r="K22" s="29"/>
@@ -3174,7 +3158,7 @@
       <c r="Q22" s="38"/>
       <c r="R22" s="37"/>
       <c r="S22" s="39"/>
-      <c r="T22" s="61">
+      <c r="T22" s="56">
         <f>K22+L22+M22+N22+O22+P22+Q22+R22+S22</f>
         <v>0</v>
       </c>
@@ -3205,12 +3189,12 @@
       <c r="P23" s="35"/>
       <c r="Q23" s="35"/>
       <c r="R23" s="35"/>
-      <c r="T23" s="73">
+      <c r="T23" s="72">
         <f>T20+T21+T22</f>
         <v>0</v>
       </c>
-      <c r="U23" s="71" t="s">
-        <v>372</v>
+      <c r="U23" s="73" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3230,7 +3214,7 @@
         <v>10</v>
       </c>
       <c r="G24" s="9"/>
-      <c r="T24" s="63"/>
+      <c r="T24" s="58"/>
     </row>
     <row r="25" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
@@ -3239,34 +3223,34 @@
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="G25" s="9"/>
-      <c r="K25" s="59" t="s">
+      <c r="K25" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="L25" s="59" t="s">
+      <c r="L25" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="M25" s="59" t="s">
+      <c r="M25" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="N25" s="59" t="s">
+      <c r="N25" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="O25" s="59" t="s">
+      <c r="O25" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="P25" s="59" t="s">
+      <c r="P25" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="Q25" s="59" t="s">
+      <c r="Q25" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="R25" s="59" t="s">
+      <c r="R25" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="S25" s="59" t="s">
+      <c r="S25" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="T25" s="63"/>
+      <c r="T25" s="58"/>
     </row>
     <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
@@ -3286,34 +3270,34 @@
       </c>
       <c r="G26" s="9"/>
       <c r="J26" s="10"/>
-      <c r="K26" s="57" t="s">
+      <c r="K26" s="52" t="s">
         <v>236</v>
       </c>
-      <c r="L26" s="57" t="s">
+      <c r="L26" s="52" t="s">
         <v>236</v>
       </c>
-      <c r="M26" s="57" t="s">
+      <c r="M26" s="52" t="s">
         <v>236</v>
       </c>
-      <c r="N26" s="57" t="s">
+      <c r="N26" s="52" t="s">
         <v>236</v>
       </c>
-      <c r="O26" s="57" t="s">
+      <c r="O26" s="52" t="s">
         <v>236</v>
       </c>
-      <c r="P26" s="57" t="s">
+      <c r="P26" s="52" t="s">
         <v>236</v>
       </c>
-      <c r="Q26" s="57" t="s">
+      <c r="Q26" s="52" t="s">
         <v>236</v>
       </c>
-      <c r="R26" s="57" t="s">
+      <c r="R26" s="52" t="s">
         <v>236</v>
       </c>
-      <c r="S26" s="57" t="s">
+      <c r="S26" s="52" t="s">
         <v>236</v>
       </c>
-      <c r="T26" s="63"/>
+      <c r="T26" s="58"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
@@ -3333,34 +3317,34 @@
       </c>
       <c r="G27" s="9"/>
       <c r="J27" s="10"/>
-      <c r="K27" s="50" t="s">
+      <c r="K27" s="45" t="s">
         <v>237</v>
       </c>
-      <c r="L27" s="50" t="s">
-        <v>240</v>
-      </c>
-      <c r="M27" s="58" t="s">
-        <v>246</v>
-      </c>
-      <c r="N27" s="50" t="s">
-        <v>250</v>
+      <c r="L27" s="74" t="s">
+        <v>239</v>
+      </c>
+      <c r="M27" s="53" t="s">
+        <v>245</v>
+      </c>
+      <c r="N27" s="45" t="s">
+        <v>249</v>
       </c>
       <c r="O27" s="12" t="s">
-        <v>267</v>
-      </c>
-      <c r="P27" s="51" t="s">
-        <v>261</v>
-      </c>
-      <c r="Q27" s="54" t="s">
+        <v>266</v>
+      </c>
+      <c r="P27" s="46" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q27" s="49" t="s">
+        <v>271</v>
+      </c>
+      <c r="R27" s="46" t="s">
         <v>272</v>
       </c>
-      <c r="R27" s="51" t="s">
-        <v>273</v>
-      </c>
-      <c r="S27" s="54" t="s">
-        <v>278</v>
-      </c>
-      <c r="T27" s="63"/>
+      <c r="S27" s="49" t="s">
+        <v>277</v>
+      </c>
+      <c r="T27" s="58"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
@@ -3379,35 +3363,35 @@
         <v>9</v>
       </c>
       <c r="G28" s="9"/>
-      <c r="H28" s="48"/>
-      <c r="K28" s="52" t="s">
-        <v>238</v>
-      </c>
-      <c r="L28" s="50" t="s">
-        <v>243</v>
-      </c>
-      <c r="M28" s="50" t="s">
-        <v>252</v>
-      </c>
-      <c r="N28" s="50" t="s">
-        <v>255</v>
+      <c r="H28" s="5"/>
+      <c r="K28" s="74" t="s">
+        <v>403</v>
+      </c>
+      <c r="L28" s="45" t="s">
+        <v>242</v>
+      </c>
+      <c r="M28" s="45" t="s">
+        <v>251</v>
+      </c>
+      <c r="N28" s="45" t="s">
+        <v>254</v>
       </c>
       <c r="O28" s="26" t="s">
-        <v>263</v>
-      </c>
-      <c r="P28" s="56" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q28" s="52" t="s">
-        <v>271</v>
-      </c>
-      <c r="R28" s="50" t="s">
-        <v>274</v>
-      </c>
-      <c r="S28" s="50" t="s">
-        <v>279</v>
-      </c>
-      <c r="T28" s="63"/>
+        <v>262</v>
+      </c>
+      <c r="P28" s="51" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q28" s="47" t="s">
+        <v>270</v>
+      </c>
+      <c r="R28" s="45" t="s">
+        <v>273</v>
+      </c>
+      <c r="S28" s="45" t="s">
+        <v>278</v>
+      </c>
+      <c r="T28" s="58"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
@@ -3426,34 +3410,34 @@
         <v>9</v>
       </c>
       <c r="J29" s="10"/>
-      <c r="K29" s="50" t="s">
-        <v>239</v>
-      </c>
-      <c r="L29" s="52" t="s">
-        <v>244</v>
-      </c>
-      <c r="M29" s="50" t="s">
-        <v>254</v>
-      </c>
-      <c r="N29" s="56" t="s">
-        <v>256</v>
+      <c r="K29" s="45" t="s">
+        <v>238</v>
+      </c>
+      <c r="L29" s="47" t="s">
+        <v>243</v>
+      </c>
+      <c r="M29" s="45" t="s">
+        <v>253</v>
+      </c>
+      <c r="N29" s="51" t="s">
+        <v>255</v>
       </c>
       <c r="O29" s="26" t="s">
-        <v>264</v>
-      </c>
-      <c r="P29" s="50" t="s">
-        <v>269</v>
-      </c>
-      <c r="Q29" s="56" t="s">
-        <v>277</v>
-      </c>
-      <c r="R29" s="50" t="s">
-        <v>275</v>
-      </c>
-      <c r="S29" s="50" t="s">
-        <v>281</v>
-      </c>
-      <c r="T29" s="63"/>
+        <v>263</v>
+      </c>
+      <c r="P29" s="45" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q29" s="51" t="s">
+        <v>276</v>
+      </c>
+      <c r="R29" s="45" t="s">
+        <v>274</v>
+      </c>
+      <c r="S29" s="45" t="s">
+        <v>280</v>
+      </c>
+      <c r="T29" s="58"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
@@ -3472,32 +3456,34 @@
         <v>9</v>
       </c>
       <c r="J30" s="10"/>
-      <c r="K30" s="79" t="s">
-        <v>241</v>
-      </c>
-      <c r="L30" s="52" t="s">
-        <v>245</v>
-      </c>
-      <c r="M30" s="50" t="s">
-        <v>253</v>
-      </c>
-      <c r="N30" s="50" t="s">
-        <v>258</v>
+      <c r="K30" s="74" t="s">
+        <v>240</v>
+      </c>
+      <c r="L30" s="47" t="s">
+        <v>244</v>
+      </c>
+      <c r="M30" s="45" t="s">
+        <v>252</v>
+      </c>
+      <c r="N30" s="45" t="s">
+        <v>257</v>
       </c>
       <c r="O30" s="17" t="s">
-        <v>265</v>
-      </c>
-      <c r="P30" s="50" t="s">
-        <v>270</v>
-      </c>
-      <c r="Q30" s="50"/>
-      <c r="R30" s="50" t="s">
-        <v>280</v>
-      </c>
-      <c r="S30" s="50" t="s">
-        <v>283</v>
-      </c>
-      <c r="T30" s="63"/>
+        <v>264</v>
+      </c>
+      <c r="P30" s="45" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q30" s="45" t="s">
+        <v>403</v>
+      </c>
+      <c r="R30" s="45" t="s">
+        <v>279</v>
+      </c>
+      <c r="S30" s="45" t="s">
+        <v>282</v>
+      </c>
+      <c r="T30" s="58"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
@@ -3516,32 +3502,32 @@
         <v>9</v>
       </c>
       <c r="J31" s="1"/>
-      <c r="K31" s="52" t="s">
-        <v>242</v>
-      </c>
-      <c r="L31" s="52" t="s">
-        <v>247</v>
-      </c>
-      <c r="M31" s="50" t="s">
-        <v>251</v>
-      </c>
-      <c r="N31" s="52" t="s">
-        <v>259</v>
+      <c r="K31" s="47" t="s">
+        <v>241</v>
+      </c>
+      <c r="L31" s="47" t="s">
+        <v>246</v>
+      </c>
+      <c r="M31" s="45" t="s">
+        <v>250</v>
+      </c>
+      <c r="N31" s="47" t="s">
+        <v>258</v>
       </c>
       <c r="O31" s="28" t="s">
-        <v>262</v>
-      </c>
-      <c r="P31" s="52" t="s">
-        <v>276</v>
-      </c>
-      <c r="Q31" s="52"/>
-      <c r="R31" s="50" t="s">
-        <v>282</v>
-      </c>
-      <c r="S31" s="52" t="s">
-        <v>284</v>
-      </c>
-      <c r="T31" s="63"/>
+        <v>261</v>
+      </c>
+      <c r="P31" s="47" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q31" s="47"/>
+      <c r="R31" s="45" t="s">
+        <v>281</v>
+      </c>
+      <c r="S31" s="47" t="s">
+        <v>283</v>
+      </c>
+      <c r="T31" s="58"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
@@ -3560,26 +3546,32 @@
         <v>9</v>
       </c>
       <c r="J32" s="1"/>
-      <c r="K32" s="79" t="s">
-        <v>249</v>
-      </c>
-      <c r="L32" s="52" t="s">
+      <c r="K32" s="74" t="s">
         <v>248</v>
       </c>
-      <c r="M32" s="50" t="s">
-        <v>257</v>
-      </c>
-      <c r="N32" s="52" t="s">
-        <v>260</v>
-      </c>
-      <c r="O32" s="28"/>
-      <c r="P32" s="52"/>
-      <c r="Q32" s="52"/>
-      <c r="R32" s="50"/>
-      <c r="S32" s="52" t="s">
-        <v>285</v>
-      </c>
-      <c r="T32" s="63"/>
+      <c r="L32" s="47" t="s">
+        <v>247</v>
+      </c>
+      <c r="M32" s="45" t="s">
+        <v>256</v>
+      </c>
+      <c r="N32" s="47" t="s">
+        <v>259</v>
+      </c>
+      <c r="O32" s="28" t="s">
+        <v>403</v>
+      </c>
+      <c r="P32" s="47" t="s">
+        <v>403</v>
+      </c>
+      <c r="Q32" s="47"/>
+      <c r="R32" s="45" t="s">
+        <v>403</v>
+      </c>
+      <c r="S32" s="47" t="s">
+        <v>284</v>
+      </c>
+      <c r="T32" s="58"/>
     </row>
     <row r="33" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
@@ -3588,22 +3580,26 @@
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="J33" s="10"/>
-      <c r="K33" s="79" t="s">
+      <c r="K33" s="74" t="s">
+        <v>402</v>
+      </c>
+      <c r="L33" s="48" t="s">
         <v>403</v>
       </c>
-      <c r="L33" s="53"/>
-      <c r="M33" s="55"/>
-      <c r="N33" s="53" t="s">
-        <v>266</v>
-      </c>
-      <c r="O33" s="44"/>
-      <c r="P33" s="53"/>
-      <c r="Q33" s="53"/>
-      <c r="R33" s="55"/>
-      <c r="S33" s="53" t="s">
-        <v>286</v>
-      </c>
-      <c r="T33" s="63" t="s">
+      <c r="M33" s="50" t="s">
+        <v>403</v>
+      </c>
+      <c r="N33" s="48" t="s">
+        <v>265</v>
+      </c>
+      <c r="O33" s="43"/>
+      <c r="P33" s="48"/>
+      <c r="Q33" s="48"/>
+      <c r="R33" s="50"/>
+      <c r="S33" s="48" t="s">
+        <v>285</v>
+      </c>
+      <c r="T33" s="58" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3623,11 +3619,11 @@
       <c r="E34" s="8">
         <v>10</v>
       </c>
-      <c r="J34" s="60" t="s">
+      <c r="J34" s="55" t="s">
         <v>20</v>
       </c>
       <c r="K34" s="31">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="L34" s="31"/>
       <c r="M34" s="31"/>
@@ -3637,9 +3633,9 @@
       <c r="Q34" s="31"/>
       <c r="R34" s="31"/>
       <c r="S34" s="31"/>
-      <c r="T34" s="64">
+      <c r="T34" s="59">
         <f>K34+L34+M34+N34+O34+P34+Q34+R34+S34</f>
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3658,13 +3654,15 @@
       <c r="E35" s="8">
         <v>10</v>
       </c>
-      <c r="J35" s="62" t="s">
+      <c r="J35" s="57" t="s">
         <v>21</v>
       </c>
       <c r="K35" s="37">
-        <v>20</v>
-      </c>
-      <c r="L35" s="37"/>
+        <v>80</v>
+      </c>
+      <c r="L35" s="37">
+        <v>30</v>
+      </c>
       <c r="M35" s="37"/>
       <c r="N35" s="37"/>
       <c r="O35" s="37"/>
@@ -3672,9 +3670,9 @@
       <c r="Q35" s="37"/>
       <c r="R35" s="37"/>
       <c r="S35" s="37"/>
-      <c r="T35" s="72">
+      <c r="T35" s="65">
         <f>K35+L35+M35+N35+O35+P35+Q35+R35+S35</f>
-        <v>20</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3697,12 +3695,12 @@
       <c r="K36" s="35"/>
       <c r="L36" s="35"/>
       <c r="R36" s="35"/>
-      <c r="T36" s="71">
+      <c r="T36" s="73">
         <f>T34+T35</f>
-        <v>40</v>
-      </c>
-      <c r="U36" s="71" t="s">
-        <v>373</v>
+        <v>145</v>
+      </c>
+      <c r="U36" s="73" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -3869,7 +3867,7 @@
       <c r="E44" s="8">
         <v>8</v>
       </c>
-      <c r="N44" s="65"/>
+      <c r="N44" s="60"/>
       <c r="O44" s="8"/>
       <c r="Q44" s="10"/>
       <c r="R44" s="8"/>
@@ -4446,7 +4444,7 @@
       <c r="E72" s="8">
         <v>10</v>
       </c>
-      <c r="H72" s="49"/>
+      <c r="H72" s="4"/>
       <c r="Q72" s="10"/>
       <c r="R72" s="8"/>
       <c r="S72" s="19"/>
@@ -5584,8 +5582,8 @@
       <c r="E132" s="8">
         <v>8</v>
       </c>
-      <c r="K132" s="65"/>
-      <c r="L132" s="65"/>
+      <c r="K132" s="60"/>
+      <c r="L132" s="60"/>
       <c r="M132" s="35"/>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
@@ -6067,7 +6065,7 @@
       <c r="E160" s="8">
         <v>4</v>
       </c>
-      <c r="R160" s="65"/>
+      <c r="R160" s="60"/>
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
@@ -6382,7 +6380,7 @@
       <c r="E180" s="8">
         <v>7</v>
       </c>
-      <c r="F180" s="48"/>
+      <c r="F180" s="5"/>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
@@ -6942,7 +6940,7 @@
       <c r="E217" s="8">
         <v>5</v>
       </c>
-      <c r="I217" s="66"/>
+      <c r="I217" s="75"/>
     </row>
     <row r="218" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
@@ -6960,7 +6958,7 @@
       <c r="E218" s="8">
         <v>5</v>
       </c>
-      <c r="I218" s="66"/>
+      <c r="I218" s="75"/>
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A219" s="5"/>
@@ -6968,7 +6966,7 @@
       <c r="C219" s="7"/>
       <c r="D219" s="8"/>
       <c r="E219" s="8"/>
-      <c r="I219" s="66"/>
+      <c r="I219" s="75"/>
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A220" s="27" t="s">
@@ -6986,7 +6984,7 @@
       <c r="E220" s="8">
         <v>5</v>
       </c>
-      <c r="I220" s="66"/>
+      <c r="I220" s="75"/>
     </row>
     <row r="221" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A221" s="27" t="s">
@@ -7004,7 +7002,7 @@
       <c r="E221" s="8">
         <v>5</v>
       </c>
-      <c r="I221" s="66"/>
+      <c r="I221" s="75"/>
       <c r="J221" s="35"/>
       <c r="K221" s="35"/>
       <c r="L221" s="35"/>
@@ -7025,7 +7023,7 @@
       <c r="E222" s="8">
         <v>5</v>
       </c>
-      <c r="I222" s="66"/>
+      <c r="I222" s="75"/>
       <c r="J222" s="35"/>
       <c r="K222" s="35"/>
       <c r="L222" s="35"/>
@@ -7046,7 +7044,7 @@
       <c r="E223" s="8">
         <v>5</v>
       </c>
-      <c r="I223" s="66"/>
+      <c r="I223" s="75"/>
       <c r="J223" s="35"/>
       <c r="K223" s="35"/>
       <c r="L223" s="35"/>
@@ -7057,7 +7055,7 @@
       <c r="C224" s="7"/>
       <c r="D224" s="8"/>
       <c r="E224" s="8"/>
-      <c r="I224" s="66"/>
+      <c r="I224" s="75"/>
       <c r="J224" s="35"/>
       <c r="K224" s="35"/>
       <c r="L224" s="35"/>
@@ -7078,7 +7076,7 @@
       <c r="E225" s="8">
         <v>5</v>
       </c>
-      <c r="I225" s="66"/>
+      <c r="I225" s="75"/>
       <c r="J225" s="35"/>
       <c r="K225" s="35"/>
       <c r="L225" s="35"/>
@@ -7100,7 +7098,7 @@
       <c r="E226" s="8">
         <v>5</v>
       </c>
-      <c r="I226" s="66"/>
+      <c r="I226" s="75"/>
       <c r="J226" s="35"/>
       <c r="K226" s="35"/>
       <c r="L226" s="35"/>
@@ -7122,7 +7120,7 @@
       <c r="E227" s="8">
         <v>5</v>
       </c>
-      <c r="I227" s="66"/>
+      <c r="I227" s="75"/>
       <c r="J227" s="35"/>
       <c r="K227" s="35"/>
       <c r="L227" s="35"/>
@@ -7144,7 +7142,7 @@
       <c r="E228" s="8">
         <v>5</v>
       </c>
-      <c r="I228" s="66"/>
+      <c r="I228" s="75"/>
       <c r="J228" s="35"/>
       <c r="K228" s="35"/>
       <c r="L228" s="35"/>
@@ -7156,8 +7154,8 @@
       <c r="C229" s="7"/>
       <c r="D229" s="8"/>
       <c r="E229" s="8"/>
-      <c r="I229" s="66"/>
-      <c r="J229" s="65"/>
+      <c r="I229" s="75"/>
+      <c r="J229" s="60"/>
       <c r="K229" s="35"/>
       <c r="L229" s="35"/>
       <c r="S229" s="35"/>
@@ -7178,7 +7176,7 @@
       <c r="E230" s="8">
         <v>6</v>
       </c>
-      <c r="I230" s="66"/>
+      <c r="I230" s="75"/>
       <c r="J230" s="35"/>
       <c r="K230" s="35"/>
       <c r="L230" s="35"/>
@@ -7200,7 +7198,7 @@
       <c r="E231" s="8">
         <v>6</v>
       </c>
-      <c r="I231" s="66"/>
+      <c r="I231" s="75"/>
       <c r="J231" s="35"/>
       <c r="K231" s="35"/>
       <c r="L231" s="35"/>
@@ -7222,7 +7220,7 @@
       <c r="E232" s="8">
         <v>6</v>
       </c>
-      <c r="I232" s="66"/>
+      <c r="I232" s="75"/>
       <c r="J232" s="15"/>
       <c r="K232" s="35"/>
       <c r="L232" s="35"/>
@@ -7244,7 +7242,7 @@
       <c r="E233" s="8">
         <v>6</v>
       </c>
-      <c r="I233" s="66"/>
+      <c r="I233" s="75"/>
       <c r="J233" s="15"/>
       <c r="K233" s="35"/>
       <c r="L233" s="35"/>
@@ -7256,7 +7254,7 @@
       <c r="C234" s="7"/>
       <c r="D234" s="8"/>
       <c r="E234" s="8"/>
-      <c r="I234" s="66"/>
+      <c r="I234" s="75"/>
       <c r="J234" s="15"/>
       <c r="K234" s="35"/>
       <c r="L234" s="35"/>
@@ -7278,7 +7276,7 @@
       <c r="E235" s="8">
         <v>6</v>
       </c>
-      <c r="I235" s="66"/>
+      <c r="I235" s="75"/>
       <c r="J235" s="15"/>
       <c r="K235" s="35"/>
       <c r="L235" s="35"/>
@@ -7300,7 +7298,7 @@
       <c r="E236" s="8">
         <v>6</v>
       </c>
-      <c r="I236" s="66"/>
+      <c r="I236" s="75"/>
       <c r="J236" s="15"/>
       <c r="K236" s="35"/>
       <c r="L236" s="35"/>
@@ -7322,7 +7320,7 @@
       <c r="E237" s="8">
         <v>6</v>
       </c>
-      <c r="I237" s="66"/>
+      <c r="I237" s="75"/>
       <c r="J237" s="35"/>
       <c r="K237" s="35"/>
       <c r="L237" s="35"/>
@@ -7344,7 +7342,7 @@
       <c r="E238" s="8">
         <v>6</v>
       </c>
-      <c r="I238" s="66"/>
+      <c r="I238" s="75"/>
       <c r="J238" s="35"/>
       <c r="K238" s="35"/>
       <c r="L238" s="35"/>
@@ -7396,7 +7394,7 @@
       <c r="E241" s="19">
         <v>6</v>
       </c>
-      <c r="J241" s="67"/>
+      <c r="J241" s="61"/>
       <c r="K241" s="35"/>
       <c r="L241" s="35"/>
     </row>
@@ -7496,8 +7494,8 @@
         <v>6</v>
       </c>
       <c r="G247" s="9"/>
-      <c r="H247" s="48"/>
-      <c r="I247" s="48"/>
+      <c r="H247" s="5"/>
+      <c r="I247" s="5"/>
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A248" s="27" t="s">
@@ -7516,16 +7514,16 @@
         <v>6</v>
       </c>
       <c r="G248" s="9"/>
-      <c r="H248" s="48"/>
-      <c r="I248" s="48"/>
+      <c r="H248" s="5"/>
+      <c r="I248" s="5"/>
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A249" s="27"/>
       <c r="B249" s="7"/>
       <c r="C249" s="7"/>
       <c r="G249" s="9"/>
-      <c r="H249" s="48"/>
-      <c r="I249" s="48"/>
+      <c r="H249" s="5"/>
+      <c r="I249" s="5"/>
     </row>
     <row r="250" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A250" s="5" t="s">
@@ -7544,8 +7542,8 @@
         <v>4</v>
       </c>
       <c r="G250" s="9"/>
-      <c r="H250" s="48"/>
-      <c r="I250" s="48"/>
+      <c r="H250" s="5"/>
+      <c r="I250" s="5"/>
     </row>
     <row r="251" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A251" s="5" t="s">
@@ -7564,8 +7562,8 @@
         <v>4</v>
       </c>
       <c r="G251" s="9"/>
-      <c r="H251" s="48"/>
-      <c r="I251" s="48"/>
+      <c r="H251" s="5"/>
+      <c r="I251" s="5"/>
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A252" s="5" t="s">
@@ -7584,8 +7582,8 @@
         <v>4</v>
       </c>
       <c r="G252" s="9"/>
-      <c r="H252" s="48"/>
-      <c r="I252" s="48"/>
+      <c r="H252" s="5"/>
+      <c r="I252" s="5"/>
     </row>
     <row r="253" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A253" s="5" t="s">
@@ -7677,16 +7675,16 @@
         <v>4</v>
       </c>
       <c r="G258" s="5"/>
-      <c r="H258" s="48"/>
-      <c r="I258" s="48"/>
+      <c r="H258" s="5"/>
+      <c r="I258" s="5"/>
     </row>
     <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" s="5"/>
       <c r="B259" s="7"/>
       <c r="C259" s="7"/>
       <c r="G259" s="5"/>
-      <c r="H259" s="48"/>
-      <c r="I259" s="48"/>
+      <c r="H259" s="5"/>
+      <c r="I259" s="5"/>
     </row>
     <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" s="5" t="s">
@@ -7705,8 +7703,8 @@
         <v>4</v>
       </c>
       <c r="G260" s="5"/>
-      <c r="H260" s="48"/>
-      <c r="I260" s="48"/>
+      <c r="H260" s="5"/>
+      <c r="I260" s="5"/>
     </row>
     <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" s="5" t="s">
@@ -7725,8 +7723,8 @@
         <v>4</v>
       </c>
       <c r="G261" s="5"/>
-      <c r="H261" s="48"/>
-      <c r="I261" s="48"/>
+      <c r="H261" s="5"/>
+      <c r="I261" s="5"/>
     </row>
     <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" s="5" t="s">
@@ -7745,8 +7743,8 @@
         <v>4</v>
       </c>
       <c r="G262" s="5"/>
-      <c r="H262" s="48"/>
-      <c r="I262" s="48"/>
+      <c r="H262" s="5"/>
+      <c r="I262" s="5"/>
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" s="5" t="s">
@@ -7765,8 +7763,8 @@
         <v>4</v>
       </c>
       <c r="G263" s="5"/>
-      <c r="H263" s="48"/>
-      <c r="I263" s="48"/>
+      <c r="H263" s="5"/>
+      <c r="I263" s="5"/>
     </row>
     <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" s="5"/>
@@ -8300,7 +8298,7 @@
       <c r="E300" s="8">
         <v>6</v>
       </c>
-      <c r="F300" s="48"/>
+      <c r="F300" s="5"/>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" s="5" t="s">
@@ -8318,7 +8316,7 @@
       <c r="E301" s="8">
         <v>6</v>
       </c>
-      <c r="F301" s="48"/>
+      <c r="F301" s="5"/>
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" s="5" t="s">
@@ -9308,7 +9306,7 @@
       <c r="E365" s="8">
         <v>6</v>
       </c>
-      <c r="F365" s="48"/>
+      <c r="F365" s="5"/>
     </row>
     <row r="366" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A366" s="27" t="s">
@@ -10959,7 +10957,7 @@
       <c r="E472" s="8">
         <v>4</v>
       </c>
-      <c r="F472" s="48"/>
+      <c r="F472" s="5"/>
     </row>
     <row r="473" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A473" s="5" t="s">
@@ -10977,7 +10975,7 @@
       <c r="E473" s="8">
         <v>4</v>
       </c>
-      <c r="F473" s="48"/>
+      <c r="F473" s="5"/>
     </row>
     <row r="474" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A474" s="5" t="s">
@@ -11336,7 +11334,7 @@
       <c r="E497" s="8">
         <v>10</v>
       </c>
-      <c r="F497" s="48"/>
+      <c r="F497" s="5"/>
     </row>
     <row r="498" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A498" s="27" t="s">
@@ -12117,7 +12115,7 @@
       <c r="E554" s="8">
         <v>9</v>
       </c>
-      <c r="F554" s="48"/>
+      <c r="F554" s="5"/>
       <c r="G554" s="41"/>
     </row>
     <row r="555" spans="1:7" x14ac:dyDescent="0.25">
@@ -12136,7 +12134,7 @@
       <c r="E555" s="8">
         <v>9</v>
       </c>
-      <c r="F555" s="48"/>
+      <c r="F555" s="5"/>
       <c r="G555" s="41"/>
     </row>
     <row r="556" spans="1:7" x14ac:dyDescent="0.25">
@@ -12145,7 +12143,7 @@
       <c r="C556" s="7"/>
       <c r="D556" s="8"/>
       <c r="E556" s="8"/>
-      <c r="F556" s="48"/>
+      <c r="F556" s="5"/>
       <c r="G556" s="41"/>
     </row>
     <row r="557" spans="1:7" x14ac:dyDescent="0.25">
@@ -12477,7 +12475,7 @@
         <f>SUM(D2:D579)</f>
         <v>2363</v>
       </c>
-      <c r="E580" s="45"/>
+      <c r="E580" s="44"/>
     </row>
     <row r="581" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A581" s="5" t="s">
@@ -12495,7 +12493,7 @@
       <c r="E581" s="8">
         <v>8</v>
       </c>
-      <c r="H581" s="49"/>
+      <c r="H581" s="4"/>
     </row>
     <row r="582" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A582" s="5" t="s">
@@ -12513,7 +12511,7 @@
       <c r="E582" s="8">
         <v>8</v>
       </c>
-      <c r="H582" s="49"/>
+      <c r="H582" s="4"/>
     </row>
     <row r="583" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A583" s="5" t="s">
@@ -12531,7 +12529,7 @@
       <c r="E583" s="8">
         <v>6</v>
       </c>
-      <c r="H583" s="49"/>
+      <c r="H583" s="4"/>
     </row>
     <row r="584" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A584" s="5" t="s">
@@ -12549,7 +12547,7 @@
       <c r="E584" s="8">
         <v>7</v>
       </c>
-      <c r="H584" s="49"/>
+      <c r="H584" s="4"/>
     </row>
     <row r="585" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A585" s="27" t="s">
@@ -12567,7 +12565,7 @@
       <c r="E585" s="8">
         <v>8</v>
       </c>
-      <c r="H585" s="49"/>
+      <c r="H585" s="4"/>
     </row>
     <row r="586" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A586" s="5" t="s">
@@ -12585,7 +12583,7 @@
       <c r="E586" s="8">
         <v>7</v>
       </c>
-      <c r="H586" s="49"/>
+      <c r="H586" s="4"/>
     </row>
     <row r="587" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A587" s="5" t="s">
@@ -12603,7 +12601,7 @@
       <c r="E587" s="8">
         <v>7</v>
       </c>
-      <c r="H587" s="49"/>
+      <c r="H587" s="4"/>
     </row>
     <row r="588" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A588" s="5" t="s">
@@ -12621,7 +12619,7 @@
       <c r="E588" s="8">
         <v>7</v>
       </c>
-      <c r="H588" s="49"/>
+      <c r="H588" s="4"/>
     </row>
     <row r="589" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A589" s="5" t="s">
@@ -12639,11 +12637,11 @@
       <c r="E589" s="8">
         <v>4</v>
       </c>
-      <c r="H589" s="49"/>
+      <c r="H589" s="4"/>
     </row>
     <row r="590" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A590" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B590" s="25" t="s">
         <v>11</v>
@@ -12657,7 +12655,7 @@
       <c r="E590" s="8">
         <v>2</v>
       </c>
-      <c r="H590" s="49"/>
+      <c r="H590" s="4"/>
     </row>
     <row r="591" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A591" s="27"/>
@@ -12665,7 +12663,7 @@
       <c r="C591" s="7"/>
       <c r="D591" s="8"/>
       <c r="E591" s="8"/>
-      <c r="H591" s="49"/>
+      <c r="H591" s="4"/>
     </row>
     <row r="592" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A592" s="5" t="s">
@@ -12683,7 +12681,7 @@
       <c r="E592" s="8">
         <v>8</v>
       </c>
-      <c r="H592" s="49"/>
+      <c r="H592" s="4"/>
     </row>
     <row r="593" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A593" s="5" t="s">
@@ -12701,7 +12699,7 @@
       <c r="E593" s="8">
         <v>7</v>
       </c>
-      <c r="H593" s="49"/>
+      <c r="H593" s="4"/>
     </row>
     <row r="594" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A594" s="5" t="s">
@@ -12719,7 +12717,7 @@
       <c r="E594" s="8">
         <v>6</v>
       </c>
-      <c r="H594" s="49"/>
+      <c r="H594" s="4"/>
     </row>
     <row r="595" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A595" s="5" t="s">
@@ -12931,7 +12929,7 @@
       <c r="E608" s="8">
         <v>7</v>
       </c>
-      <c r="H608" s="49"/>
+      <c r="H608" s="4"/>
     </row>
     <row r="609" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A609" s="5" t="s">
@@ -12949,7 +12947,7 @@
       <c r="E609" s="8">
         <v>8</v>
       </c>
-      <c r="H609" s="49"/>
+      <c r="H609" s="4"/>
     </row>
     <row r="610" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A610" s="5" t="s">
@@ -12967,7 +12965,7 @@
       <c r="E610" s="8">
         <v>9</v>
       </c>
-      <c r="H610" s="49"/>
+      <c r="H610" s="4"/>
     </row>
     <row r="611" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A611" s="27" t="s">
@@ -12985,7 +12983,7 @@
       <c r="E611" s="8">
         <v>10</v>
       </c>
-      <c r="H611" s="49"/>
+      <c r="H611" s="4"/>
     </row>
     <row r="612" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A612" s="5" t="s">
@@ -13003,7 +13001,7 @@
       <c r="E612" s="8">
         <v>7</v>
       </c>
-      <c r="H612" s="49"/>
+      <c r="H612" s="4"/>
     </row>
     <row r="613" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A613" s="5" t="s">
@@ -13021,7 +13019,7 @@
       <c r="E613" s="8">
         <v>4</v>
       </c>
-      <c r="H613" s="49"/>
+      <c r="H613" s="4"/>
     </row>
     <row r="614" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A614" s="5" t="s">
@@ -13039,7 +13037,7 @@
       <c r="E614" s="8">
         <v>4</v>
       </c>
-      <c r="H614" s="49"/>
+      <c r="H614" s="4"/>
     </row>
     <row r="615" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A615" s="5" t="s">
@@ -13088,7 +13086,7 @@
       <c r="C618" s="7"/>
       <c r="D618" s="8"/>
       <c r="E618" s="8"/>
-      <c r="F618" s="43"/>
+      <c r="F618" s="9"/>
     </row>
     <row r="619" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A619" s="5" t="s">
@@ -13106,7 +13104,7 @@
       <c r="E619" s="8">
         <v>6</v>
       </c>
-      <c r="F619" s="43"/>
+      <c r="F619" s="9"/>
     </row>
     <row r="620" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A620" s="27" t="s">

</xml_diff>

<commit_message>
Alles geupdate UML & Asset List & Uren Registratie Nicu
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -2105,7 +2105,7 @@
   <dimension ref="A1:U1028"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44"/>
+      <selection activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3662,7 +3662,7 @@
         <v>20</v>
       </c>
       <c r="K35" s="30">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="L35" s="30"/>
       <c r="M35" s="30"/>
@@ -3674,7 +3674,7 @@
       <c r="S35" s="30"/>
       <c r="T35" s="54">
         <f>K35+L35+M35+N35+O35+P35+Q35+R35+S35</f>
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3739,7 +3739,7 @@
       <c r="R37" s="31"/>
       <c r="T37" s="68">
         <f>T35+T36</f>
-        <v>230</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Bug fixes met cover
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -1560,7 +1560,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1785,6 +1785,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2105,7 +2111,7 @@
   <dimension ref="A1:U1028"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O41" sqref="O41"/>
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3376,7 +3382,7 @@
       <c r="K28" s="69" t="s">
         <v>403</v>
       </c>
-      <c r="L28" s="14" t="s">
+      <c r="L28" s="79" t="s">
         <v>242</v>
       </c>
       <c r="M28" s="40" t="s">
@@ -3558,7 +3564,7 @@
       <c r="K32" s="69" t="s">
         <v>248</v>
       </c>
-      <c r="L32" s="15" t="s">
+      <c r="L32" s="78" t="s">
         <v>247</v>
       </c>
       <c r="M32" s="40" t="s">
@@ -3700,7 +3706,7 @@
         <v>110</v>
       </c>
       <c r="L36" s="33">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="M36" s="33"/>
       <c r="N36" s="33"/>
@@ -3711,7 +3717,7 @@
       <c r="S36" s="33"/>
       <c r="T36" s="60">
         <f>K36+L36+M36+N36+O36+P36+Q36+R36+S36</f>
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="U36" s="68" t="s">
         <v>372</v>
@@ -3739,7 +3745,7 @@
       <c r="R37" s="31"/>
       <c r="T37" s="68">
         <f>T35+T36</f>
-        <v>235</v>
+        <v>275</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Uren Registratie 15-03-2016 & UML Update & Jump
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -1560,7 +1560,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1769,9 +1769,6 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1790,7 +1787,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2111,7 +2108,7 @@
   <dimension ref="A1:U1028"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O40" sqref="O40"/>
+      <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3332,28 +3329,28 @@
       </c>
       <c r="G27" s="9"/>
       <c r="J27" s="10"/>
-      <c r="K27" s="72" t="s">
+      <c r="K27" s="78" t="s">
         <v>237</v>
       </c>
-      <c r="L27" s="76" t="s">
+      <c r="L27" s="75" t="s">
         <v>239</v>
       </c>
       <c r="M27" s="44" t="s">
         <v>245</v>
       </c>
-      <c r="N27" s="74" t="s">
+      <c r="N27" s="73" t="s">
         <v>249</v>
       </c>
       <c r="O27" s="44" t="s">
         <v>266</v>
       </c>
-      <c r="P27" s="74" t="s">
+      <c r="P27" s="73" t="s">
         <v>260</v>
       </c>
       <c r="Q27" s="44" t="s">
         <v>271</v>
       </c>
-      <c r="R27" s="74" t="s">
+      <c r="R27" s="73" t="s">
         <v>272</v>
       </c>
       <c r="S27" s="44" t="s">
@@ -3382,7 +3379,7 @@
       <c r="K28" s="69" t="s">
         <v>403</v>
       </c>
-      <c r="L28" s="79" t="s">
+      <c r="L28" s="77" t="s">
         <v>242</v>
       </c>
       <c r="M28" s="40" t="s">
@@ -3394,7 +3391,7 @@
       <c r="O28" s="71" t="s">
         <v>262</v>
       </c>
-      <c r="P28" s="75" t="s">
+      <c r="P28" s="74" t="s">
         <v>267</v>
       </c>
       <c r="Q28" s="42" t="s">
@@ -3434,7 +3431,7 @@
       <c r="M29" s="40" t="s">
         <v>253</v>
       </c>
-      <c r="N29" s="75" t="s">
+      <c r="N29" s="74" t="s">
         <v>255</v>
       </c>
       <c r="O29" s="71" t="s">
@@ -3564,7 +3561,7 @@
       <c r="K32" s="69" t="s">
         <v>248</v>
       </c>
-      <c r="L32" s="78" t="s">
+      <c r="L32" s="77" t="s">
         <v>247</v>
       </c>
       <c r="M32" s="40" t="s">
@@ -3635,7 +3632,7 @@
         <v>10</v>
       </c>
       <c r="J34" s="10"/>
-      <c r="K34" s="77" t="s">
+      <c r="K34" s="76" t="s">
         <v>404</v>
       </c>
       <c r="L34" s="26"/>
@@ -3644,7 +3641,7 @@
       <c r="O34" s="43"/>
       <c r="P34" s="26"/>
       <c r="Q34" s="43"/>
-      <c r="R34" s="73"/>
+      <c r="R34" s="72"/>
       <c r="S34" s="43"/>
       <c r="T34" s="53"/>
     </row>
@@ -3668,7 +3665,7 @@
         <v>20</v>
       </c>
       <c r="K35" s="30">
-        <v>95</v>
+        <v>165</v>
       </c>
       <c r="L35" s="30"/>
       <c r="M35" s="30"/>
@@ -3680,7 +3677,7 @@
       <c r="S35" s="30"/>
       <c r="T35" s="54">
         <f>K35+L35+M35+N35+O35+P35+Q35+R35+S35</f>
-        <v>95</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3706,7 +3703,7 @@
         <v>110</v>
       </c>
       <c r="L36" s="33">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="M36" s="33"/>
       <c r="N36" s="33"/>
@@ -3717,7 +3714,7 @@
       <c r="S36" s="33"/>
       <c r="T36" s="60">
         <f>K36+L36+M36+N36+O36+P36+Q36+R36+S36</f>
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="U36" s="68" t="s">
         <v>372</v>
@@ -3745,7 +3742,7 @@
       <c r="R37" s="31"/>
       <c r="T37" s="68">
         <f>T35+T36</f>
-        <v>275</v>
+        <v>365</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Uren Registratie Vorig Week, check of het even klopt & Asset list update
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -1560,7 +1560,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1788,6 +1788,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2107,8 +2113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O42" sqref="O42"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2278,7 +2284,7 @@
         <v>229</v>
       </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="28" t="s">
+      <c r="K3" s="80" t="s">
         <v>288</v>
       </c>
       <c r="L3" s="61" t="s">
@@ -2335,7 +2341,7 @@
         <v>230</v>
       </c>
       <c r="J4" s="10"/>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="79" t="s">
         <v>289</v>
       </c>
       <c r="L4" s="13" t="s">
@@ -2449,7 +2455,7 @@
         <v>224</v>
       </c>
       <c r="J6" s="1"/>
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="79" t="s">
         <v>295</v>
       </c>
       <c r="L6" s="58" t="s">
@@ -2608,7 +2614,7 @@
         <v>226</v>
       </c>
       <c r="J9" s="1"/>
-      <c r="K9" s="21" t="s">
+      <c r="K9" s="79" t="s">
         <v>294</v>
       </c>
       <c r="L9" s="58" t="s">
@@ -3471,7 +3477,7 @@
       <c r="K30" s="69" t="s">
         <v>240</v>
       </c>
-      <c r="L30" s="15" t="s">
+      <c r="L30" s="77" t="s">
         <v>244</v>
       </c>
       <c r="M30" s="40" t="s">
@@ -3595,7 +3601,7 @@
       <c r="K33" s="69" t="s">
         <v>402</v>
       </c>
-      <c r="L33" s="15" t="s">
+      <c r="L33" s="77" t="s">
         <v>403</v>
       </c>
       <c r="M33" s="40" t="s">
@@ -3703,7 +3709,7 @@
         <v>110</v>
       </c>
       <c r="L36" s="33">
-        <v>90</v>
+        <v>145</v>
       </c>
       <c r="M36" s="33"/>
       <c r="N36" s="33"/>
@@ -3714,7 +3720,7 @@
       <c r="S36" s="33"/>
       <c r="T36" s="60">
         <f>K36+L36+M36+N36+O36+P36+Q36+R36+S36</f>
-        <v>200</v>
+        <v>255</v>
       </c>
       <c r="U36" s="68" t="s">
         <v>372</v>
@@ -3742,7 +3748,7 @@
       <c r="R37" s="31"/>
       <c r="T37" s="68">
         <f>T35+T36</f>
-        <v>365</v>
+        <v>420</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AI Conversation af & Asset list update artist en development
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1839" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="406">
   <si>
     <t>ID Code</t>
   </si>
@@ -1232,6 +1232,9 @@
   </si>
   <si>
     <t>Player_Interaction (70)</t>
+  </si>
+  <si>
+    <t>Game_ConversationTrigger(10)</t>
   </si>
 </sst>
 </file>
@@ -1560,7 +1563,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1794,6 +1797,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2114,7 +2120,7 @@
   <dimension ref="A1:U1028"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2398,7 +2404,7 @@
         <v>234</v>
       </c>
       <c r="J5" s="10"/>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="79" t="s">
         <v>290</v>
       </c>
       <c r="L5" s="58" t="s">
@@ -2512,7 +2518,7 @@
         <v>225</v>
       </c>
       <c r="J7" s="1"/>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="79" t="s">
         <v>292</v>
       </c>
       <c r="L7" s="58" t="s">
@@ -2569,7 +2575,7 @@
         <v>231</v>
       </c>
       <c r="J8" s="1"/>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="57" t="s">
         <v>293</v>
       </c>
       <c r="L8" s="58" t="s">
@@ -3431,7 +3437,7 @@
       <c r="K29" s="69" t="s">
         <v>238</v>
       </c>
-      <c r="L29" s="15" t="s">
+      <c r="L29" s="77" t="s">
         <v>243</v>
       </c>
       <c r="M29" s="40" t="s">
@@ -3641,7 +3647,9 @@
       <c r="K34" s="76" t="s">
         <v>404</v>
       </c>
-      <c r="L34" s="26"/>
+      <c r="L34" s="81" t="s">
+        <v>405</v>
+      </c>
       <c r="M34" s="45"/>
       <c r="N34" s="26"/>
       <c r="O34" s="43"/>
@@ -3673,7 +3681,9 @@
       <c r="K35" s="30">
         <v>165</v>
       </c>
-      <c r="L35" s="30"/>
+      <c r="L35" s="30">
+        <v>60</v>
+      </c>
       <c r="M35" s="30"/>
       <c r="N35" s="30"/>
       <c r="O35" s="30"/>
@@ -3683,7 +3693,7 @@
       <c r="S35" s="30"/>
       <c r="T35" s="54">
         <f>K35+L35+M35+N35+O35+P35+Q35+R35+S35</f>
-        <v>165</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3748,7 +3758,7 @@
       <c r="R37" s="31"/>
       <c r="T37" s="68">
         <f>T35+T36</f>
-        <v>420</v>
+        <v>480</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Scene met melee in elkaar gezet & UML update met Asset list
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -730,18 +730,12 @@
     <t>Development</t>
   </si>
   <si>
-    <t>Player_Movement (70)</t>
-  </si>
-  <si>
     <t>Weapons_WeaponManager (60)</t>
   </si>
   <si>
     <t>Weapons_AbstractWeapons (30)</t>
   </si>
   <si>
-    <t>Player_CameraControl (10)</t>
-  </si>
-  <si>
     <t>Player_Interact (10)</t>
   </si>
   <si>
@@ -1231,10 +1225,16 @@
     <t>Game_GameManager (15)</t>
   </si>
   <si>
-    <t>Player_Interaction (70)</t>
-  </si>
-  <si>
-    <t>Game_ConversationTrigger(10)</t>
+    <t>Player_Movement (80)</t>
+  </si>
+  <si>
+    <t>Player_CameraControl (20)</t>
+  </si>
+  <si>
+    <t>Game_Interaction (70)</t>
+  </si>
+  <si>
+    <t>Game_ConversationTrigger (10)</t>
   </si>
 </sst>
 </file>
@@ -2120,7 +2120,7 @@
   <dimension ref="A1:U1028"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2291,31 +2291,31 @@
       </c>
       <c r="J3" s="10"/>
       <c r="K3" s="80" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="L3" s="61" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="M3" s="61" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="N3" s="65" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="P3" s="41" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="R3" s="41" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="S3" s="65" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -2348,31 +2348,31 @@
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="79" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="N4" s="42" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="O4" s="15" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="P4" s="40" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="R4" s="40" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="S4" s="42" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -2405,31 +2405,31 @@
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="79" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="L5" s="58" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="N5" s="42" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="O5" s="15" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="P5" s="42" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="Q5" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="R5" s="42" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="S5" s="40" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -2462,31 +2462,31 @@
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="79" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="L6" s="58" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="N6" s="42" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O6" s="15" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="P6" s="40" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="R6" s="40" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="S6" s="40" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -2519,31 +2519,31 @@
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="79" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="L7" s="58" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="N7" s="42" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O7" s="58" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="P7" s="42" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="R7" s="40" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="S7" s="40" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -2576,31 +2576,31 @@
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="57" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="L8" s="58" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="M8" s="13" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="N8" s="48" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O8" s="58" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="P8" s="40" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="R8" s="40" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="S8" s="40" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -2621,31 +2621,31 @@
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="79" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="L9" s="58" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="N9" s="46" t="s">
+        <v>315</v>
+      </c>
+      <c r="O9" s="58" t="s">
         <v>317</v>
       </c>
-      <c r="O9" s="58" t="s">
-        <v>319</v>
-      </c>
       <c r="P9" s="40" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="Q9" s="10" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="R9" s="40" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="S9" s="40" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -2676,31 +2676,31 @@
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="58" t="s">
+        <v>392</v>
+      </c>
+      <c r="L10" s="64" t="s">
         <v>394</v>
       </c>
-      <c r="L10" s="64" t="s">
-        <v>396</v>
-      </c>
       <c r="M10" s="13" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="N10" s="46" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="O10" s="13" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="P10" s="40" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="Q10" s="58" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="R10" s="40" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="S10" s="40" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -2730,28 +2730,28 @@
       <c r="J11" s="1"/>
       <c r="K11" s="21"/>
       <c r="L11" s="13" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="M11" s="57" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="N11" s="42" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="O11" s="13" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="P11" s="40" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="Q11" s="13" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="R11" s="40" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="S11" s="40" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -2775,33 +2775,33 @@
         <v>41</v>
       </c>
       <c r="I12" s="66" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="21"/>
       <c r="L12" s="13" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="M12" s="58" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="N12" s="46" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="O12" s="58" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="P12" s="42" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="Q12" s="13" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="R12" s="40" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="S12" s="42" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -2825,33 +2825,33 @@
         <v>41</v>
       </c>
       <c r="I13" s="66" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="21"/>
       <c r="L13" s="13" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="M13" s="58" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="N13" s="42" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="O13" s="13" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="P13" s="40" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="Q13" s="13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="R13" s="40" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="S13" s="42" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -2875,31 +2875,31 @@
         <v>215</v>
       </c>
       <c r="I14" s="66" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
       <c r="M14" s="58" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="N14" s="30" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="O14" s="58" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="P14" s="40" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="Q14" s="13" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="R14" s="40" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="S14" s="40" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -2929,17 +2929,17 @@
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
       <c r="M15" s="58" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="N15" s="40" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="P15" s="30"/>
       <c r="R15" s="40" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="S15" s="40" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -2969,12 +2969,12 @@
       <c r="K16" s="21"/>
       <c r="L16" s="21"/>
       <c r="M16" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="N16" s="42"/>
       <c r="P16" s="30"/>
       <c r="R16" s="40" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="S16" s="30"/>
     </row>
@@ -2999,7 +2999,7 @@
       <c r="P17" s="42"/>
       <c r="Q17" s="14"/>
       <c r="R17" s="40" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="S17" s="30"/>
     </row>
@@ -3218,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="U23" s="68" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3342,31 +3342,31 @@
       <c r="G27" s="9"/>
       <c r="J27" s="10"/>
       <c r="K27" s="78" t="s">
-        <v>237</v>
+        <v>402</v>
       </c>
       <c r="L27" s="75" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M27" s="44" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="N27" s="73" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="O27" s="44" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="P27" s="73" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="Q27" s="44" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="R27" s="73" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="S27" s="44" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="T27" s="53"/>
     </row>
@@ -3389,31 +3389,31 @@
       <c r="G28" s="9"/>
       <c r="H28" s="5"/>
       <c r="K28" s="69" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="L28" s="77" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="M28" s="40" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="N28" s="14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="O28" s="71" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="P28" s="74" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="Q28" s="42" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="R28" s="14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="S28" s="40" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="T28" s="53"/>
     </row>
@@ -3435,31 +3435,31 @@
       </c>
       <c r="J29" s="10"/>
       <c r="K29" s="69" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L29" s="77" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M29" s="40" t="s">
+        <v>251</v>
+      </c>
+      <c r="N29" s="74" t="s">
         <v>253</v>
       </c>
-      <c r="N29" s="74" t="s">
-        <v>255</v>
-      </c>
       <c r="O29" s="71" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="P29" s="14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="Q29" s="46" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="R29" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="S29" s="40" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="T29" s="53"/>
     </row>
@@ -3481,31 +3481,31 @@
       </c>
       <c r="J30" s="10"/>
       <c r="K30" s="69" t="s">
-        <v>240</v>
+        <v>403</v>
       </c>
       <c r="L30" s="77" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="M30" s="40" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="N30" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="O30" s="40" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="P30" s="14" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="Q30" s="40" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="R30" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="S30" s="40" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="T30" s="53"/>
     </row>
@@ -3527,29 +3527,29 @@
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="69" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="L31" s="15" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="M31" s="40" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="N31" s="15" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="O31" s="42" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="P31" s="15" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="Q31" s="42"/>
       <c r="R31" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="S31" s="42" t="s">
         <v>281</v>
-      </c>
-      <c r="S31" s="42" t="s">
-        <v>283</v>
       </c>
       <c r="T31" s="53"/>
     </row>
@@ -3571,29 +3571,29 @@
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="69" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="L32" s="77" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="M32" s="40" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="N32" s="15" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="O32" s="42" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="P32" s="15" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="Q32" s="42"/>
       <c r="R32" s="14" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="S32" s="42" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="T32" s="53"/>
     </row>
@@ -3605,23 +3605,23 @@
       <c r="E33" s="8"/>
       <c r="J33" s="10"/>
       <c r="K33" s="69" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L33" s="77" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="M33" s="40" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="N33" s="15" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="O33" s="42"/>
       <c r="P33" s="15"/>
       <c r="Q33" s="42"/>
       <c r="R33" s="14"/>
       <c r="S33" s="42" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="T33" s="53" t="s">
         <v>31</v>
@@ -3679,7 +3679,7 @@
         <v>20</v>
       </c>
       <c r="K35" s="30">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="L35" s="30">
         <v>60</v>
@@ -3693,7 +3693,7 @@
       <c r="S35" s="30"/>
       <c r="T35" s="54">
         <f>K35+L35+M35+N35+O35+P35+Q35+R35+S35</f>
-        <v>225</v>
+        <v>235</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3733,7 +3733,7 @@
         <v>255</v>
       </c>
       <c r="U36" s="68" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3758,7 +3758,7 @@
       <c r="R37" s="31"/>
       <c r="T37" s="68">
         <f>T35+T36</f>
-        <v>480</v>
+        <v>490</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -12682,7 +12682,7 @@
     </row>
     <row r="590" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A590" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B590" s="23" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Uren registratie & begin Script Assaultrifle
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$A$1:$E$673</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1240,7 +1240,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2119,8 +2119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2575,7 +2575,7 @@
         <v>231</v>
       </c>
       <c r="J8" s="1"/>
-      <c r="K8" s="57" t="s">
+      <c r="K8" s="79" t="s">
         <v>291</v>
       </c>
       <c r="L8" s="58" t="s">

</xml_diff>

<commit_message>
Uren Registratie & Asset List Update
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -1563,7 +1563,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1800,6 +1800,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2119,8 +2125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2675,7 +2681,7 @@
         <v>227</v>
       </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="58" t="s">
+      <c r="K10" s="83" t="s">
         <v>392</v>
       </c>
       <c r="L10" s="64" t="s">
@@ -3099,7 +3105,9 @@
       <c r="J20" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="K20" s="28"/>
+      <c r="K20" s="28">
+        <v>6</v>
+      </c>
       <c r="L20" s="30"/>
       <c r="M20" s="31"/>
       <c r="N20" s="30"/>
@@ -3110,7 +3118,7 @@
       <c r="S20" s="32"/>
       <c r="T20" s="50">
         <f>K20+L20+M20+N20+O20+P20+Q20+R20+S20</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -3215,7 +3223,7 @@
       <c r="R23" s="31"/>
       <c r="T23" s="67">
         <f>T20+T21+T22</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U23" s="68" t="s">
         <v>369</v>
@@ -3529,7 +3537,7 @@
       <c r="K31" s="69" t="s">
         <v>239</v>
       </c>
-      <c r="L31" s="15" t="s">
+      <c r="L31" s="82" t="s">
         <v>244</v>
       </c>
       <c r="M31" s="40" t="s">

</xml_diff>

<commit_message>
Wat kleine scripts gemaakt en verwijdert enzo
Heb alle scripts behalve HUDManager klaar. en de planning en UML
aangepast
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$A$1:$E$673</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -763,15 +763,9 @@
     <t>Items_AmmoPack (30)</t>
   </si>
   <si>
-    <t>Enemy_AbstractEnemy (30)</t>
-  </si>
-  <si>
     <t>Game_HUDManager (70)</t>
   </si>
   <si>
-    <t>Weapons_AbstractGrenades (30)</t>
-  </si>
-  <si>
     <t>Weapons_FragGrenades (50)</t>
   </si>
   <si>
@@ -1235,12 +1229,18 @@
   </si>
   <si>
     <t>Game_ConversationTrigger (10)</t>
+  </si>
+  <si>
+    <t>Enemy_AbstractEnemy (10)</t>
+  </si>
+  <si>
+    <t>Weapons_AbstractGrenades (10)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1575,7 +1575,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1838,6 +1838,24 @@
     <xf numFmtId="0" fontId="4" fillId="17" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Controlecel" xfId="4" builtinId="23"/>
@@ -1850,9 +1868,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FF99"/>
       <color rgb="FFFF66CC"/>
       <color rgb="FF808080"/>
-      <color rgb="FF00FF99"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2155,8 +2173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N42" sqref="N42"/>
+    <sheetView tabSelected="1" topLeftCell="K2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2327,31 +2345,31 @@
       </c>
       <c r="J3" s="10"/>
       <c r="K3" s="78" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="L3" s="82" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="M3" s="60" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="N3" s="63" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="P3" s="41" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="R3" s="41" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="S3" s="63" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -2384,31 +2402,31 @@
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="77" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="L4" s="77" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M4" s="83" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="N4" s="42" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="O4" s="15" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="P4" s="40" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="R4" s="40" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="S4" s="42" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -2441,31 +2459,31 @@
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="77" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="L5" s="57" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="M5" s="83" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="N5" s="42" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="O5" s="15" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="P5" s="69" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="Q5" s="10" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="R5" s="42" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="S5" s="40" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -2498,31 +2516,31 @@
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="77" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="L6" s="77" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="N6" s="84" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="O6" s="15" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="P6" s="40" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="R6" s="40" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="S6" s="40" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -2555,31 +2573,31 @@
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="77" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="L7" s="57" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="N7" s="84" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="O7" s="57" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="P7" s="42" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="R7" s="40" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="S7" s="40" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -2612,31 +2630,31 @@
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="77" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="L8" s="85" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="M8" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="N8" s="48" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O8" s="57" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="P8" s="40" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="R8" s="40" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="S8" s="88" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -2657,31 +2675,31 @@
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="77" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="L9" s="85" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="N9" s="46" t="s">
+        <v>313</v>
+      </c>
+      <c r="O9" s="57" t="s">
         <v>315</v>
       </c>
-      <c r="O9" s="57" t="s">
-        <v>317</v>
-      </c>
       <c r="P9" s="40" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="Q9" s="10" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="R9" s="40" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="S9" s="40" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -2712,31 +2730,31 @@
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="81" t="s">
+        <v>390</v>
+      </c>
+      <c r="L10" s="87" t="s">
         <v>392</v>
       </c>
-      <c r="L10" s="87" t="s">
-        <v>394</v>
-      </c>
       <c r="M10" s="13" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="N10" s="46" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O10" s="13" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="P10" s="40" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="Q10" s="57" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="R10" s="40" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="S10" s="40" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -2766,28 +2784,28 @@
       <c r="J11" s="1"/>
       <c r="K11" s="21"/>
       <c r="L11" s="13" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="M11" s="86" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="N11" s="42" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="O11" s="13" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="P11" s="40" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="Q11" s="89" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="R11" s="40" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="S11" s="40" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -2811,33 +2829,33 @@
         <v>41</v>
       </c>
       <c r="I12" s="64" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="21"/>
       <c r="L12" s="13" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="M12" s="85" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="N12" s="46" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="O12" s="57" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="P12" s="42" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="Q12" s="13" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="R12" s="40" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="S12" s="42" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -2861,33 +2879,33 @@
         <v>41</v>
       </c>
       <c r="I13" s="64" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="21"/>
       <c r="L13" s="83" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="M13" s="57" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="N13" s="84" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="O13" s="13" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="P13" s="40" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="Q13" s="13" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="R13" s="40" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="S13" s="42" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -2911,31 +2929,31 @@
         <v>215</v>
       </c>
       <c r="I14" s="64" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
       <c r="M14" s="57" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="N14" s="30" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="O14" s="57" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="P14" s="40" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="Q14" s="13" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="R14" s="40" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="S14" s="40" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -2965,17 +2983,17 @@
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
       <c r="M15" s="57" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="N15" s="40" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="P15" s="30"/>
       <c r="R15" s="88" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="S15" s="40" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -3005,12 +3023,12 @@
       <c r="K16" s="21"/>
       <c r="L16" s="21"/>
       <c r="M16" s="13" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="N16" s="42"/>
       <c r="P16" s="30"/>
       <c r="R16" s="88" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="S16" s="30"/>
     </row>
@@ -3035,7 +3053,7 @@
       <c r="P17" s="42"/>
       <c r="Q17" s="14"/>
       <c r="R17" s="88" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="S17" s="30"/>
     </row>
@@ -3256,7 +3274,7 @@
         <v>6</v>
       </c>
       <c r="U23" s="66" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3380,31 +3398,31 @@
       <c r="G27" s="9"/>
       <c r="J27" s="10"/>
       <c r="K27" s="76" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L27" s="73" t="s">
         <v>238</v>
       </c>
-      <c r="M27" s="44" t="s">
+      <c r="M27" s="93" t="s">
         <v>243</v>
       </c>
       <c r="N27" s="73" t="s">
         <v>247</v>
       </c>
       <c r="O27" s="44" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="P27" s="71" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="Q27" s="44" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="R27" s="71" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="S27" s="44" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="T27" s="53"/>
     </row>
@@ -3427,31 +3445,31 @@
       <c r="G28" s="9"/>
       <c r="H28" s="5"/>
       <c r="K28" s="67" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="L28" s="75" t="s">
         <v>240</v>
       </c>
       <c r="M28" s="40" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="N28" s="14" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O28" s="69" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="P28" s="72" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="Q28" s="42" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="R28" s="14" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="S28" s="40" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="T28" s="53"/>
     </row>
@@ -3478,26 +3496,26 @@
       <c r="L29" s="75" t="s">
         <v>241</v>
       </c>
-      <c r="M29" s="40" t="s">
+      <c r="M29" s="95" t="s">
+        <v>249</v>
+      </c>
+      <c r="N29" s="72" t="s">
         <v>251</v>
       </c>
-      <c r="N29" s="72" t="s">
-        <v>253</v>
-      </c>
       <c r="O29" s="69" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="P29" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="Q29" s="46" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="R29" s="14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="S29" s="40" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="T29" s="53"/>
     </row>
@@ -3519,31 +3537,31 @@
       </c>
       <c r="J30" s="10"/>
       <c r="K30" s="67" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="L30" s="75" t="s">
         <v>242</v>
       </c>
-      <c r="M30" s="40" t="s">
-        <v>250</v>
+      <c r="M30" s="95" t="s">
+        <v>405</v>
       </c>
       <c r="N30" s="14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="O30" s="40" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="P30" s="14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="Q30" s="40" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="R30" s="14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="S30" s="40" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="T30" s="53"/>
     </row>
@@ -3570,24 +3588,24 @@
       <c r="L31" s="80" t="s">
         <v>244</v>
       </c>
-      <c r="M31" s="40" t="s">
-        <v>248</v>
+      <c r="M31" s="95" t="s">
+        <v>404</v>
       </c>
       <c r="N31" s="15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O31" s="42" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="P31" s="15" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="Q31" s="42"/>
       <c r="R31" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="S31" s="42" t="s">
         <v>279</v>
-      </c>
-      <c r="S31" s="42" t="s">
-        <v>281</v>
       </c>
       <c r="T31" s="53"/>
     </row>
@@ -3614,24 +3632,24 @@
       <c r="L32" s="75" t="s">
         <v>245</v>
       </c>
-      <c r="M32" s="40" t="s">
-        <v>254</v>
+      <c r="M32" s="94" t="s">
+        <v>252</v>
       </c>
       <c r="N32" s="15" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="O32" s="42" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="P32" s="15" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="Q32" s="42"/>
       <c r="R32" s="14" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="S32" s="42" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="T32" s="53"/>
     </row>
@@ -3643,23 +3661,23 @@
       <c r="E33" s="8"/>
       <c r="J33" s="10"/>
       <c r="K33" s="67" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="L33" s="75" t="s">
-        <v>401</v>
-      </c>
-      <c r="M33" s="40" t="s">
-        <v>401</v>
+        <v>399</v>
+      </c>
+      <c r="M33" s="95" t="s">
+        <v>399</v>
       </c>
       <c r="N33" s="15" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="O33" s="42"/>
       <c r="P33" s="15"/>
       <c r="Q33" s="42"/>
       <c r="R33" s="14"/>
       <c r="S33" s="42" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="T33" s="53" t="s">
         <v>31</v>
@@ -3683,10 +3701,10 @@
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="74" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="L34" s="79" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="M34" s="45"/>
       <c r="N34" s="26"/>
@@ -3761,7 +3779,9 @@
       <c r="L36" s="33">
         <v>145</v>
       </c>
-      <c r="M36" s="33"/>
+      <c r="M36" s="33">
+        <v>85</v>
+      </c>
       <c r="N36" s="33"/>
       <c r="O36" s="33"/>
       <c r="P36" s="33"/>
@@ -3770,10 +3790,10 @@
       <c r="S36" s="33"/>
       <c r="T36" s="59">
         <f>K36+L36+M36+N36+O36+P36+Q36+R36+S36</f>
-        <v>255</v>
+        <v>340</v>
       </c>
       <c r="U36" s="66" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3798,7 +3818,7 @@
       <c r="R37" s="31"/>
       <c r="T37" s="66">
         <f>T35+T36</f>
-        <v>520</v>
+        <v>605</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -12667,19 +12687,19 @@
       <c r="H586" s="4"/>
     </row>
     <row r="587" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A587" s="5" t="s">
+      <c r="A587" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="B587" s="23" t="s">
+      <c r="B587" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C587" s="7" t="s">
+      <c r="C587" s="91" t="s">
         <v>89</v>
       </c>
-      <c r="D587" s="8">
+      <c r="D587" s="92">
         <v>20</v>
       </c>
-      <c r="E587" s="8">
+      <c r="E587" s="92">
         <v>7</v>
       </c>
       <c r="H587" s="4"/>
@@ -12722,7 +12742,7 @@
     </row>
     <row r="590" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A590" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B590" s="23" t="s">
         <v>11</v>
@@ -13365,19 +13385,19 @@
       </c>
     </row>
     <row r="631" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A631" s="5" t="s">
+      <c r="A631" s="90" t="s">
         <v>81</v>
       </c>
-      <c r="B631" s="23" t="s">
+      <c r="B631" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C631" s="7" t="s">
+      <c r="C631" s="91" t="s">
         <v>89</v>
       </c>
-      <c r="D631" s="8">
+      <c r="D631" s="92">
         <v>60</v>
       </c>
-      <c r="E631" s="8">
+      <c r="E631" s="92">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Assetlist Update & Start HUD Manager
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$A$1:$E$673</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -730,9 +730,6 @@
     <t>Development</t>
   </si>
   <si>
-    <t>Weapons_WeaponManager (60)</t>
-  </si>
-  <si>
     <t>Weapons_AbstractWeapons (30)</t>
   </si>
   <si>
@@ -1235,12 +1232,15 @@
   </si>
   <si>
     <t>Weapons_AbstractGrenades (10)</t>
+  </si>
+  <si>
+    <t>Weapons_WeaponManager (70)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1575,7 +1575,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1814,9 +1814,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1851,9 +1848,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2174,7 +2168,7 @@
   <dimension ref="A1:U1028"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2345,31 +2339,31 @@
       </c>
       <c r="J3" s="10"/>
       <c r="K3" s="78" t="s">
-        <v>284</v>
-      </c>
-      <c r="L3" s="82" t="s">
-        <v>292</v>
+        <v>283</v>
+      </c>
+      <c r="L3" s="78" t="s">
+        <v>291</v>
       </c>
       <c r="M3" s="60" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="N3" s="63" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="P3" s="41" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="R3" s="41" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="S3" s="63" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -2402,31 +2396,31 @@
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="77" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L4" s="77" t="s">
-        <v>293</v>
-      </c>
-      <c r="M4" s="83" t="s">
-        <v>297</v>
+        <v>292</v>
+      </c>
+      <c r="M4" s="82" t="s">
+        <v>296</v>
       </c>
       <c r="N4" s="42" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O4" s="15" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="P4" s="40" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="R4" s="40" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="S4" s="42" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -2459,31 +2453,31 @@
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="77" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L5" s="57" t="s">
-        <v>294</v>
-      </c>
-      <c r="M5" s="83" t="s">
-        <v>298</v>
+        <v>293</v>
+      </c>
+      <c r="M5" s="82" t="s">
+        <v>297</v>
       </c>
       <c r="N5" s="42" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="O5" s="15" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="P5" s="69" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q5" s="10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="R5" s="42" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="S5" s="40" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -2516,31 +2510,31 @@
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="77" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L6" s="77" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>299</v>
-      </c>
-      <c r="N6" s="84" t="s">
-        <v>310</v>
+        <v>298</v>
+      </c>
+      <c r="N6" s="83" t="s">
+        <v>309</v>
       </c>
       <c r="O6" s="15" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P6" s="40" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="R6" s="40" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="S6" s="40" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -2573,31 +2567,31 @@
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="77" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L7" s="57" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="N7" s="84" t="s">
-        <v>311</v>
+        <v>299</v>
+      </c>
+      <c r="N7" s="83" t="s">
+        <v>310</v>
       </c>
       <c r="O7" s="57" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="P7" s="42" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="R7" s="40" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="S7" s="40" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -2630,31 +2624,31 @@
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="77" t="s">
-        <v>289</v>
-      </c>
-      <c r="L8" s="85" t="s">
-        <v>389</v>
+        <v>288</v>
+      </c>
+      <c r="L8" s="84" t="s">
+        <v>388</v>
       </c>
       <c r="M8" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="N8" s="48" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="O8" s="57" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="P8" s="40" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="R8" s="40" t="s">
-        <v>365</v>
-      </c>
-      <c r="S8" s="88" t="s">
-        <v>381</v>
+        <v>364</v>
+      </c>
+      <c r="S8" s="87" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -2675,31 +2669,31 @@
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="77" t="s">
-        <v>290</v>
-      </c>
-      <c r="L9" s="85" t="s">
-        <v>391</v>
+        <v>289</v>
+      </c>
+      <c r="L9" s="84" t="s">
+        <v>390</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N9" s="46" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="O9" s="57" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="P9" s="40" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="Q9" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="R9" s="40" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="S9" s="40" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -2730,31 +2724,31 @@
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="81" t="s">
-        <v>390</v>
-      </c>
-      <c r="L10" s="87" t="s">
-        <v>392</v>
+        <v>389</v>
+      </c>
+      <c r="L10" s="86" t="s">
+        <v>391</v>
       </c>
       <c r="M10" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="N10" s="46" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O10" s="13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="P10" s="40" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="Q10" s="57" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="R10" s="40" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="S10" s="40" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -2784,28 +2778,28 @@
       <c r="J11" s="1"/>
       <c r="K11" s="21"/>
       <c r="L11" s="13" t="s">
-        <v>394</v>
-      </c>
-      <c r="M11" s="86" t="s">
-        <v>303</v>
+        <v>393</v>
+      </c>
+      <c r="M11" s="85" t="s">
+        <v>302</v>
       </c>
       <c r="N11" s="42" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O11" s="13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="P11" s="40" t="s">
-        <v>342</v>
-      </c>
-      <c r="Q11" s="89" t="s">
-        <v>358</v>
+        <v>341</v>
+      </c>
+      <c r="Q11" s="88" t="s">
+        <v>357</v>
       </c>
       <c r="R11" s="40" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="S11" s="40" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -2829,33 +2823,33 @@
         <v>41</v>
       </c>
       <c r="I12" s="64" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="21"/>
       <c r="L12" s="13" t="s">
-        <v>395</v>
-      </c>
-      <c r="M12" s="85" t="s">
-        <v>304</v>
+        <v>394</v>
+      </c>
+      <c r="M12" s="84" t="s">
+        <v>303</v>
       </c>
       <c r="N12" s="46" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="O12" s="57" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="P12" s="42" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="Q12" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="R12" s="40" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="S12" s="42" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -2879,33 +2873,33 @@
         <v>41</v>
       </c>
       <c r="I13" s="64" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="21"/>
-      <c r="L13" s="83" t="s">
-        <v>287</v>
+      <c r="L13" s="82" t="s">
+        <v>286</v>
       </c>
       <c r="M13" s="57" t="s">
-        <v>305</v>
-      </c>
-      <c r="N13" s="84" t="s">
-        <v>320</v>
+        <v>304</v>
+      </c>
+      <c r="N13" s="83" t="s">
+        <v>319</v>
       </c>
       <c r="O13" s="13" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P13" s="40" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Q13" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="R13" s="40" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="S13" s="42" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -2929,31 +2923,31 @@
         <v>215</v>
       </c>
       <c r="I14" s="64" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
       <c r="M14" s="57" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="N14" s="30" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="O14" s="57" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="P14" s="40" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Q14" s="13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="R14" s="40" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="S14" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -2983,17 +2977,17 @@
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
       <c r="M15" s="57" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="N15" s="40" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="P15" s="30"/>
-      <c r="R15" s="88" t="s">
-        <v>374</v>
+      <c r="R15" s="87" t="s">
+        <v>373</v>
       </c>
       <c r="S15" s="40" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -3023,12 +3017,12 @@
       <c r="K16" s="21"/>
       <c r="L16" s="21"/>
       <c r="M16" s="13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N16" s="42"/>
       <c r="P16" s="30"/>
-      <c r="R16" s="88" t="s">
-        <v>375</v>
+      <c r="R16" s="87" t="s">
+        <v>374</v>
       </c>
       <c r="S16" s="30"/>
     </row>
@@ -3052,8 +3046,8 @@
       <c r="N17" s="42"/>
       <c r="P17" s="42"/>
       <c r="Q17" s="14"/>
-      <c r="R17" s="88" t="s">
-        <v>376</v>
+      <c r="R17" s="87" t="s">
+        <v>375</v>
       </c>
       <c r="S17" s="30"/>
     </row>
@@ -3274,7 +3268,7 @@
         <v>6</v>
       </c>
       <c r="U23" s="66" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3398,31 +3392,31 @@
       <c r="G27" s="9"/>
       <c r="J27" s="10"/>
       <c r="K27" s="76" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="L27" s="73" t="s">
-        <v>238</v>
-      </c>
-      <c r="M27" s="93" t="s">
-        <v>243</v>
+        <v>237</v>
+      </c>
+      <c r="M27" s="92" t="s">
+        <v>242</v>
       </c>
       <c r="N27" s="73" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O27" s="44" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="P27" s="71" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Q27" s="44" t="s">
+        <v>266</v>
+      </c>
+      <c r="R27" s="71" t="s">
         <v>267</v>
       </c>
-      <c r="R27" s="71" t="s">
-        <v>268</v>
-      </c>
       <c r="S27" s="44" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="T27" s="53"/>
     </row>
@@ -3445,31 +3439,31 @@
       <c r="G28" s="9"/>
       <c r="H28" s="5"/>
       <c r="K28" s="67" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="L28" s="75" t="s">
-        <v>240</v>
-      </c>
-      <c r="M28" s="40" t="s">
-        <v>248</v>
+        <v>239</v>
+      </c>
+      <c r="M28" s="69" t="s">
+        <v>247</v>
       </c>
       <c r="N28" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O28" s="69" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="P28" s="72" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q28" s="42" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="R28" s="14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="S28" s="40" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="T28" s="53"/>
     </row>
@@ -3491,31 +3485,31 @@
       </c>
       <c r="J29" s="10"/>
       <c r="K29" s="67" t="s">
-        <v>237</v>
+        <v>405</v>
       </c>
       <c r="L29" s="75" t="s">
-        <v>241</v>
-      </c>
-      <c r="M29" s="95" t="s">
-        <v>249</v>
+        <v>240</v>
+      </c>
+      <c r="M29" s="67" t="s">
+        <v>248</v>
       </c>
       <c r="N29" s="72" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O29" s="69" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P29" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Q29" s="46" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="R29" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="S29" s="40" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T29" s="53"/>
     </row>
@@ -3537,31 +3531,31 @@
       </c>
       <c r="J30" s="10"/>
       <c r="K30" s="67" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="L30" s="75" t="s">
-        <v>242</v>
-      </c>
-      <c r="M30" s="95" t="s">
-        <v>405</v>
+        <v>241</v>
+      </c>
+      <c r="M30" s="67" t="s">
+        <v>404</v>
       </c>
       <c r="N30" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O30" s="40" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="P30" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Q30" s="40" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="R30" s="14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="S30" s="40" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="T30" s="53"/>
     </row>
@@ -3583,29 +3577,29 @@
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="67" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L31" s="80" t="s">
-        <v>244</v>
-      </c>
-      <c r="M31" s="95" t="s">
-        <v>404</v>
+        <v>243</v>
+      </c>
+      <c r="M31" s="67" t="s">
+        <v>403</v>
       </c>
       <c r="N31" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O31" s="42" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="P31" s="15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Q31" s="42"/>
       <c r="R31" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="S31" s="42" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T31" s="53"/>
     </row>
@@ -3627,29 +3621,29 @@
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="67" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L32" s="75" t="s">
-        <v>245</v>
-      </c>
-      <c r="M32" s="94" t="s">
-        <v>252</v>
+        <v>244</v>
+      </c>
+      <c r="M32" s="93" t="s">
+        <v>251</v>
       </c>
       <c r="N32" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O32" s="42" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="P32" s="15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="Q32" s="42"/>
       <c r="R32" s="14" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="S32" s="42" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="T32" s="53"/>
     </row>
@@ -3661,23 +3655,23 @@
       <c r="E33" s="8"/>
       <c r="J33" s="10"/>
       <c r="K33" s="67" t="s">
+        <v>397</v>
+      </c>
+      <c r="L33" s="75" t="s">
         <v>398</v>
       </c>
-      <c r="L33" s="75" t="s">
-        <v>399</v>
-      </c>
-      <c r="M33" s="95" t="s">
-        <v>399</v>
+      <c r="M33" s="67" t="s">
+        <v>398</v>
       </c>
       <c r="N33" s="15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="O33" s="42"/>
       <c r="P33" s="15"/>
       <c r="Q33" s="42"/>
       <c r="R33" s="14"/>
       <c r="S33" s="42" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="T33" s="53" t="s">
         <v>31</v>
@@ -3701,10 +3695,10 @@
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="74" t="s">
+        <v>401</v>
+      </c>
+      <c r="L34" s="79" t="s">
         <v>402</v>
-      </c>
-      <c r="L34" s="79" t="s">
-        <v>403</v>
       </c>
       <c r="M34" s="45"/>
       <c r="N34" s="26"/>
@@ -3774,13 +3768,13 @@
         <v>21</v>
       </c>
       <c r="K36" s="33">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="L36" s="33">
         <v>145</v>
       </c>
       <c r="M36" s="33">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="N36" s="33"/>
       <c r="O36" s="33"/>
@@ -3790,10 +3784,10 @@
       <c r="S36" s="33"/>
       <c r="T36" s="59">
         <f>K36+L36+M36+N36+O36+P36+Q36+R36+S36</f>
-        <v>340</v>
+        <v>370</v>
       </c>
       <c r="U36" s="66" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3818,7 +3812,7 @@
       <c r="R37" s="31"/>
       <c r="T37" s="66">
         <f>T35+T36</f>
-        <v>605</v>
+        <v>635</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -12687,19 +12681,19 @@
       <c r="H586" s="4"/>
     </row>
     <row r="587" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A587" s="90" t="s">
+      <c r="A587" s="89" t="s">
         <v>53</v>
       </c>
       <c r="B587" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C587" s="91" t="s">
+      <c r="C587" s="90" t="s">
         <v>89</v>
       </c>
-      <c r="D587" s="92">
+      <c r="D587" s="91">
         <v>20</v>
       </c>
-      <c r="E587" s="92">
+      <c r="E587" s="91">
         <v>7</v>
       </c>
       <c r="H587" s="4"/>
@@ -12742,7 +12736,7 @@
     </row>
     <row r="590" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A590" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B590" s="23" t="s">
         <v>11</v>
@@ -13385,19 +13379,19 @@
       </c>
     </row>
     <row r="631" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A631" s="90" t="s">
+      <c r="A631" s="89" t="s">
         <v>81</v>
       </c>
       <c r="B631" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C631" s="91" t="s">
+      <c r="C631" s="90" t="s">
         <v>89</v>
       </c>
-      <c r="D631" s="92">
+      <c r="D631" s="91">
         <v>60</v>
       </c>
-      <c r="E631" s="92">
+      <c r="E631" s="91">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Uren Registratie 12-04-2016 & Asset List Update & Menu
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -2167,7 +2167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
@@ -3444,7 +3444,7 @@
       <c r="L28" s="75" t="s">
         <v>239</v>
       </c>
-      <c r="M28" s="69" t="s">
+      <c r="M28" s="67" t="s">
         <v>247</v>
       </c>
       <c r="N28" s="14" t="s">
@@ -3734,7 +3734,9 @@
       <c r="L35" s="30">
         <v>60</v>
       </c>
-      <c r="M35" s="30"/>
+      <c r="M35" s="30">
+        <v>70</v>
+      </c>
       <c r="N35" s="30">
         <v>30</v>
       </c>
@@ -3745,7 +3747,7 @@
       <c r="S35" s="30"/>
       <c r="T35" s="54">
         <f>K35+L35+M35+N35+O35+P35+Q35+R35+S35</f>
-        <v>265</v>
+        <v>335</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3812,7 +3814,7 @@
       <c r="R37" s="31"/>
       <c r="T37" s="66">
         <f>T35+T36</f>
-        <v>635</v>
+        <v>705</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UML & Asset list update
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -1216,9 +1216,6 @@
     <t>Game_GameManager (15)</t>
   </si>
   <si>
-    <t>Player_Movement (80)</t>
-  </si>
-  <si>
     <t>Player_CameraControl (20)</t>
   </si>
   <si>
@@ -1235,6 +1232,9 @@
   </si>
   <si>
     <t>Weapons_WeaponManager (70)</t>
+  </si>
+  <si>
+    <t>Player_Movement (100)</t>
   </si>
 </sst>
 </file>
@@ -2167,8 +2167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3392,7 +3392,7 @@
       <c r="G27" s="9"/>
       <c r="J27" s="10"/>
       <c r="K27" s="76" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="L27" s="73" t="s">
         <v>237</v>
@@ -3447,7 +3447,7 @@
       <c r="M28" s="67" t="s">
         <v>247</v>
       </c>
-      <c r="N28" s="14" t="s">
+      <c r="N28" s="75" t="s">
         <v>249</v>
       </c>
       <c r="O28" s="69" t="s">
@@ -3485,7 +3485,7 @@
       </c>
       <c r="J29" s="10"/>
       <c r="K29" s="67" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L29" s="75" t="s">
         <v>240</v>
@@ -3493,7 +3493,7 @@
       <c r="M29" s="67" t="s">
         <v>248</v>
       </c>
-      <c r="N29" s="72" t="s">
+      <c r="N29" s="75" t="s">
         <v>250</v>
       </c>
       <c r="O29" s="69" t="s">
@@ -3531,13 +3531,13 @@
       </c>
       <c r="J30" s="10"/>
       <c r="K30" s="67" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="L30" s="75" t="s">
         <v>241</v>
       </c>
       <c r="M30" s="67" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="N30" s="14" t="s">
         <v>252</v>
@@ -3583,7 +3583,7 @@
         <v>243</v>
       </c>
       <c r="M31" s="67" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="N31" s="15" t="s">
         <v>253</v>
@@ -3629,7 +3629,7 @@
       <c r="M32" s="93" t="s">
         <v>251</v>
       </c>
-      <c r="N32" s="15" t="s">
+      <c r="N32" s="75" t="s">
         <v>254</v>
       </c>
       <c r="O32" s="42" t="s">
@@ -3663,7 +3663,7 @@
       <c r="M33" s="67" t="s">
         <v>398</v>
       </c>
-      <c r="N33" s="15" t="s">
+      <c r="N33" s="80" t="s">
         <v>260</v>
       </c>
       <c r="O33" s="42"/>
@@ -3695,10 +3695,10 @@
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="74" t="s">
+        <v>400</v>
+      </c>
+      <c r="L34" s="79" t="s">
         <v>401</v>
-      </c>
-      <c r="L34" s="79" t="s">
-        <v>402</v>
       </c>
       <c r="M34" s="45"/>
       <c r="N34" s="26"/>
@@ -3729,7 +3729,7 @@
         <v>20</v>
       </c>
       <c r="K35" s="30">
-        <v>175</v>
+        <v>205</v>
       </c>
       <c r="L35" s="30">
         <v>60</v>
@@ -3747,7 +3747,7 @@
       <c r="S35" s="30"/>
       <c r="T35" s="54">
         <f>K35+L35+M35+N35+O35+P35+Q35+R35+S35</f>
-        <v>335</v>
+        <v>365</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3770,7 +3770,7 @@
         <v>21</v>
       </c>
       <c r="K36" s="33">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="L36" s="33">
         <v>145</v>
@@ -3778,7 +3778,9 @@
       <c r="M36" s="33">
         <v>105</v>
       </c>
-      <c r="N36" s="33"/>
+      <c r="N36" s="33">
+        <v>60</v>
+      </c>
       <c r="O36" s="33"/>
       <c r="P36" s="33"/>
       <c r="Q36" s="33"/>
@@ -3786,7 +3788,7 @@
       <c r="S36" s="33"/>
       <c r="T36" s="59">
         <f>K36+L36+M36+N36+O36+P36+Q36+R36+S36</f>
-        <v>370</v>
+        <v>420</v>
       </c>
       <c r="U36" s="66" t="s">
         <v>367</v>
@@ -3814,7 +3816,7 @@
       <c r="R37" s="31"/>
       <c r="T37" s="66">
         <f>T35+T36</f>
-        <v>705</v>
+        <v>785</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Stun en FragGRenades 90% af
de laatste 10 procent zijn de enemies, maar die kan ik beter doen als er
enemies zijn gescript, dus voor nu laat ik het maar zo. Heeft fancy ass
particles gekregen denkzij onze nieuwe ExplosionPool script. Ook heeft
het luxe UI elementen zoals TWEE placeholder icons voor zowel onze frag
-en stungrenades plus een handige counter die het volume bijhoudt. OH en
de stun grenade kan je niet stunnen als je er nie naar kijkt. Wat wil je
nog meer?
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$A$1:$E$673</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$A$1:$E$674</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1844" uniqueCount="408">
   <si>
     <t>ID Code</t>
   </si>
@@ -688,9 +688,6 @@
     <t>| WeaponManager | AbstractWeapons | MeleeWeapon | Shotgun | Pistol | HarpoonGun | FlareGun |</t>
   </si>
   <si>
-    <t xml:space="preserve">| AssaultRifle | AbstractGrenades | FragGrenades | StunGrenades | SmokeGrenades | AbstractMines </t>
-  </si>
-  <si>
     <t xml:space="preserve">| ToolBox | Welder | Grinder | Hammer | SconicScrewDriver |  Generator | FusionCore | TelePorter | Computer | AssemblyLine | </t>
   </si>
   <si>
@@ -1235,12 +1232,21 @@
   </si>
   <si>
     <t>Player_Movement (100)</t>
+  </si>
+  <si>
+    <t>Weapons_ExplosionPool</t>
+  </si>
+  <si>
+    <t>| AssaultRifle | AbstractGrenades | FragGrenades | StunGrenades | SmokeGrenades | AbstractMines | ExplosionPool</t>
+  </si>
+  <si>
+    <t>Weapons_ExplosionPool (40)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2165,10 +2171,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U1028"/>
+  <dimension ref="A1:U1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N40" sqref="N40"/>
+    <sheetView tabSelected="1" topLeftCell="J4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2219,7 +2225,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>30</v>
@@ -2278,7 +2284,7 @@
         <v>22</v>
       </c>
       <c r="I2" s="64" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="47" t="s">
@@ -2335,35 +2341,35 @@
         <v>23</v>
       </c>
       <c r="I3" s="64" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J3" s="10"/>
       <c r="K3" s="78" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L3" s="78" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="M3" s="60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="N3" s="63" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="P3" s="41" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="R3" s="41" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="S3" s="63" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -2392,35 +2398,35 @@
         <v>24</v>
       </c>
       <c r="I4" s="64" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="77" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L4" s="77" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M4" s="82" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="N4" s="42" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="O4" s="15" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="P4" s="40" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="R4" s="40" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="S4" s="42" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -2449,35 +2455,35 @@
         <v>25</v>
       </c>
       <c r="I5" s="64" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="77" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L5" s="57" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M5" s="82" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N5" s="42" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O5" s="15" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="P5" s="69" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q5" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="R5" s="42" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="S5" s="40" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -2506,35 +2512,35 @@
         <v>25</v>
       </c>
       <c r="I6" s="64" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="77" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L6" s="77" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="N6" s="83" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="O6" s="15" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="P6" s="40" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="R6" s="40" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="S6" s="40" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -2563,35 +2569,35 @@
         <v>25</v>
       </c>
       <c r="I7" s="64" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="77" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L7" s="57" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="N7" s="83" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O7" s="57" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="P7" s="42" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="R7" s="40" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="S7" s="40" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -2620,35 +2626,35 @@
         <v>26</v>
       </c>
       <c r="I8" s="64" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="77" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L8" s="84" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="M8" s="13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="N8" s="48" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="O8" s="57" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="P8" s="40" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="R8" s="40" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="S8" s="87" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -2665,35 +2671,35 @@
         <v>27</v>
       </c>
       <c r="I9" s="64" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="77" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L9" s="84" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="N9" s="46" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="O9" s="57" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="P9" s="40" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="Q9" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="R9" s="40" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="S9" s="40" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -2720,35 +2726,35 @@
         <v>27</v>
       </c>
       <c r="I10" s="64" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="81" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L10" s="86" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="M10" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N10" s="46" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="O10" s="13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P10" s="40" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="Q10" s="57" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="R10" s="40" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="S10" s="40" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -2773,33 +2779,33 @@
         <v>41</v>
       </c>
       <c r="I11" s="64" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="21"/>
       <c r="L11" s="13" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M11" s="85" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="N11" s="42" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O11" s="13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="P11" s="40" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Q11" s="88" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="R11" s="40" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="S11" s="40" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -2823,33 +2829,33 @@
         <v>41</v>
       </c>
       <c r="I12" s="64" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="21"/>
       <c r="L12" s="13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="M12" s="84" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N12" s="46" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O12" s="57" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="P12" s="42" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="Q12" s="13" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="R12" s="40" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="S12" s="42" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -2873,33 +2879,33 @@
         <v>41</v>
       </c>
       <c r="I13" s="64" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="21"/>
       <c r="L13" s="82" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M13" s="57" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="N13" s="83" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="O13" s="13" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="P13" s="40" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q13" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="R13" s="40" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="S13" s="42" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -2923,31 +2929,31 @@
         <v>215</v>
       </c>
       <c r="I14" s="64" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
       <c r="M14" s="57" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="N14" s="30" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="O14" s="57" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P14" s="40" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Q14" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="R14" s="40" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S14" s="40" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -2977,17 +2983,17 @@
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
       <c r="M15" s="57" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N15" s="40" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="P15" s="30"/>
       <c r="R15" s="87" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="S15" s="40" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -3017,12 +3023,12 @@
       <c r="K16" s="21"/>
       <c r="L16" s="21"/>
       <c r="M16" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="N16" s="42"/>
       <c r="P16" s="30"/>
       <c r="R16" s="87" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="S16" s="30"/>
     </row>
@@ -3047,7 +3053,7 @@
       <c r="P17" s="42"/>
       <c r="Q17" s="14"/>
       <c r="R17" s="87" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="S17" s="30"/>
     </row>
@@ -3184,7 +3190,7 @@
         <v>221</v>
       </c>
       <c r="I21" s="64" t="s">
-        <v>223</v>
+        <v>406</v>
       </c>
       <c r="J21" s="51" t="s">
         <v>17</v>
@@ -3268,7 +3274,7 @@
         <v>6</v>
       </c>
       <c r="U23" s="66" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3345,31 +3351,31 @@
       <c r="G26" s="9"/>
       <c r="J26" s="10"/>
       <c r="K26" s="47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L26" s="47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M26" s="47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N26" s="47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O26" s="47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="P26" s="47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Q26" s="47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="R26" s="47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="S26" s="47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="T26" s="53"/>
     </row>
@@ -3392,31 +3398,31 @@
       <c r="G27" s="9"/>
       <c r="J27" s="10"/>
       <c r="K27" s="76" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L27" s="73" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M27" s="92" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N27" s="73" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O27" s="44" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="P27" s="71" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q27" s="44" t="s">
+        <v>265</v>
+      </c>
+      <c r="R27" s="71" t="s">
         <v>266</v>
       </c>
-      <c r="R27" s="71" t="s">
-        <v>267</v>
-      </c>
       <c r="S27" s="44" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="T27" s="53"/>
     </row>
@@ -3439,31 +3445,31 @@
       <c r="G28" s="9"/>
       <c r="H28" s="5"/>
       <c r="K28" s="67" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="L28" s="75" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M28" s="67" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N28" s="75" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="O28" s="69" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="P28" s="72" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q28" s="42" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="R28" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="S28" s="40" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="T28" s="53"/>
     </row>
@@ -3485,31 +3491,31 @@
       </c>
       <c r="J29" s="10"/>
       <c r="K29" s="67" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="L29" s="75" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M29" s="67" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N29" s="75" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O29" s="69" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="P29" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q29" s="46" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="R29" s="14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="S29" s="40" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T29" s="53"/>
     </row>
@@ -3531,31 +3537,31 @@
       </c>
       <c r="J30" s="10"/>
       <c r="K30" s="67" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="L30" s="75" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M30" s="67" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="N30" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O30" s="40" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P30" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Q30" s="40" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="R30" s="14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="S30" s="40" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="T30" s="53"/>
     </row>
@@ -3577,29 +3583,29 @@
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="67" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L31" s="80" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M31" s="67" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="N31" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O31" s="42" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="P31" s="15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Q31" s="42"/>
       <c r="R31" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="S31" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="T31" s="53"/>
     </row>
@@ -3621,29 +3627,29 @@
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="67" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L32" s="75" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M32" s="93" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N32" s="75" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O32" s="42" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="P32" s="15" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="Q32" s="42"/>
       <c r="R32" s="14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="S32" s="42" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T32" s="53"/>
     </row>
@@ -3655,23 +3661,23 @@
       <c r="E33" s="8"/>
       <c r="J33" s="10"/>
       <c r="K33" s="67" t="s">
+        <v>396</v>
+      </c>
+      <c r="L33" s="75" t="s">
         <v>397</v>
       </c>
-      <c r="L33" s="75" t="s">
-        <v>398</v>
-      </c>
       <c r="M33" s="67" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="N33" s="80" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="O33" s="42"/>
       <c r="P33" s="15"/>
       <c r="Q33" s="42"/>
       <c r="R33" s="14"/>
       <c r="S33" s="42" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="T33" s="53" t="s">
         <v>31</v>
@@ -3695,13 +3701,15 @@
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="74" t="s">
+        <v>399</v>
+      </c>
+      <c r="L34" s="79" t="s">
         <v>400</v>
       </c>
-      <c r="L34" s="79" t="s">
-        <v>401</v>
-      </c>
       <c r="M34" s="45"/>
-      <c r="N34" s="26"/>
+      <c r="N34" s="26" t="s">
+        <v>407</v>
+      </c>
       <c r="O34" s="43"/>
       <c r="P34" s="26"/>
       <c r="Q34" s="43"/>
@@ -3779,7 +3787,7 @@
         <v>105</v>
       </c>
       <c r="N36" s="33">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="O36" s="33"/>
       <c r="P36" s="33"/>
@@ -3788,10 +3796,10 @@
       <c r="S36" s="33"/>
       <c r="T36" s="59">
         <f>K36+L36+M36+N36+O36+P36+Q36+R36+S36</f>
-        <v>420</v>
+        <v>450</v>
       </c>
       <c r="U36" s="66" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3816,7 +3824,7 @@
       <c r="R37" s="31"/>
       <c r="T37" s="66">
         <f>T35+T36</f>
-        <v>785</v>
+        <v>815</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -11419,7 +11427,7 @@
     </row>
     <row r="497" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A497" s="24" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B497" s="6" t="s">
         <v>5</v>
@@ -11437,7 +11445,7 @@
     </row>
     <row r="498" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A498" s="24" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B498" s="16" t="s">
         <v>10</v>
@@ -12740,7 +12748,7 @@
     </row>
     <row r="590" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A590" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B590" s="23" t="s">
         <v>11</v>
@@ -13502,17 +13510,30 @@
       </c>
     </row>
     <row r="638" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A638" s="4"/>
-      <c r="B638" s="4"/>
-      <c r="C638" s="7"/>
+      <c r="A638" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="B638" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C638" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="D638" s="8">
-        <f>SUM(D581:D637)</f>
-        <v>2350</v>
+        <v>40</v>
+      </c>
+      <c r="E638" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="639" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A639" s="5"/>
-      <c r="B639" s="24"/>
+      <c r="A639" s="4"/>
+      <c r="B639" s="4"/>
+      <c r="C639" s="7"/>
+      <c r="D639" s="8">
+        <f>SUM(D581:D638)</f>
+        <v>2390</v>
+      </c>
     </row>
     <row r="640" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A640" s="5"/>
@@ -13527,11 +13548,11 @@
       <c r="B642" s="24"/>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A643" s="24"/>
+      <c r="A643" s="5"/>
       <c r="B643" s="24"/>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A644" s="5"/>
+      <c r="A644" s="24"/>
       <c r="B644" s="24"/>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.25">
@@ -13563,11 +13584,11 @@
       <c r="B651" s="24"/>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A652" s="24"/>
+      <c r="A652" s="5"/>
       <c r="B652" s="24"/>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A653" s="5"/>
+      <c r="A653" s="24"/>
       <c r="B653" s="24"/>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.25">
@@ -13583,11 +13604,11 @@
       <c r="B656" s="24"/>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A657" s="24"/>
+      <c r="A657" s="5"/>
       <c r="B657" s="24"/>
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A658" s="5"/>
+      <c r="A658" s="24"/>
       <c r="B658" s="24"/>
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.25">
@@ -13603,11 +13624,11 @@
       <c r="B661" s="24"/>
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A662" s="24"/>
+      <c r="A662" s="5"/>
       <c r="B662" s="24"/>
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A663" s="5"/>
+      <c r="A663" s="24"/>
       <c r="B663" s="24"/>
     </row>
     <row r="664" spans="1:2" x14ac:dyDescent="0.25">
@@ -13623,11 +13644,11 @@
       <c r="B666" s="24"/>
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A667" s="24"/>
+      <c r="A667" s="5"/>
       <c r="B667" s="24"/>
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A668" s="5"/>
+      <c r="A668" s="24"/>
       <c r="B668" s="24"/>
     </row>
     <row r="669" spans="1:2" x14ac:dyDescent="0.25">
@@ -13643,11 +13664,11 @@
       <c r="B671" s="24"/>
     </row>
     <row r="672" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A672" s="24"/>
+      <c r="A672" s="5"/>
       <c r="B672" s="24"/>
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A673" s="5"/>
+      <c r="A673" s="24"/>
       <c r="B673" s="24"/>
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.25">
@@ -13663,11 +13684,11 @@
       <c r="B676" s="24"/>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A677" s="24"/>
+      <c r="A677" s="5"/>
       <c r="B677" s="24"/>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A678" s="5"/>
+      <c r="A678" s="24"/>
       <c r="B678" s="24"/>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.25">
@@ -13683,11 +13704,11 @@
       <c r="B681" s="24"/>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A682" s="24"/>
+      <c r="A682" s="5"/>
       <c r="B682" s="24"/>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A683" s="5"/>
+      <c r="A683" s="24"/>
       <c r="B683" s="24"/>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.25">
@@ -13703,11 +13724,11 @@
       <c r="B686" s="24"/>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A687" s="24"/>
+      <c r="A687" s="5"/>
       <c r="B687" s="24"/>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A688" s="5"/>
+      <c r="A688" s="24"/>
       <c r="B688" s="24"/>
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.25">
@@ -13723,11 +13744,11 @@
       <c r="B691" s="24"/>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A692" s="24"/>
+      <c r="A692" s="5"/>
       <c r="B692" s="24"/>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A693" s="5"/>
+      <c r="A693" s="24"/>
       <c r="B693" s="24"/>
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.25">
@@ -13747,11 +13768,11 @@
       <c r="B697" s="24"/>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A698" s="24"/>
+      <c r="A698" s="5"/>
       <c r="B698" s="24"/>
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A699" s="5"/>
+      <c r="A699" s="24"/>
       <c r="B699" s="24"/>
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.25">
@@ -13767,11 +13788,11 @@
       <c r="B702" s="24"/>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A703" s="24"/>
+      <c r="A703" s="5"/>
       <c r="B703" s="24"/>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A704" s="5"/>
+      <c r="A704" s="24"/>
       <c r="B704" s="24"/>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.25">
@@ -13787,11 +13808,11 @@
       <c r="B707" s="24"/>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A708" s="24"/>
+      <c r="A708" s="5"/>
       <c r="B708" s="24"/>
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A709" s="5"/>
+      <c r="A709" s="24"/>
       <c r="B709" s="24"/>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.25">
@@ -13807,11 +13828,11 @@
       <c r="B712" s="24"/>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A713" s="24"/>
+      <c r="A713" s="5"/>
       <c r="B713" s="24"/>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A714" s="5"/>
+      <c r="A714" s="24"/>
       <c r="B714" s="24"/>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.25">
@@ -13827,11 +13848,11 @@
       <c r="B717" s="24"/>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A718" s="24"/>
+      <c r="A718" s="5"/>
       <c r="B718" s="24"/>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A719" s="5"/>
+      <c r="A719" s="24"/>
       <c r="B719" s="24"/>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.25">
@@ -13847,11 +13868,11 @@
       <c r="B722" s="24"/>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A723" s="24"/>
+      <c r="A723" s="5"/>
       <c r="B723" s="24"/>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A724" s="5"/>
+      <c r="A724" s="24"/>
       <c r="B724" s="24"/>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.25">
@@ -13867,12 +13888,12 @@
       <c r="B727" s="24"/>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A728" s="8"/>
-      <c r="B728" s="8"/>
+      <c r="A728" s="5"/>
+      <c r="B728" s="24"/>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A729" s="5"/>
-      <c r="B729" s="24"/>
+      <c r="A729" s="8"/>
+      <c r="B729" s="8"/>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A730" s="5"/>
@@ -13903,11 +13924,11 @@
       <c r="B736" s="24"/>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A737" s="24"/>
+      <c r="A737" s="5"/>
       <c r="B737" s="24"/>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A738" s="5"/>
+      <c r="A738" s="24"/>
       <c r="B738" s="24"/>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.25">
@@ -13939,11 +13960,11 @@
       <c r="B745" s="24"/>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A746" s="24"/>
+      <c r="A746" s="5"/>
       <c r="B746" s="24"/>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A747" s="5"/>
+      <c r="A747" s="24"/>
       <c r="B747" s="24"/>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.25">
@@ -13975,11 +13996,11 @@
       <c r="B754" s="24"/>
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A755" s="24"/>
+      <c r="A755" s="5"/>
       <c r="B755" s="24"/>
     </row>
     <row r="756" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A756" s="5"/>
+      <c r="A756" s="24"/>
       <c r="B756" s="24"/>
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.25">
@@ -14011,11 +14032,11 @@
       <c r="B763" s="24"/>
     </row>
     <row r="764" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A764" s="24"/>
+      <c r="A764" s="5"/>
       <c r="B764" s="24"/>
     </row>
     <row r="765" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A765" s="5"/>
+      <c r="A765" s="24"/>
       <c r="B765" s="24"/>
     </row>
     <row r="766" spans="1:2" x14ac:dyDescent="0.25">
@@ -14047,11 +14068,11 @@
       <c r="B772" s="24"/>
     </row>
     <row r="773" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A773" s="24"/>
+      <c r="A773" s="5"/>
       <c r="B773" s="24"/>
     </row>
     <row r="774" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A774" s="5"/>
+      <c r="A774" s="24"/>
       <c r="B774" s="24"/>
     </row>
     <row r="775" spans="1:2" x14ac:dyDescent="0.25">
@@ -14067,11 +14088,11 @@
       <c r="B777" s="24"/>
     </row>
     <row r="778" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A778" s="24"/>
+      <c r="A778" s="5"/>
       <c r="B778" s="24"/>
     </row>
     <row r="779" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A779" s="5"/>
+      <c r="A779" s="24"/>
       <c r="B779" s="24"/>
     </row>
     <row r="780" spans="1:2" x14ac:dyDescent="0.25">
@@ -14087,11 +14108,11 @@
       <c r="B782" s="24"/>
     </row>
     <row r="783" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A783" s="24"/>
+      <c r="A783" s="5"/>
       <c r="B783" s="24"/>
     </row>
     <row r="784" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A784" s="5"/>
+      <c r="A784" s="24"/>
       <c r="B784" s="24"/>
     </row>
     <row r="785" spans="1:2" x14ac:dyDescent="0.25">
@@ -14107,11 +14128,11 @@
       <c r="B787" s="24"/>
     </row>
     <row r="788" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A788" s="24"/>
+      <c r="A788" s="5"/>
       <c r="B788" s="24"/>
     </row>
     <row r="789" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A789" s="5"/>
+      <c r="A789" s="24"/>
       <c r="B789" s="24"/>
     </row>
     <row r="790" spans="1:2" x14ac:dyDescent="0.25">
@@ -14127,11 +14148,11 @@
       <c r="B792" s="24"/>
     </row>
     <row r="793" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A793" s="24"/>
+      <c r="A793" s="5"/>
       <c r="B793" s="24"/>
     </row>
     <row r="794" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A794" s="5"/>
+      <c r="A794" s="24"/>
       <c r="B794" s="24"/>
     </row>
     <row r="795" spans="1:2" x14ac:dyDescent="0.25">
@@ -14147,11 +14168,11 @@
       <c r="B797" s="24"/>
     </row>
     <row r="798" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A798" s="24"/>
+      <c r="A798" s="5"/>
       <c r="B798" s="24"/>
     </row>
     <row r="799" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A799" s="5"/>
+      <c r="A799" s="24"/>
       <c r="B799" s="24"/>
     </row>
     <row r="800" spans="1:2" x14ac:dyDescent="0.25">
@@ -14167,11 +14188,11 @@
       <c r="B802" s="24"/>
     </row>
     <row r="803" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A803" s="24"/>
+      <c r="A803" s="5"/>
       <c r="B803" s="24"/>
     </row>
     <row r="804" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A804" s="5"/>
+      <c r="A804" s="24"/>
       <c r="B804" s="24"/>
     </row>
     <row r="805" spans="1:2" x14ac:dyDescent="0.25">
@@ -14187,11 +14208,11 @@
       <c r="B807" s="24"/>
     </row>
     <row r="808" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A808" s="24"/>
+      <c r="A808" s="5"/>
       <c r="B808" s="24"/>
     </row>
     <row r="809" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A809" s="5"/>
+      <c r="A809" s="24"/>
       <c r="B809" s="24"/>
     </row>
     <row r="810" spans="1:2" x14ac:dyDescent="0.25">
@@ -14207,11 +14228,11 @@
       <c r="B812" s="24"/>
     </row>
     <row r="813" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A813" s="24"/>
+      <c r="A813" s="5"/>
       <c r="B813" s="24"/>
     </row>
     <row r="814" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A814" s="5"/>
+      <c r="A814" s="24"/>
       <c r="B814" s="24"/>
     </row>
     <row r="815" spans="1:2" x14ac:dyDescent="0.25">
@@ -14227,11 +14248,11 @@
       <c r="B817" s="24"/>
     </row>
     <row r="818" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A818" s="24"/>
+      <c r="A818" s="5"/>
       <c r="B818" s="24"/>
     </row>
     <row r="819" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A819" s="5"/>
+      <c r="A819" s="24"/>
       <c r="B819" s="24"/>
     </row>
     <row r="820" spans="1:2" x14ac:dyDescent="0.25">
@@ -14251,11 +14272,11 @@
       <c r="B823" s="24"/>
     </row>
     <row r="824" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A824" s="24"/>
+      <c r="A824" s="5"/>
       <c r="B824" s="24"/>
     </row>
     <row r="825" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A825" s="5"/>
+      <c r="A825" s="24"/>
       <c r="B825" s="24"/>
     </row>
     <row r="826" spans="1:2" x14ac:dyDescent="0.25">
@@ -14271,11 +14292,11 @@
       <c r="B828" s="24"/>
     </row>
     <row r="829" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A829" s="24"/>
+      <c r="A829" s="5"/>
       <c r="B829" s="24"/>
     </row>
     <row r="830" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A830" s="5"/>
+      <c r="A830" s="24"/>
       <c r="B830" s="24"/>
     </row>
     <row r="831" spans="1:2" x14ac:dyDescent="0.25">
@@ -14295,11 +14316,11 @@
       <c r="B834" s="24"/>
     </row>
     <row r="835" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A835" s="24"/>
+      <c r="A835" s="5"/>
       <c r="B835" s="24"/>
     </row>
     <row r="836" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A836" s="5"/>
+      <c r="A836" s="24"/>
       <c r="B836" s="24"/>
     </row>
     <row r="837" spans="1:2" x14ac:dyDescent="0.25">
@@ -14319,12 +14340,12 @@
       <c r="B840" s="24"/>
     </row>
     <row r="841" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A841" s="8"/>
-      <c r="B841" s="8"/>
+      <c r="A841" s="5"/>
+      <c r="B841" s="24"/>
     </row>
     <row r="842" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A842" s="5"/>
-      <c r="B842" s="24"/>
+      <c r="A842" s="8"/>
+      <c r="B842" s="8"/>
     </row>
     <row r="843" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A843" s="5"/>
@@ -14339,11 +14360,11 @@
       <c r="B845" s="24"/>
     </row>
     <row r="846" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A846" s="24"/>
+      <c r="A846" s="5"/>
       <c r="B846" s="24"/>
     </row>
     <row r="847" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A847" s="5"/>
+      <c r="A847" s="24"/>
       <c r="B847" s="24"/>
     </row>
     <row r="848" spans="1:2" x14ac:dyDescent="0.25">
@@ -14359,11 +14380,11 @@
       <c r="B850" s="24"/>
     </row>
     <row r="851" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A851" s="24"/>
+      <c r="A851" s="5"/>
       <c r="B851" s="24"/>
     </row>
     <row r="852" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A852" s="5"/>
+      <c r="A852" s="24"/>
       <c r="B852" s="24"/>
     </row>
     <row r="853" spans="1:2" x14ac:dyDescent="0.25">
@@ -14379,11 +14400,11 @@
       <c r="B855" s="24"/>
     </row>
     <row r="856" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A856" s="24"/>
+      <c r="A856" s="5"/>
       <c r="B856" s="24"/>
     </row>
     <row r="857" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A857" s="5"/>
+      <c r="A857" s="24"/>
       <c r="B857" s="24"/>
     </row>
     <row r="858" spans="1:2" x14ac:dyDescent="0.25">
@@ -14399,11 +14420,11 @@
       <c r="B860" s="24"/>
     </row>
     <row r="861" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A861" s="24"/>
+      <c r="A861" s="5"/>
       <c r="B861" s="24"/>
     </row>
     <row r="862" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A862" s="5"/>
+      <c r="A862" s="24"/>
       <c r="B862" s="24"/>
     </row>
     <row r="863" spans="1:2" x14ac:dyDescent="0.25">
@@ -14419,11 +14440,11 @@
       <c r="B865" s="24"/>
     </row>
     <row r="866" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A866" s="24"/>
+      <c r="A866" s="5"/>
       <c r="B866" s="24"/>
     </row>
     <row r="867" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A867" s="5"/>
+      <c r="A867" s="24"/>
       <c r="B867" s="24"/>
     </row>
     <row r="868" spans="1:2" x14ac:dyDescent="0.25">
@@ -14431,11 +14452,11 @@
       <c r="B868" s="24"/>
     </row>
     <row r="869" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A869" s="24"/>
+      <c r="A869" s="5"/>
       <c r="B869" s="24"/>
     </row>
     <row r="870" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A870" s="5"/>
+      <c r="A870" s="24"/>
       <c r="B870" s="24"/>
     </row>
     <row r="871" spans="1:2" x14ac:dyDescent="0.25">
@@ -14443,11 +14464,11 @@
       <c r="B871" s="24"/>
     </row>
     <row r="872" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A872" s="24"/>
+      <c r="A872" s="5"/>
       <c r="B872" s="24"/>
     </row>
     <row r="873" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A873" s="5"/>
+      <c r="A873" s="24"/>
       <c r="B873" s="24"/>
     </row>
     <row r="874" spans="1:2" x14ac:dyDescent="0.25">
@@ -14455,11 +14476,11 @@
       <c r="B874" s="24"/>
     </row>
     <row r="875" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A875" s="24"/>
+      <c r="A875" s="5"/>
       <c r="B875" s="24"/>
     </row>
     <row r="876" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A876" s="5"/>
+      <c r="A876" s="24"/>
       <c r="B876" s="24"/>
     </row>
     <row r="877" spans="1:2" x14ac:dyDescent="0.25">
@@ -14467,11 +14488,11 @@
       <c r="B877" s="24"/>
     </row>
     <row r="878" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A878" s="24"/>
+      <c r="A878" s="5"/>
       <c r="B878" s="24"/>
     </row>
     <row r="879" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A879" s="5"/>
+      <c r="A879" s="24"/>
       <c r="B879" s="24"/>
     </row>
     <row r="880" spans="1:2" x14ac:dyDescent="0.25">
@@ -14479,11 +14500,11 @@
       <c r="B880" s="24"/>
     </row>
     <row r="881" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A881" s="24"/>
+      <c r="A881" s="5"/>
       <c r="B881" s="24"/>
     </row>
     <row r="882" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A882" s="5"/>
+      <c r="A882" s="24"/>
       <c r="B882" s="24"/>
     </row>
     <row r="883" spans="1:2" x14ac:dyDescent="0.25">
@@ -14491,11 +14512,11 @@
       <c r="B883" s="24"/>
     </row>
     <row r="884" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A884" s="24"/>
+      <c r="A884" s="5"/>
       <c r="B884" s="24"/>
     </row>
     <row r="885" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A885" s="5"/>
+      <c r="A885" s="24"/>
       <c r="B885" s="24"/>
     </row>
     <row r="886" spans="1:2" x14ac:dyDescent="0.25">
@@ -14503,11 +14524,11 @@
       <c r="B886" s="24"/>
     </row>
     <row r="887" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A887" s="24"/>
+      <c r="A887" s="5"/>
       <c r="B887" s="24"/>
     </row>
     <row r="888" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A888" s="5"/>
+      <c r="A888" s="24"/>
       <c r="B888" s="24"/>
     </row>
     <row r="889" spans="1:2" x14ac:dyDescent="0.25">
@@ -14515,11 +14536,11 @@
       <c r="B889" s="24"/>
     </row>
     <row r="890" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A890" s="24"/>
+      <c r="A890" s="5"/>
       <c r="B890" s="24"/>
     </row>
     <row r="891" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A891" s="5"/>
+      <c r="A891" s="24"/>
       <c r="B891" s="24"/>
     </row>
     <row r="892" spans="1:2" x14ac:dyDescent="0.25">
@@ -14527,11 +14548,11 @@
       <c r="B892" s="24"/>
     </row>
     <row r="893" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A893" s="24"/>
+      <c r="A893" s="5"/>
       <c r="B893" s="24"/>
     </row>
     <row r="894" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A894" s="5"/>
+      <c r="A894" s="24"/>
       <c r="B894" s="24"/>
     </row>
     <row r="895" spans="1:2" x14ac:dyDescent="0.25">
@@ -14539,11 +14560,11 @@
       <c r="B895" s="24"/>
     </row>
     <row r="896" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A896" s="24"/>
+      <c r="A896" s="5"/>
       <c r="B896" s="24"/>
     </row>
     <row r="897" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A897" s="5"/>
+      <c r="A897" s="24"/>
       <c r="B897" s="24"/>
     </row>
     <row r="898" spans="1:2" x14ac:dyDescent="0.25">
@@ -14551,11 +14572,11 @@
       <c r="B898" s="24"/>
     </row>
     <row r="899" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A899" s="24"/>
+      <c r="A899" s="5"/>
       <c r="B899" s="24"/>
     </row>
     <row r="900" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A900" s="5"/>
+      <c r="A900" s="24"/>
       <c r="B900" s="24"/>
     </row>
     <row r="901" spans="1:2" x14ac:dyDescent="0.25">
@@ -14563,11 +14584,11 @@
       <c r="B901" s="24"/>
     </row>
     <row r="902" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A902" s="24"/>
+      <c r="A902" s="5"/>
       <c r="B902" s="24"/>
     </row>
     <row r="903" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A903" s="5"/>
+      <c r="A903" s="24"/>
       <c r="B903" s="24"/>
     </row>
     <row r="904" spans="1:2" x14ac:dyDescent="0.25">
@@ -14575,11 +14596,11 @@
       <c r="B904" s="24"/>
     </row>
     <row r="905" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A905" s="24"/>
+      <c r="A905" s="5"/>
       <c r="B905" s="24"/>
     </row>
     <row r="906" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A906" s="5"/>
+      <c r="A906" s="24"/>
       <c r="B906" s="24"/>
     </row>
     <row r="907" spans="1:2" x14ac:dyDescent="0.25">
@@ -14587,35 +14608,35 @@
       <c r="B907" s="24"/>
     </row>
     <row r="908" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A908" s="24"/>
+      <c r="A908" s="5"/>
       <c r="B908" s="24"/>
     </row>
     <row r="909" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A909" s="5"/>
+      <c r="A909" s="24"/>
       <c r="B909" s="24"/>
     </row>
     <row r="910" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A910" s="24"/>
+      <c r="A910" s="5"/>
       <c r="B910" s="24"/>
     </row>
     <row r="911" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A911" s="5"/>
+      <c r="A911" s="24"/>
       <c r="B911" s="24"/>
     </row>
     <row r="912" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A912" s="24"/>
+      <c r="A912" s="5"/>
       <c r="B912" s="24"/>
     </row>
     <row r="913" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A913" s="5"/>
+      <c r="A913" s="24"/>
       <c r="B913" s="24"/>
     </row>
     <row r="914" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A914" s="24"/>
+      <c r="A914" s="5"/>
       <c r="B914" s="24"/>
     </row>
     <row r="915" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A915" s="5"/>
+      <c r="A915" s="24"/>
       <c r="B915" s="24"/>
     </row>
     <row r="916" spans="1:2" x14ac:dyDescent="0.25">
@@ -14623,11 +14644,11 @@
       <c r="B916" s="24"/>
     </row>
     <row r="917" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A917" s="24"/>
+      <c r="A917" s="5"/>
       <c r="B917" s="24"/>
     </row>
     <row r="918" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A918" s="5"/>
+      <c r="A918" s="24"/>
       <c r="B918" s="24"/>
     </row>
     <row r="919" spans="1:2" x14ac:dyDescent="0.25">
@@ -14663,11 +14684,11 @@
       <c r="B926" s="24"/>
     </row>
     <row r="927" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A927" s="24"/>
+      <c r="A927" s="5"/>
       <c r="B927" s="24"/>
     </row>
     <row r="928" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A928" s="5"/>
+      <c r="A928" s="24"/>
       <c r="B928" s="24"/>
     </row>
     <row r="929" spans="1:2" x14ac:dyDescent="0.25">
@@ -14691,12 +14712,12 @@
       <c r="B933" s="24"/>
     </row>
     <row r="934" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A934" s="8"/>
-      <c r="B934" s="8"/>
+      <c r="A934" s="5"/>
+      <c r="B934" s="24"/>
     </row>
     <row r="935" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A935" s="5"/>
-      <c r="B935" s="24"/>
+      <c r="A935" s="8"/>
+      <c r="B935" s="8"/>
     </row>
     <row r="936" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A936" s="5"/>
@@ -14731,11 +14752,11 @@
       <c r="B943" s="24"/>
     </row>
     <row r="944" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A944" s="24"/>
+      <c r="A944" s="5"/>
       <c r="B944" s="24"/>
     </row>
     <row r="945" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A945" s="5"/>
+      <c r="A945" s="24"/>
       <c r="B945" s="24"/>
     </row>
     <row r="946" spans="1:2" x14ac:dyDescent="0.25">
@@ -14771,11 +14792,11 @@
       <c r="B953" s="24"/>
     </row>
     <row r="954" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A954" s="24"/>
+      <c r="A954" s="5"/>
       <c r="B954" s="24"/>
     </row>
     <row r="955" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A955" s="5"/>
+      <c r="A955" s="24"/>
       <c r="B955" s="24"/>
     </row>
     <row r="956" spans="1:2" x14ac:dyDescent="0.25">
@@ -14831,11 +14852,11 @@
       <c r="B968" s="24"/>
     </row>
     <row r="969" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A969" s="24"/>
+      <c r="A969" s="5"/>
       <c r="B969" s="24"/>
     </row>
     <row r="970" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A970" s="5"/>
+      <c r="A970" s="24"/>
       <c r="B970" s="24"/>
     </row>
     <row r="971" spans="1:2" x14ac:dyDescent="0.25">
@@ -14859,14 +14880,18 @@
       <c r="B975" s="24"/>
     </row>
     <row r="976" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A976" s="24"/>
+      <c r="A976" s="5"/>
       <c r="B976" s="24"/>
     </row>
-    <row r="1028" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1028" s="5"/>
+    <row r="977" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A977" s="24"/>
+      <c r="B977" s="24"/>
+    </row>
+    <row r="1029" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1029" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E673"/>
+  <autoFilter ref="A1:E674"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
UML update uren registratie en effect ammo
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$A$1:$E$674</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1246,7 +1246,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2174,7 +2174,7 @@
   <dimension ref="A1:U1029"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N37" sqref="N37"/>
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3669,7 +3669,7 @@
       <c r="M33" s="67" t="s">
         <v>397</v>
       </c>
-      <c r="N33" s="80" t="s">
+      <c r="N33" s="75" t="s">
         <v>259</v>
       </c>
       <c r="O33" s="42"/>
@@ -3707,7 +3707,7 @@
         <v>400</v>
       </c>
       <c r="M34" s="45"/>
-      <c r="N34" s="26" t="s">
+      <c r="N34" s="79" t="s">
         <v>407</v>
       </c>
       <c r="O34" s="43"/>
@@ -3787,7 +3787,7 @@
         <v>105</v>
       </c>
       <c r="N36" s="33">
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="O36" s="33"/>
       <c r="P36" s="33"/>
@@ -3796,7 +3796,7 @@
       <c r="S36" s="33"/>
       <c r="T36" s="59">
         <f>K36+L36+M36+N36+O36+P36+Q36+R36+S36</f>
-        <v>450</v>
+        <v>530</v>
       </c>
       <c r="U36" s="66" t="s">
         <v>366</v>
@@ -3824,7 +3824,7 @@
       <c r="R37" s="31"/>
       <c r="T37" s="66">
         <f>T35+T36</f>
-        <v>815</v>
+        <v>895</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Uren registratie sprints toegevoegd & Asset list Update & Flechette shooting
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -1581,7 +1581,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1812,9 +1812,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2174,7 +2171,7 @@
   <dimension ref="A1:U1029"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2407,7 +2404,7 @@
       <c r="L4" s="77" t="s">
         <v>291</v>
       </c>
-      <c r="M4" s="82" t="s">
+      <c r="M4" s="81" t="s">
         <v>295</v>
       </c>
       <c r="N4" s="42" t="s">
@@ -2464,7 +2461,7 @@
       <c r="L5" s="57" t="s">
         <v>292</v>
       </c>
-      <c r="M5" s="82" t="s">
+      <c r="M5" s="81" t="s">
         <v>296</v>
       </c>
       <c r="N5" s="42" t="s">
@@ -2524,7 +2521,7 @@
       <c r="M6" s="13" t="s">
         <v>297</v>
       </c>
-      <c r="N6" s="83" t="s">
+      <c r="N6" s="82" t="s">
         <v>308</v>
       </c>
       <c r="O6" s="15" t="s">
@@ -2581,7 +2578,7 @@
       <c r="M7" s="13" t="s">
         <v>298</v>
       </c>
-      <c r="N7" s="83" t="s">
+      <c r="N7" s="82" t="s">
         <v>309</v>
       </c>
       <c r="O7" s="57" t="s">
@@ -2632,7 +2629,7 @@
       <c r="K8" s="77" t="s">
         <v>287</v>
       </c>
-      <c r="L8" s="84" t="s">
+      <c r="L8" s="83" t="s">
         <v>387</v>
       </c>
       <c r="M8" s="13" t="s">
@@ -2653,7 +2650,7 @@
       <c r="R8" s="40" t="s">
         <v>363</v>
       </c>
-      <c r="S8" s="87" t="s">
+      <c r="S8" s="86" t="s">
         <v>379</v>
       </c>
     </row>
@@ -2677,7 +2674,7 @@
       <c r="K9" s="77" t="s">
         <v>288</v>
       </c>
-      <c r="L9" s="84" t="s">
+      <c r="L9" s="83" t="s">
         <v>389</v>
       </c>
       <c r="M9" s="13" t="s">
@@ -2729,10 +2726,10 @@
         <v>226</v>
       </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="81" t="s">
+      <c r="K10" s="80" t="s">
         <v>388</v>
       </c>
-      <c r="L10" s="86" t="s">
+      <c r="L10" s="85" t="s">
         <v>390</v>
       </c>
       <c r="M10" s="13" t="s">
@@ -2786,7 +2783,7 @@
       <c r="L11" s="13" t="s">
         <v>392</v>
       </c>
-      <c r="M11" s="85" t="s">
+      <c r="M11" s="84" t="s">
         <v>301</v>
       </c>
       <c r="N11" s="42" t="s">
@@ -2798,7 +2795,7 @@
       <c r="P11" s="40" t="s">
         <v>340</v>
       </c>
-      <c r="Q11" s="88" t="s">
+      <c r="Q11" s="87" t="s">
         <v>356</v>
       </c>
       <c r="R11" s="40" t="s">
@@ -2836,7 +2833,7 @@
       <c r="L12" s="13" t="s">
         <v>393</v>
       </c>
-      <c r="M12" s="84" t="s">
+      <c r="M12" s="83" t="s">
         <v>302</v>
       </c>
       <c r="N12" s="46" t="s">
@@ -2883,13 +2880,13 @@
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="21"/>
-      <c r="L13" s="82" t="s">
+      <c r="L13" s="81" t="s">
         <v>285</v>
       </c>
       <c r="M13" s="57" t="s">
         <v>303</v>
       </c>
-      <c r="N13" s="83" t="s">
+      <c r="N13" s="82" t="s">
         <v>318</v>
       </c>
       <c r="O13" s="13" t="s">
@@ -2989,7 +2986,7 @@
         <v>317</v>
       </c>
       <c r="P15" s="30"/>
-      <c r="R15" s="87" t="s">
+      <c r="R15" s="86" t="s">
         <v>372</v>
       </c>
       <c r="S15" s="40" t="s">
@@ -3027,7 +3024,7 @@
       </c>
       <c r="N16" s="42"/>
       <c r="P16" s="30"/>
-      <c r="R16" s="87" t="s">
+      <c r="R16" s="86" t="s">
         <v>373</v>
       </c>
       <c r="S16" s="30"/>
@@ -3052,7 +3049,7 @@
       <c r="N17" s="42"/>
       <c r="P17" s="42"/>
       <c r="Q17" s="14"/>
-      <c r="R17" s="87" t="s">
+      <c r="R17" s="86" t="s">
         <v>374</v>
       </c>
       <c r="S17" s="30"/>
@@ -3403,7 +3400,7 @@
       <c r="L27" s="73" t="s">
         <v>236</v>
       </c>
-      <c r="M27" s="92" t="s">
+      <c r="M27" s="91" t="s">
         <v>241</v>
       </c>
       <c r="N27" s="73" t="s">
@@ -3585,7 +3582,7 @@
       <c r="K31" s="67" t="s">
         <v>237</v>
       </c>
-      <c r="L31" s="80" t="s">
+      <c r="L31" s="75" t="s">
         <v>242</v>
       </c>
       <c r="M31" s="67" t="s">
@@ -3632,7 +3629,7 @@
       <c r="L32" s="75" t="s">
         <v>243</v>
       </c>
-      <c r="M32" s="93" t="s">
+      <c r="M32" s="92" t="s">
         <v>250</v>
       </c>
       <c r="N32" s="75" t="s">
@@ -3740,7 +3737,7 @@
         <v>205</v>
       </c>
       <c r="L35" s="30">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="M35" s="30">
         <v>70</v>
@@ -3755,7 +3752,7 @@
       <c r="S35" s="30"/>
       <c r="T35" s="54">
         <f>K35+L35+M35+N35+O35+P35+Q35+R35+S35</f>
-        <v>365</v>
+        <v>445</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3824,7 +3821,7 @@
       <c r="R37" s="31"/>
       <c r="T37" s="66">
         <f>T35+T36</f>
-        <v>895</v>
+        <v>975</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -12693,19 +12690,19 @@
       <c r="H586" s="4"/>
     </row>
     <row r="587" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A587" s="89" t="s">
+      <c r="A587" s="88" t="s">
         <v>53</v>
       </c>
       <c r="B587" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C587" s="90" t="s">
+      <c r="C587" s="89" t="s">
         <v>89</v>
       </c>
-      <c r="D587" s="91">
+      <c r="D587" s="90">
         <v>20</v>
       </c>
-      <c r="E587" s="91">
+      <c r="E587" s="90">
         <v>7</v>
       </c>
       <c r="H587" s="4"/>
@@ -13391,19 +13388,19 @@
       </c>
     </row>
     <row r="631" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A631" s="89" t="s">
+      <c r="A631" s="88" t="s">
         <v>81</v>
       </c>
       <c r="B631" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C631" s="90" t="s">
+      <c r="C631" s="89" t="s">
         <v>89</v>
       </c>
-      <c r="D631" s="91">
+      <c r="D631" s="90">
         <v>60</v>
       </c>
-      <c r="E631" s="91">
+      <c r="E631" s="90">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AIEnemy Abstract af, Asset list en uren registratie
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -2171,7 +2171,7 @@
   <dimension ref="A1:U1029"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3588,7 +3588,7 @@
       <c r="M31" s="67" t="s">
         <v>401</v>
       </c>
-      <c r="N31" s="15" t="s">
+      <c r="N31" s="75" t="s">
         <v>252</v>
       </c>
       <c r="O31" s="42" t="s">
@@ -3743,7 +3743,7 @@
         <v>70</v>
       </c>
       <c r="N35" s="30">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="O35" s="30"/>
       <c r="P35" s="30"/>
@@ -3752,7 +3752,7 @@
       <c r="S35" s="30"/>
       <c r="T35" s="54">
         <f>K35+L35+M35+N35+O35+P35+Q35+R35+S35</f>
-        <v>445</v>
+        <v>465</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3821,7 +3821,7 @@
       <c r="R37" s="31"/>
       <c r="T37" s="66">
         <f>T35+T36</f>
-        <v>975</v>
+        <v>995</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Asset list update & Loot manager done voor nu
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -2171,7 +2171,7 @@
   <dimension ref="A1:U1029"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3542,7 +3542,7 @@
       <c r="M30" s="67" t="s">
         <v>402</v>
       </c>
-      <c r="N30" s="14" t="s">
+      <c r="N30" s="75" t="s">
         <v>251</v>
       </c>
       <c r="O30" s="40" t="s">
@@ -3743,7 +3743,7 @@
         <v>70</v>
       </c>
       <c r="N35" s="30">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="O35" s="30"/>
       <c r="P35" s="30"/>
@@ -3752,7 +3752,7 @@
       <c r="S35" s="30"/>
       <c r="T35" s="54">
         <f>K35+L35+M35+N35+O35+P35+Q35+R35+S35</f>
-        <v>465</v>
+        <v>545</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3821,7 +3821,7 @@
       <c r="R37" s="31"/>
       <c r="T37" s="66">
         <f>T35+T36</f>
-        <v>995</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UML & Asset List & Uren Registratie & LOOT
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1844" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="409">
   <si>
     <t>ID Code</t>
   </si>
@@ -1241,6 +1241,9 @@
   </si>
   <si>
     <t>Weapons_ExplosionPool (40)</t>
+  </si>
+  <si>
+    <t>Items_LootPackage (30)</t>
   </si>
 </sst>
 </file>
@@ -2171,7 +2174,7 @@
   <dimension ref="A1:U1029"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N40" sqref="N40"/>
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3703,7 +3706,9 @@
       <c r="L34" s="79" t="s">
         <v>400</v>
       </c>
-      <c r="M34" s="45"/>
+      <c r="M34" s="74" t="s">
+        <v>408</v>
+      </c>
       <c r="N34" s="79" t="s">
         <v>407</v>
       </c>
@@ -3740,7 +3745,7 @@
         <v>140</v>
       </c>
       <c r="M35" s="30">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="N35" s="30">
         <v>130</v>
@@ -3752,7 +3757,7 @@
       <c r="S35" s="30"/>
       <c r="T35" s="54">
         <f>K35+L35+M35+N35+O35+P35+Q35+R35+S35</f>
-        <v>545</v>
+        <v>575</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3821,7 +3826,7 @@
       <c r="R37" s="31"/>
       <c r="T37" s="66">
         <f>T35+T36</f>
-        <v>1075</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Uren Registratie & AssetList Update
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -1308,7 +1308,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1393,18 +1393,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1584,7 +1572,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1721,9 +1709,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1755,9 +1740,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1808,37 +1790,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1854,6 +1809,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2173,8 +2134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2230,31 +2191,31 @@
       <c r="I1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="49" t="s">
+      <c r="L1" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="49" t="s">
+      <c r="M1" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="49" t="s">
+      <c r="N1" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="49" t="s">
+      <c r="O1" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="49" t="s">
+      <c r="P1" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="49" t="s">
+      <c r="Q1" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="49" t="s">
+      <c r="R1" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="S1" s="49" t="s">
+      <c r="S1" s="48" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2280,23 +2241,23 @@
       <c r="G2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="64" t="s">
+      <c r="H2" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="62" t="s">
         <v>227</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="62" t="s">
+      <c r="L2" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="62" t="s">
+      <c r="M2" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="62" t="s">
+      <c r="N2" s="60" t="s">
         <v>16</v>
       </c>
       <c r="O2" s="47" t="s">
@@ -2308,10 +2269,10 @@
       <c r="Q2" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="62" t="s">
+      <c r="R2" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="62" t="s">
+      <c r="S2" s="60" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2337,26 +2298,26 @@
       <c r="G3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="64" t="s">
+      <c r="H3" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="64" t="s">
+      <c r="I3" s="62" t="s">
         <v>228</v>
       </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="78" t="s">
+      <c r="K3" s="83" t="s">
         <v>282</v>
       </c>
-      <c r="L3" s="78" t="s">
+      <c r="L3" s="83" t="s">
         <v>290</v>
       </c>
-      <c r="M3" s="60" t="s">
+      <c r="M3" s="83" t="s">
         <v>391</v>
       </c>
-      <c r="N3" s="63" t="s">
+      <c r="N3" s="61" t="s">
         <v>304</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="7" t="s">
         <v>321</v>
       </c>
       <c r="P3" s="41" t="s">
@@ -2368,7 +2329,7 @@
       <c r="R3" s="41" t="s">
         <v>334</v>
       </c>
-      <c r="S3" s="63" t="s">
+      <c r="S3" s="61" t="s">
         <v>371</v>
       </c>
     </row>
@@ -2394,26 +2355,26 @@
       <c r="G4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="64" t="s">
+      <c r="H4" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="64" t="s">
+      <c r="I4" s="62" t="s">
         <v>229</v>
       </c>
       <c r="J4" s="10"/>
-      <c r="K4" s="77" t="s">
+      <c r="K4" s="76" t="s">
         <v>283</v>
       </c>
-      <c r="L4" s="77" t="s">
+      <c r="L4" s="76" t="s">
         <v>291</v>
       </c>
-      <c r="M4" s="81" t="s">
+      <c r="M4" s="76" t="s">
         <v>295</v>
       </c>
       <c r="N4" s="42" t="s">
         <v>305</v>
       </c>
-      <c r="O4" s="15" t="s">
+      <c r="O4" s="73" t="s">
         <v>322</v>
       </c>
       <c r="P4" s="40" t="s">
@@ -2451,20 +2412,20 @@
       <c r="G5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="64" t="s">
+      <c r="H5" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="64" t="s">
+      <c r="I5" s="62" t="s">
         <v>233</v>
       </c>
       <c r="J5" s="10"/>
-      <c r="K5" s="77" t="s">
+      <c r="K5" s="76" t="s">
         <v>284</v>
       </c>
-      <c r="L5" s="57" t="s">
+      <c r="L5" s="56" t="s">
         <v>292</v>
       </c>
-      <c r="M5" s="81" t="s">
+      <c r="M5" s="13" t="s">
         <v>296</v>
       </c>
       <c r="N5" s="42" t="s">
@@ -2473,7 +2434,7 @@
       <c r="O5" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="P5" s="69" t="s">
+      <c r="P5" s="65" t="s">
         <v>331</v>
       </c>
       <c r="Q5" s="10" t="s">
@@ -2508,23 +2469,23 @@
       <c r="G6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="64" t="s">
+      <c r="H6" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="64" t="s">
+      <c r="I6" s="62" t="s">
         <v>223</v>
       </c>
       <c r="J6" s="1"/>
-      <c r="K6" s="77" t="s">
+      <c r="K6" s="82" t="s">
         <v>289</v>
       </c>
-      <c r="L6" s="77" t="s">
+      <c r="L6" s="76" t="s">
         <v>293</v>
       </c>
       <c r="M6" s="13" t="s">
         <v>297</v>
       </c>
-      <c r="N6" s="82" t="s">
+      <c r="N6" s="42" t="s">
         <v>308</v>
       </c>
       <c r="O6" s="15" t="s">
@@ -2565,26 +2526,26 @@
       <c r="G7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="64" t="s">
+      <c r="H7" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="64" t="s">
+      <c r="I7" s="62" t="s">
         <v>224</v>
       </c>
       <c r="J7" s="1"/>
-      <c r="K7" s="77" t="s">
+      <c r="K7" s="76" t="s">
         <v>286</v>
       </c>
-      <c r="L7" s="57" t="s">
+      <c r="L7" s="56" t="s">
         <v>294</v>
       </c>
       <c r="M7" s="13" t="s">
         <v>298</v>
       </c>
-      <c r="N7" s="82" t="s">
+      <c r="N7" s="42" t="s">
         <v>309</v>
       </c>
-      <c r="O7" s="57" t="s">
+      <c r="O7" s="56" t="s">
         <v>315</v>
       </c>
       <c r="P7" s="42" t="s">
@@ -2622,26 +2583,26 @@
       <c r="G8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="64" t="s">
+      <c r="H8" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="64" t="s">
+      <c r="I8" s="62" t="s">
         <v>230</v>
       </c>
       <c r="J8" s="1"/>
-      <c r="K8" s="77" t="s">
+      <c r="K8" s="76" t="s">
         <v>287</v>
       </c>
-      <c r="L8" s="83" t="s">
+      <c r="L8" s="76" t="s">
         <v>387</v>
       </c>
       <c r="M8" s="13" t="s">
         <v>354</v>
       </c>
-      <c r="N8" s="48" t="s">
+      <c r="N8" s="65" t="s">
         <v>310</v>
       </c>
-      <c r="O8" s="57" t="s">
+      <c r="O8" s="56" t="s">
         <v>316</v>
       </c>
       <c r="P8" s="40" t="s">
@@ -2653,7 +2614,7 @@
       <c r="R8" s="40" t="s">
         <v>363</v>
       </c>
-      <c r="S8" s="86" t="s">
+      <c r="S8" s="65" t="s">
         <v>379</v>
       </c>
     </row>
@@ -2667,17 +2628,17 @@
       <c r="G9" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="H9" s="64" t="s">
+      <c r="H9" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="64" t="s">
+      <c r="I9" s="62" t="s">
         <v>225</v>
       </c>
       <c r="J9" s="1"/>
-      <c r="K9" s="77" t="s">
+      <c r="K9" s="76" t="s">
         <v>288</v>
       </c>
-      <c r="L9" s="83" t="s">
+      <c r="L9" s="76" t="s">
         <v>389</v>
       </c>
       <c r="M9" s="13" t="s">
@@ -2686,7 +2647,7 @@
       <c r="N9" s="46" t="s">
         <v>311</v>
       </c>
-      <c r="O9" s="57" t="s">
+      <c r="O9" s="56" t="s">
         <v>313</v>
       </c>
       <c r="P9" s="40" t="s">
@@ -2722,17 +2683,17 @@
         <v>12</v>
       </c>
       <c r="G10" s="9"/>
-      <c r="H10" s="64" t="s">
+      <c r="H10" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="64" t="s">
+      <c r="I10" s="62" t="s">
         <v>226</v>
       </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="80" t="s">
+      <c r="K10" s="76" t="s">
         <v>388</v>
       </c>
-      <c r="L10" s="85" t="s">
+      <c r="L10" s="76" t="s">
         <v>390</v>
       </c>
       <c r="M10" s="13" t="s">
@@ -2747,7 +2708,7 @@
       <c r="P10" s="40" t="s">
         <v>351</v>
       </c>
-      <c r="Q10" s="57" t="s">
+      <c r="Q10" s="56" t="s">
         <v>355</v>
       </c>
       <c r="R10" s="40" t="s">
@@ -2775,18 +2736,18 @@
       </c>
       <c r="F11" s="24"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="64" t="s">
+      <c r="H11" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="64" t="s">
+      <c r="I11" s="62" t="s">
         <v>231</v>
       </c>
       <c r="J11" s="1"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="13" t="s">
+      <c r="K11" s="56"/>
+      <c r="L11" s="76" t="s">
         <v>392</v>
       </c>
-      <c r="M11" s="84" t="s">
+      <c r="M11" s="82" t="s">
         <v>301</v>
       </c>
       <c r="N11" s="42" t="s">
@@ -2798,7 +2759,7 @@
       <c r="P11" s="40" t="s">
         <v>340</v>
       </c>
-      <c r="Q11" s="87" t="s">
+      <c r="Q11" s="13" t="s">
         <v>356</v>
       </c>
       <c r="R11" s="40" t="s">
@@ -2825,24 +2786,24 @@
         <v>10</v>
       </c>
       <c r="G12" s="9"/>
-      <c r="H12" s="64" t="s">
+      <c r="H12" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="64" t="s">
+      <c r="I12" s="62" t="s">
         <v>280</v>
       </c>
       <c r="J12" s="1"/>
-      <c r="K12" s="21"/>
+      <c r="K12" s="56"/>
       <c r="L12" s="13" t="s">
         <v>393</v>
       </c>
-      <c r="M12" s="83" t="s">
+      <c r="M12" s="76" t="s">
         <v>302</v>
       </c>
       <c r="N12" s="46" t="s">
         <v>319</v>
       </c>
-      <c r="O12" s="57" t="s">
+      <c r="O12" s="56" t="s">
         <v>327</v>
       </c>
       <c r="P12" s="42" t="s">
@@ -2851,7 +2812,7 @@
       <c r="Q12" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="R12" s="40" t="s">
+      <c r="R12" s="65" t="s">
         <v>337</v>
       </c>
       <c r="S12" s="42" t="s">
@@ -2875,27 +2836,27 @@
         <v>10</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="64" t="s">
+      <c r="H13" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="I13" s="64" t="s">
+      <c r="I13" s="62" t="s">
         <v>281</v>
       </c>
       <c r="J13" s="1"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="81" t="s">
+      <c r="K13" s="56"/>
+      <c r="L13" s="76" t="s">
         <v>285</v>
       </c>
-      <c r="M13" s="57" t="s">
+      <c r="M13" s="76" t="s">
         <v>303</v>
       </c>
-      <c r="N13" s="82" t="s">
+      <c r="N13" s="42" t="s">
         <v>318</v>
       </c>
       <c r="O13" s="13" t="s">
         <v>328</v>
       </c>
-      <c r="P13" s="40" t="s">
+      <c r="P13" s="65" t="s">
         <v>336</v>
       </c>
       <c r="Q13" s="13" t="s">
@@ -2925,25 +2886,25 @@
         <v>10</v>
       </c>
       <c r="G14" s="9"/>
-      <c r="H14" s="64" t="s">
+      <c r="H14" s="62" t="s">
         <v>215</v>
       </c>
-      <c r="I14" s="64" t="s">
+      <c r="I14" s="62" t="s">
         <v>395</v>
       </c>
       <c r="J14" s="1"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="57" t="s">
+      <c r="K14" s="56"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="56" t="s">
         <v>307</v>
       </c>
-      <c r="N14" s="30" t="s">
+      <c r="N14" s="42" t="s">
         <v>320</v>
       </c>
-      <c r="O14" s="57" t="s">
+      <c r="O14" s="56" t="s">
         <v>339</v>
       </c>
-      <c r="P14" s="40" t="s">
+      <c r="P14" s="65" t="s">
         <v>338</v>
       </c>
       <c r="Q14" s="13" t="s">
@@ -2973,23 +2934,25 @@
         <v>10</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="64" t="s">
+      <c r="H15" s="62" t="s">
         <v>216</v>
       </c>
-      <c r="I15" s="64" t="s">
+      <c r="I15" s="62" t="s">
         <v>207</v>
       </c>
       <c r="J15" s="1"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="57" t="s">
+      <c r="K15" s="56"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="76" t="s">
         <v>353</v>
       </c>
       <c r="N15" s="40" t="s">
         <v>317</v>
       </c>
-      <c r="P15" s="30"/>
-      <c r="R15" s="86" t="s">
+      <c r="O15" s="7"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="65" t="s">
         <v>372</v>
       </c>
       <c r="S15" s="40" t="s">
@@ -3013,21 +2976,23 @@
         <v>10</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="64" t="s">
+      <c r="H16" s="62" t="s">
         <v>217</v>
       </c>
-      <c r="I16" s="64" t="s">
+      <c r="I16" s="62" t="s">
         <v>211</v>
       </c>
       <c r="J16" s="1"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="56"/>
       <c r="M16" s="13" t="s">
         <v>352</v>
       </c>
       <c r="N16" s="42"/>
-      <c r="P16" s="30"/>
-      <c r="R16" s="86" t="s">
+      <c r="O16" s="7"/>
+      <c r="P16" s="42"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="65" t="s">
         <v>373</v>
       </c>
       <c r="S16" s="30"/>
@@ -3039,20 +3004,21 @@
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="64" t="s">
+      <c r="H17" s="62" t="s">
         <v>218</v>
       </c>
-      <c r="I17" s="64" t="s">
+      <c r="I17" s="62" t="s">
         <v>212</v>
       </c>
       <c r="J17" s="1"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="56"/>
       <c r="M17" s="13"/>
       <c r="N17" s="42"/>
+      <c r="O17" s="7"/>
       <c r="P17" s="42"/>
       <c r="Q17" s="14"/>
-      <c r="R17" s="86" t="s">
+      <c r="R17" s="65" t="s">
         <v>374</v>
       </c>
       <c r="S17" s="30"/>
@@ -3074,20 +3040,21 @@
         <v>10</v>
       </c>
       <c r="G18" s="9"/>
-      <c r="H18" s="64" t="s">
+      <c r="H18" s="62" t="s">
         <v>219</v>
       </c>
-      <c r="I18" s="64" t="s">
+      <c r="I18" s="62" t="s">
         <v>213</v>
       </c>
       <c r="J18" s="1"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="57"/>
+      <c r="K18" s="56"/>
+      <c r="L18" s="56"/>
       <c r="M18" s="13"/>
       <c r="N18" s="42"/>
+      <c r="O18" s="7"/>
       <c r="P18" s="42"/>
       <c r="Q18" s="14"/>
-      <c r="R18" s="30"/>
+      <c r="R18" s="42"/>
       <c r="S18" s="30"/>
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3107,23 +3074,23 @@
         <v>10</v>
       </c>
       <c r="G19" s="9"/>
-      <c r="H19" s="64" t="s">
+      <c r="H19" s="62" t="s">
         <v>220</v>
       </c>
-      <c r="I19" s="64" t="s">
+      <c r="I19" s="62" t="s">
         <v>214</v>
       </c>
       <c r="J19" s="10"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="58"/>
-      <c r="M19" s="61"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="59"/>
       <c r="N19" s="43"/>
       <c r="O19" s="26"/>
       <c r="P19" s="43"/>
       <c r="Q19" s="14"/>
       <c r="R19" s="45"/>
       <c r="S19" s="33"/>
-      <c r="T19" s="53" t="s">
+      <c r="T19" s="52" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3144,13 +3111,13 @@
         <v>10</v>
       </c>
       <c r="G20" s="9"/>
-      <c r="H20" s="64" t="s">
+      <c r="H20" s="62" t="s">
         <v>221</v>
       </c>
-      <c r="I20" s="64" t="s">
+      <c r="I20" s="62" t="s">
         <v>222</v>
       </c>
-      <c r="J20" s="50" t="s">
+      <c r="J20" s="49" t="s">
         <v>19</v>
       </c>
       <c r="K20" s="28">
@@ -3164,7 +3131,7 @@
       <c r="Q20" s="29"/>
       <c r="R20" s="30"/>
       <c r="S20" s="32"/>
-      <c r="T20" s="50">
+      <c r="T20" s="49">
         <f>K20+L20+M20+N20+O20+P20+Q20+R20+S20</f>
         <v>6</v>
       </c>
@@ -3186,13 +3153,13 @@
         <v>10</v>
       </c>
       <c r="G21" s="9"/>
-      <c r="H21" s="64" t="s">
+      <c r="H21" s="62" t="s">
         <v>221</v>
       </c>
-      <c r="I21" s="64" t="s">
+      <c r="I21" s="62" t="s">
         <v>406</v>
       </c>
-      <c r="J21" s="51" t="s">
+      <c r="J21" s="50" t="s">
         <v>17</v>
       </c>
       <c r="K21" s="21"/>
@@ -3204,7 +3171,7 @@
       <c r="Q21" s="31"/>
       <c r="R21" s="30"/>
       <c r="S21" s="32"/>
-      <c r="T21" s="51">
+      <c r="T21" s="50">
         <f>K21+L21+M21+N21+O21+P21+Q21+R21+S21</f>
         <v>0</v>
       </c>
@@ -3226,7 +3193,7 @@
         <v>10</v>
       </c>
       <c r="G22" s="9"/>
-      <c r="J22" s="52" t="s">
+      <c r="J22" s="51" t="s">
         <v>18</v>
       </c>
       <c r="K22" s="25"/>
@@ -3238,7 +3205,7 @@
       <c r="Q22" s="34"/>
       <c r="R22" s="33"/>
       <c r="S22" s="35"/>
-      <c r="T22" s="51">
+      <c r="T22" s="50">
         <f>K22+L22+M22+N22+O22+P22+Q22+R22+S22</f>
         <v>0</v>
       </c>
@@ -3269,11 +3236,11 @@
       <c r="P23" s="31"/>
       <c r="Q23" s="31"/>
       <c r="R23" s="31"/>
-      <c r="T23" s="65">
+      <c r="T23" s="63">
         <f>T20+T21+T22</f>
         <v>6</v>
       </c>
-      <c r="U23" s="66" t="s">
+      <c r="U23" s="64" t="s">
         <v>365</v>
       </c>
     </row>
@@ -3294,7 +3261,7 @@
         <v>10</v>
       </c>
       <c r="G24" s="9"/>
-      <c r="T24" s="53"/>
+      <c r="T24" s="52"/>
     </row>
     <row r="25" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
@@ -3303,34 +3270,34 @@
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="G25" s="9"/>
-      <c r="K25" s="49" t="s">
+      <c r="K25" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="L25" s="49" t="s">
+      <c r="L25" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="M25" s="49" t="s">
+      <c r="M25" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="N25" s="49" t="s">
+      <c r="N25" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="O25" s="49" t="s">
+      <c r="O25" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="P25" s="49" t="s">
+      <c r="P25" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="Q25" s="49" t="s">
+      <c r="Q25" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="R25" s="49" t="s">
+      <c r="R25" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="S25" s="49" t="s">
+      <c r="S25" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="T25" s="53"/>
+      <c r="T25" s="52"/>
     </row>
     <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
@@ -3377,7 +3344,7 @@
       <c r="S26" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="T26" s="53"/>
+      <c r="T26" s="52"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
@@ -3397,34 +3364,34 @@
       </c>
       <c r="G27" s="9"/>
       <c r="J27" s="10"/>
-      <c r="K27" s="76" t="s">
+      <c r="K27" s="74" t="s">
         <v>404</v>
       </c>
-      <c r="L27" s="73" t="s">
+      <c r="L27" s="71" t="s">
         <v>236</v>
       </c>
-      <c r="M27" s="91" t="s">
+      <c r="M27" s="80" t="s">
         <v>241</v>
       </c>
-      <c r="N27" s="73" t="s">
+      <c r="N27" s="71" t="s">
         <v>245</v>
       </c>
       <c r="O27" s="44" t="s">
         <v>260</v>
       </c>
-      <c r="P27" s="71" t="s">
+      <c r="P27" s="69" t="s">
         <v>254</v>
       </c>
       <c r="Q27" s="44" t="s">
         <v>265</v>
       </c>
-      <c r="R27" s="71" t="s">
+      <c r="R27" s="69" t="s">
         <v>266</v>
       </c>
       <c r="S27" s="44" t="s">
         <v>271</v>
       </c>
-      <c r="T27" s="53"/>
+      <c r="T27" s="52"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
@@ -3444,22 +3411,22 @@
       </c>
       <c r="G28" s="9"/>
       <c r="H28" s="5"/>
-      <c r="K28" s="67" t="s">
+      <c r="K28" s="65" t="s">
         <v>397</v>
       </c>
-      <c r="L28" s="75" t="s">
+      <c r="L28" s="73" t="s">
         <v>238</v>
       </c>
-      <c r="M28" s="67" t="s">
+      <c r="M28" s="65" t="s">
         <v>246</v>
       </c>
-      <c r="N28" s="75" t="s">
+      <c r="N28" s="73" t="s">
         <v>248</v>
       </c>
-      <c r="O28" s="69" t="s">
+      <c r="O28" s="67" t="s">
         <v>256</v>
       </c>
-      <c r="P28" s="72" t="s">
+      <c r="P28" s="70" t="s">
         <v>261</v>
       </c>
       <c r="Q28" s="42" t="s">
@@ -3471,7 +3438,7 @@
       <c r="S28" s="40" t="s">
         <v>272</v>
       </c>
-      <c r="T28" s="53"/>
+      <c r="T28" s="52"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
@@ -3490,19 +3457,19 @@
         <v>9</v>
       </c>
       <c r="J29" s="10"/>
-      <c r="K29" s="67" t="s">
+      <c r="K29" s="65" t="s">
         <v>403</v>
       </c>
-      <c r="L29" s="75" t="s">
+      <c r="L29" s="73" t="s">
         <v>239</v>
       </c>
-      <c r="M29" s="67" t="s">
+      <c r="M29" s="65" t="s">
         <v>247</v>
       </c>
-      <c r="N29" s="75" t="s">
+      <c r="N29" s="73" t="s">
         <v>249</v>
       </c>
-      <c r="O29" s="69" t="s">
+      <c r="O29" s="67" t="s">
         <v>257</v>
       </c>
       <c r="P29" s="14" t="s">
@@ -3517,7 +3484,7 @@
       <c r="S29" s="40" t="s">
         <v>274</v>
       </c>
-      <c r="T29" s="53"/>
+      <c r="T29" s="52"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
@@ -3536,16 +3503,16 @@
         <v>9</v>
       </c>
       <c r="J30" s="10"/>
-      <c r="K30" s="67" t="s">
+      <c r="K30" s="65" t="s">
         <v>398</v>
       </c>
-      <c r="L30" s="75" t="s">
+      <c r="L30" s="73" t="s">
         <v>240</v>
       </c>
-      <c r="M30" s="67" t="s">
+      <c r="M30" s="65" t="s">
         <v>402</v>
       </c>
-      <c r="N30" s="75" t="s">
+      <c r="N30" s="73" t="s">
         <v>251</v>
       </c>
       <c r="O30" s="40" t="s">
@@ -3563,7 +3530,7 @@
       <c r="S30" s="40" t="s">
         <v>276</v>
       </c>
-      <c r="T30" s="53"/>
+      <c r="T30" s="52"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
@@ -3582,16 +3549,16 @@
         <v>9</v>
       </c>
       <c r="J31" s="1"/>
-      <c r="K31" s="67" t="s">
+      <c r="K31" s="65" t="s">
         <v>237</v>
       </c>
-      <c r="L31" s="75" t="s">
+      <c r="L31" s="73" t="s">
         <v>242</v>
       </c>
-      <c r="M31" s="67" t="s">
+      <c r="M31" s="65" t="s">
         <v>401</v>
       </c>
-      <c r="N31" s="75" t="s">
+      <c r="N31" s="73" t="s">
         <v>252</v>
       </c>
       <c r="O31" s="42" t="s">
@@ -3607,7 +3574,7 @@
       <c r="S31" s="42" t="s">
         <v>277</v>
       </c>
-      <c r="T31" s="53"/>
+      <c r="T31" s="52"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
@@ -3626,16 +3593,16 @@
         <v>9</v>
       </c>
       <c r="J32" s="1"/>
-      <c r="K32" s="67" t="s">
+      <c r="K32" s="65" t="s">
         <v>244</v>
       </c>
-      <c r="L32" s="75" t="s">
+      <c r="L32" s="73" t="s">
         <v>243</v>
       </c>
-      <c r="M32" s="92" t="s">
+      <c r="M32" s="81" t="s">
         <v>250</v>
       </c>
-      <c r="N32" s="75" t="s">
+      <c r="N32" s="73" t="s">
         <v>253</v>
       </c>
       <c r="O32" s="42" t="s">
@@ -3651,7 +3618,7 @@
       <c r="S32" s="42" t="s">
         <v>278</v>
       </c>
-      <c r="T32" s="53"/>
+      <c r="T32" s="52"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
@@ -3660,16 +3627,16 @@
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="J33" s="10"/>
-      <c r="K33" s="67" t="s">
+      <c r="K33" s="65" t="s">
         <v>396</v>
       </c>
-      <c r="L33" s="75" t="s">
+      <c r="L33" s="73" t="s">
         <v>397</v>
       </c>
-      <c r="M33" s="67" t="s">
+      <c r="M33" s="65" t="s">
         <v>397</v>
       </c>
-      <c r="N33" s="75" t="s">
+      <c r="N33" s="73" t="s">
         <v>259</v>
       </c>
       <c r="O33" s="42"/>
@@ -3679,7 +3646,7 @@
       <c r="S33" s="42" t="s">
         <v>279</v>
       </c>
-      <c r="T33" s="53" t="s">
+      <c r="T33" s="52" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3700,24 +3667,24 @@
         <v>10</v>
       </c>
       <c r="J34" s="10"/>
-      <c r="K34" s="74" t="s">
+      <c r="K34" s="72" t="s">
         <v>399</v>
       </c>
-      <c r="L34" s="79" t="s">
+      <c r="L34" s="75" t="s">
         <v>400</v>
       </c>
-      <c r="M34" s="74" t="s">
+      <c r="M34" s="72" t="s">
         <v>408</v>
       </c>
-      <c r="N34" s="79" t="s">
+      <c r="N34" s="75" t="s">
         <v>407</v>
       </c>
       <c r="O34" s="43"/>
       <c r="P34" s="26"/>
       <c r="Q34" s="43"/>
-      <c r="R34" s="70"/>
+      <c r="R34" s="68"/>
       <c r="S34" s="43"/>
-      <c r="T34" s="53"/>
+      <c r="T34" s="52"/>
     </row>
     <row r="35" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
@@ -3735,7 +3702,7 @@
       <c r="E35" s="8">
         <v>10</v>
       </c>
-      <c r="J35" s="50" t="s">
+      <c r="J35" s="49" t="s">
         <v>20</v>
       </c>
       <c r="K35" s="30">
@@ -3755,7 +3722,7 @@
       <c r="Q35" s="30"/>
       <c r="R35" s="30"/>
       <c r="S35" s="30"/>
-      <c r="T35" s="54">
+      <c r="T35" s="53">
         <f>K35+L35+M35+N35+O35+P35+Q35+R35+S35</f>
         <v>575</v>
       </c>
@@ -3776,7 +3743,7 @@
       <c r="E36" s="8">
         <v>10</v>
       </c>
-      <c r="J36" s="52" t="s">
+      <c r="J36" s="51" t="s">
         <v>21</v>
       </c>
       <c r="K36" s="33">
@@ -3796,11 +3763,11 @@
       <c r="Q36" s="33"/>
       <c r="R36" s="33"/>
       <c r="S36" s="33"/>
-      <c r="T36" s="59">
+      <c r="T36" s="58">
         <f>K36+L36+M36+N36+O36+P36+Q36+R36+S36</f>
         <v>530</v>
       </c>
-      <c r="U36" s="66" t="s">
+      <c r="U36" s="64" t="s">
         <v>366</v>
       </c>
     </row>
@@ -3824,7 +3791,7 @@
       <c r="K37" s="31"/>
       <c r="L37" s="31"/>
       <c r="R37" s="31"/>
-      <c r="T37" s="66">
+      <c r="T37" s="64">
         <f>T35+T36</f>
         <v>1105</v>
       </c>
@@ -3993,7 +3960,7 @@
       <c r="E45" s="8">
         <v>8</v>
       </c>
-      <c r="N45" s="55"/>
+      <c r="N45" s="54"/>
       <c r="O45" s="8"/>
       <c r="Q45" s="10"/>
       <c r="R45" s="8"/>
@@ -5708,8 +5675,8 @@
       <c r="E133" s="8">
         <v>8</v>
       </c>
-      <c r="K133" s="55"/>
-      <c r="L133" s="55"/>
+      <c r="K133" s="54"/>
+      <c r="L133" s="54"/>
       <c r="M133" s="31"/>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
@@ -6191,7 +6158,7 @@
       <c r="E161" s="8">
         <v>4</v>
       </c>
-      <c r="R161" s="55"/>
+      <c r="R161" s="54"/>
     </row>
     <row r="162" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
@@ -7049,7 +7016,7 @@
       <c r="E217" s="8">
         <v>5</v>
       </c>
-      <c r="I217" s="68"/>
+      <c r="I217" s="66"/>
     </row>
     <row r="218" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
@@ -7067,7 +7034,7 @@
       <c r="E218" s="8">
         <v>5</v>
       </c>
-      <c r="I218" s="68"/>
+      <c r="I218" s="66"/>
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A219" s="5"/>
@@ -7075,7 +7042,7 @@
       <c r="C219" s="7"/>
       <c r="D219" s="8"/>
       <c r="E219" s="8"/>
-      <c r="I219" s="68"/>
+      <c r="I219" s="66"/>
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A220" s="24" t="s">
@@ -7093,7 +7060,7 @@
       <c r="E220" s="8">
         <v>5</v>
       </c>
-      <c r="I220" s="68"/>
+      <c r="I220" s="66"/>
     </row>
     <row r="221" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A221" s="24" t="s">
@@ -7111,7 +7078,7 @@
       <c r="E221" s="8">
         <v>5</v>
       </c>
-      <c r="I221" s="68"/>
+      <c r="I221" s="66"/>
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A222" s="24" t="s">
@@ -7129,7 +7096,7 @@
       <c r="E222" s="8">
         <v>5</v>
       </c>
-      <c r="I222" s="68"/>
+      <c r="I222" s="66"/>
       <c r="J222" s="31"/>
       <c r="K222" s="31"/>
       <c r="L222" s="31"/>
@@ -7150,7 +7117,7 @@
       <c r="E223" s="8">
         <v>5</v>
       </c>
-      <c r="I223" s="68"/>
+      <c r="I223" s="66"/>
       <c r="J223" s="31"/>
       <c r="K223" s="31"/>
       <c r="L223" s="31"/>
@@ -7161,7 +7128,7 @@
       <c r="C224" s="7"/>
       <c r="D224" s="8"/>
       <c r="E224" s="8"/>
-      <c r="I224" s="68"/>
+      <c r="I224" s="66"/>
       <c r="J224" s="31"/>
       <c r="K224" s="31"/>
       <c r="L224" s="31"/>
@@ -7182,7 +7149,7 @@
       <c r="E225" s="8">
         <v>5</v>
       </c>
-      <c r="I225" s="68"/>
+      <c r="I225" s="66"/>
       <c r="J225" s="31"/>
       <c r="K225" s="31"/>
       <c r="L225" s="31"/>
@@ -7203,7 +7170,7 @@
       <c r="E226" s="8">
         <v>5</v>
       </c>
-      <c r="I226" s="68"/>
+      <c r="I226" s="66"/>
       <c r="J226" s="31"/>
       <c r="K226" s="31"/>
       <c r="L226" s="31"/>
@@ -7225,7 +7192,7 @@
       <c r="E227" s="8">
         <v>5</v>
       </c>
-      <c r="I227" s="68"/>
+      <c r="I227" s="66"/>
       <c r="J227" s="31"/>
       <c r="K227" s="31"/>
       <c r="L227" s="31"/>
@@ -7247,7 +7214,7 @@
       <c r="E228" s="8">
         <v>5</v>
       </c>
-      <c r="I228" s="68"/>
+      <c r="I228" s="66"/>
       <c r="J228" s="31"/>
       <c r="K228" s="31"/>
       <c r="L228" s="31"/>
@@ -7259,7 +7226,7 @@
       <c r="C229" s="7"/>
       <c r="D229" s="8"/>
       <c r="E229" s="8"/>
-      <c r="I229" s="68"/>
+      <c r="I229" s="66"/>
       <c r="J229" s="31"/>
       <c r="K229" s="31"/>
       <c r="L229" s="31"/>
@@ -7281,8 +7248,8 @@
       <c r="E230" s="8">
         <v>6</v>
       </c>
-      <c r="I230" s="68"/>
-      <c r="J230" s="55"/>
+      <c r="I230" s="66"/>
+      <c r="J230" s="54"/>
       <c r="K230" s="31"/>
       <c r="L230" s="31"/>
       <c r="S230" s="31"/>
@@ -7303,7 +7270,7 @@
       <c r="E231" s="8">
         <v>6</v>
       </c>
-      <c r="I231" s="68"/>
+      <c r="I231" s="66"/>
       <c r="J231" s="31"/>
       <c r="K231" s="31"/>
       <c r="L231" s="31"/>
@@ -7325,7 +7292,7 @@
       <c r="E232" s="8">
         <v>6</v>
       </c>
-      <c r="I232" s="68"/>
+      <c r="I232" s="66"/>
       <c r="J232" s="31"/>
       <c r="K232" s="31"/>
       <c r="L232" s="31"/>
@@ -7347,7 +7314,7 @@
       <c r="E233" s="8">
         <v>6</v>
       </c>
-      <c r="I233" s="68"/>
+      <c r="I233" s="66"/>
       <c r="J233" s="14"/>
       <c r="K233" s="31"/>
       <c r="L233" s="31"/>
@@ -7359,7 +7326,7 @@
       <c r="C234" s="7"/>
       <c r="D234" s="8"/>
       <c r="E234" s="8"/>
-      <c r="I234" s="68"/>
+      <c r="I234" s="66"/>
       <c r="J234" s="14"/>
       <c r="K234" s="31"/>
       <c r="L234" s="31"/>
@@ -7381,7 +7348,7 @@
       <c r="E235" s="8">
         <v>6</v>
       </c>
-      <c r="I235" s="68"/>
+      <c r="I235" s="66"/>
       <c r="J235" s="14"/>
       <c r="K235" s="31"/>
       <c r="L235" s="31"/>
@@ -7403,7 +7370,7 @@
       <c r="E236" s="8">
         <v>6</v>
       </c>
-      <c r="I236" s="68"/>
+      <c r="I236" s="66"/>
       <c r="J236" s="14"/>
       <c r="K236" s="31"/>
       <c r="L236" s="31"/>
@@ -7425,7 +7392,7 @@
       <c r="E237" s="8">
         <v>6</v>
       </c>
-      <c r="I237" s="68"/>
+      <c r="I237" s="66"/>
       <c r="J237" s="14"/>
       <c r="K237" s="31"/>
       <c r="L237" s="31"/>
@@ -7447,7 +7414,7 @@
       <c r="E238" s="8">
         <v>6</v>
       </c>
-      <c r="I238" s="68"/>
+      <c r="I238" s="66"/>
       <c r="J238" s="31"/>
       <c r="K238" s="31"/>
       <c r="L238" s="31"/>
@@ -7520,7 +7487,7 @@
       <c r="E242" s="17">
         <v>6</v>
       </c>
-      <c r="J242" s="56"/>
+      <c r="J242" s="55"/>
       <c r="K242" s="31"/>
       <c r="L242" s="31"/>
     </row>
@@ -12695,19 +12662,19 @@
       <c r="H586" s="4"/>
     </row>
     <row r="587" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A587" s="88" t="s">
+      <c r="A587" s="77" t="s">
         <v>53</v>
       </c>
       <c r="B587" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C587" s="89" t="s">
+      <c r="C587" s="78" t="s">
         <v>89</v>
       </c>
-      <c r="D587" s="90">
+      <c r="D587" s="79">
         <v>20</v>
       </c>
-      <c r="E587" s="90">
+      <c r="E587" s="79">
         <v>7</v>
       </c>
       <c r="H587" s="4"/>
@@ -13393,19 +13360,19 @@
       </c>
     </row>
     <row r="631" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A631" s="88" t="s">
+      <c r="A631" s="77" t="s">
         <v>81</v>
       </c>
       <c r="B631" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C631" s="89" t="s">
+      <c r="C631" s="78" t="s">
         <v>89</v>
       </c>
-      <c r="D631" s="90">
+      <c r="D631" s="79">
         <v>60</v>
       </c>
-      <c r="E631" s="90">
+      <c r="E631" s="79">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Survivor met continue button & UML Update & Asset List Update
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1846" uniqueCount="410">
   <si>
     <t>ID Code</t>
   </si>
@@ -1244,6 +1244,9 @@
   </si>
   <si>
     <t>Items_LootPackage (30)</t>
+  </si>
+  <si>
+    <t>Items_LootPackage (10)</t>
   </si>
 </sst>
 </file>
@@ -1572,7 +1575,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1769,9 +1772,6 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1781,16 +1781,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1815,6 +1809,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2134,8 +2131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N40" sqref="N40"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2305,13 +2302,13 @@
         <v>228</v>
       </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="83" t="s">
+      <c r="K3" s="80" t="s">
         <v>282</v>
       </c>
-      <c r="L3" s="83" t="s">
+      <c r="L3" s="80" t="s">
         <v>290</v>
       </c>
-      <c r="M3" s="83" t="s">
+      <c r="M3" s="80" t="s">
         <v>391</v>
       </c>
       <c r="N3" s="61" t="s">
@@ -2362,19 +2359,19 @@
         <v>229</v>
       </c>
       <c r="J4" s="10"/>
-      <c r="K4" s="76" t="s">
+      <c r="K4" s="73" t="s">
         <v>283</v>
       </c>
-      <c r="L4" s="76" t="s">
+      <c r="L4" s="73" t="s">
         <v>291</v>
       </c>
-      <c r="M4" s="76" t="s">
+      <c r="M4" s="73" t="s">
         <v>295</v>
       </c>
       <c r="N4" s="42" t="s">
         <v>305</v>
       </c>
-      <c r="O4" s="73" t="s">
+      <c r="O4" s="71" t="s">
         <v>322</v>
       </c>
       <c r="P4" s="40" t="s">
@@ -2419,7 +2416,7 @@
         <v>233</v>
       </c>
       <c r="J5" s="10"/>
-      <c r="K5" s="76" t="s">
+      <c r="K5" s="73" t="s">
         <v>284</v>
       </c>
       <c r="L5" s="56" t="s">
@@ -2476,10 +2473,10 @@
         <v>223</v>
       </c>
       <c r="J6" s="1"/>
-      <c r="K6" s="82" t="s">
+      <c r="K6" s="79" t="s">
         <v>289</v>
       </c>
-      <c r="L6" s="76" t="s">
+      <c r="L6" s="73" t="s">
         <v>293</v>
       </c>
       <c r="M6" s="13" t="s">
@@ -2533,7 +2530,7 @@
         <v>224</v>
       </c>
       <c r="J7" s="1"/>
-      <c r="K7" s="76" t="s">
+      <c r="K7" s="73" t="s">
         <v>286</v>
       </c>
       <c r="L7" s="56" t="s">
@@ -2590,10 +2587,10 @@
         <v>230</v>
       </c>
       <c r="J8" s="1"/>
-      <c r="K8" s="76" t="s">
+      <c r="K8" s="73" t="s">
         <v>287</v>
       </c>
-      <c r="L8" s="76" t="s">
+      <c r="L8" s="73" t="s">
         <v>387</v>
       </c>
       <c r="M8" s="13" t="s">
@@ -2635,10 +2632,10 @@
         <v>225</v>
       </c>
       <c r="J9" s="1"/>
-      <c r="K9" s="76" t="s">
+      <c r="K9" s="73" t="s">
         <v>288</v>
       </c>
-      <c r="L9" s="76" t="s">
+      <c r="L9" s="73" t="s">
         <v>389</v>
       </c>
       <c r="M9" s="13" t="s">
@@ -2690,10 +2687,10 @@
         <v>226</v>
       </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="76" t="s">
+      <c r="K10" s="73" t="s">
         <v>388</v>
       </c>
-      <c r="L10" s="76" t="s">
+      <c r="L10" s="73" t="s">
         <v>390</v>
       </c>
       <c r="M10" s="13" t="s">
@@ -2744,10 +2741,10 @@
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="56"/>
-      <c r="L11" s="76" t="s">
+      <c r="L11" s="73" t="s">
         <v>392</v>
       </c>
-      <c r="M11" s="82" t="s">
+      <c r="M11" s="79" t="s">
         <v>301</v>
       </c>
       <c r="N11" s="42" t="s">
@@ -2797,7 +2794,7 @@
       <c r="L12" s="13" t="s">
         <v>393</v>
       </c>
-      <c r="M12" s="76" t="s">
+      <c r="M12" s="73" t="s">
         <v>302</v>
       </c>
       <c r="N12" s="46" t="s">
@@ -2844,10 +2841,10 @@
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="56"/>
-      <c r="L13" s="76" t="s">
+      <c r="L13" s="73" t="s">
         <v>285</v>
       </c>
-      <c r="M13" s="76" t="s">
+      <c r="M13" s="73" t="s">
         <v>303</v>
       </c>
       <c r="N13" s="42" t="s">
@@ -2943,7 +2940,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="56"/>
       <c r="L15" s="56"/>
-      <c r="M15" s="76" t="s">
+      <c r="M15" s="73" t="s">
         <v>353</v>
       </c>
       <c r="N15" s="40" t="s">
@@ -3364,28 +3361,28 @@
       </c>
       <c r="G27" s="9"/>
       <c r="J27" s="10"/>
-      <c r="K27" s="74" t="s">
+      <c r="K27" s="72" t="s">
         <v>404</v>
       </c>
-      <c r="L27" s="71" t="s">
+      <c r="L27" s="70" t="s">
         <v>236</v>
       </c>
-      <c r="M27" s="80" t="s">
+      <c r="M27" s="77" t="s">
         <v>241</v>
       </c>
-      <c r="N27" s="71" t="s">
+      <c r="N27" s="70" t="s">
         <v>245</v>
       </c>
       <c r="O27" s="44" t="s">
         <v>260</v>
       </c>
-      <c r="P27" s="69" t="s">
+      <c r="P27" s="68" t="s">
         <v>254</v>
       </c>
       <c r="Q27" s="44" t="s">
         <v>265</v>
       </c>
-      <c r="R27" s="69" t="s">
+      <c r="R27" s="68" t="s">
         <v>266</v>
       </c>
       <c r="S27" s="44" t="s">
@@ -3414,19 +3411,19 @@
       <c r="K28" s="65" t="s">
         <v>397</v>
       </c>
-      <c r="L28" s="73" t="s">
+      <c r="L28" s="71" t="s">
         <v>238</v>
       </c>
       <c r="M28" s="65" t="s">
         <v>246</v>
       </c>
-      <c r="N28" s="73" t="s">
+      <c r="N28" s="71" t="s">
         <v>248</v>
       </c>
       <c r="O28" s="67" t="s">
         <v>256</v>
       </c>
-      <c r="P28" s="70" t="s">
+      <c r="P28" s="69" t="s">
         <v>261</v>
       </c>
       <c r="Q28" s="42" t="s">
@@ -3460,13 +3457,13 @@
       <c r="K29" s="65" t="s">
         <v>403</v>
       </c>
-      <c r="L29" s="73" t="s">
+      <c r="L29" s="71" t="s">
         <v>239</v>
       </c>
       <c r="M29" s="65" t="s">
         <v>247</v>
       </c>
-      <c r="N29" s="73" t="s">
+      <c r="N29" s="71" t="s">
         <v>249</v>
       </c>
       <c r="O29" s="67" t="s">
@@ -3506,13 +3503,13 @@
       <c r="K30" s="65" t="s">
         <v>398</v>
       </c>
-      <c r="L30" s="73" t="s">
+      <c r="L30" s="71" t="s">
         <v>240</v>
       </c>
       <c r="M30" s="65" t="s">
         <v>402</v>
       </c>
-      <c r="N30" s="73" t="s">
+      <c r="N30" s="71" t="s">
         <v>251</v>
       </c>
       <c r="O30" s="40" t="s">
@@ -3552,16 +3549,16 @@
       <c r="K31" s="65" t="s">
         <v>237</v>
       </c>
-      <c r="L31" s="73" t="s">
+      <c r="L31" s="71" t="s">
         <v>242</v>
       </c>
       <c r="M31" s="65" t="s">
         <v>401</v>
       </c>
-      <c r="N31" s="73" t="s">
-        <v>252</v>
-      </c>
-      <c r="O31" s="42" t="s">
+      <c r="N31" s="81" t="s">
+        <v>409</v>
+      </c>
+      <c r="O31" s="65" t="s">
         <v>255</v>
       </c>
       <c r="P31" s="15" t="s">
@@ -3596,14 +3593,14 @@
       <c r="K32" s="65" t="s">
         <v>244</v>
       </c>
-      <c r="L32" s="73" t="s">
+      <c r="L32" s="71" t="s">
         <v>243</v>
       </c>
-      <c r="M32" s="81" t="s">
+      <c r="M32" s="78" t="s">
         <v>250</v>
       </c>
-      <c r="N32" s="73" t="s">
-        <v>253</v>
+      <c r="N32" s="71" t="s">
+        <v>252</v>
       </c>
       <c r="O32" s="42" t="s">
         <v>397</v>
@@ -3630,14 +3627,14 @@
       <c r="K33" s="65" t="s">
         <v>396</v>
       </c>
-      <c r="L33" s="73" t="s">
+      <c r="L33" s="71" t="s">
         <v>397</v>
       </c>
       <c r="M33" s="65" t="s">
         <v>397</v>
       </c>
-      <c r="N33" s="73" t="s">
-        <v>259</v>
+      <c r="N33" s="71" t="s">
+        <v>253</v>
       </c>
       <c r="O33" s="42"/>
       <c r="P33" s="15"/>
@@ -3646,11 +3643,8 @@
       <c r="S33" s="42" t="s">
         <v>279</v>
       </c>
-      <c r="T33" s="52" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>96</v>
       </c>
@@ -3667,24 +3661,23 @@
         <v>10</v>
       </c>
       <c r="J34" s="10"/>
-      <c r="K34" s="72" t="s">
+      <c r="K34" s="65" t="s">
         <v>399</v>
       </c>
-      <c r="L34" s="75" t="s">
+      <c r="L34" s="71" t="s">
         <v>400</v>
       </c>
-      <c r="M34" s="72" t="s">
+      <c r="M34" s="65" t="s">
         <v>408</v>
       </c>
-      <c r="N34" s="75" t="s">
-        <v>407</v>
-      </c>
-      <c r="O34" s="43"/>
-      <c r="P34" s="26"/>
-      <c r="Q34" s="43"/>
-      <c r="R34" s="68"/>
-      <c r="S34" s="43"/>
-      <c r="T34" s="52"/>
+      <c r="N34" s="71" t="s">
+        <v>259</v>
+      </c>
+      <c r="O34" s="42"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="42"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="42"/>
     </row>
     <row r="35" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
@@ -3702,29 +3695,19 @@
       <c r="E35" s="8">
         <v>10</v>
       </c>
-      <c r="J35" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="K35" s="30">
-        <v>205</v>
-      </c>
-      <c r="L35" s="30">
-        <v>140</v>
-      </c>
-      <c r="M35" s="30">
-        <v>100</v>
-      </c>
-      <c r="N35" s="30">
-        <v>130</v>
-      </c>
-      <c r="O35" s="30"/>
-      <c r="P35" s="30"/>
-      <c r="Q35" s="30"/>
-      <c r="R35" s="30"/>
-      <c r="S35" s="30"/>
-      <c r="T35" s="53">
-        <f>K35+L35+M35+N35+O35+P35+Q35+R35+S35</f>
-        <v>575</v>
+      <c r="K35" s="45"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="45"/>
+      <c r="N35" s="71" t="s">
+        <v>407</v>
+      </c>
+      <c r="O35" s="43"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="43"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="43"/>
+      <c r="T35" s="52" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3743,32 +3726,29 @@
       <c r="E36" s="8">
         <v>10</v>
       </c>
-      <c r="J36" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="K36" s="33">
-        <v>110</v>
-      </c>
-      <c r="L36" s="33">
-        <v>145</v>
-      </c>
-      <c r="M36" s="33">
-        <v>105</v>
-      </c>
-      <c r="N36" s="33">
-        <v>170</v>
-      </c>
-      <c r="O36" s="33"/>
-      <c r="P36" s="33"/>
-      <c r="Q36" s="33"/>
-      <c r="R36" s="33"/>
-      <c r="S36" s="33"/>
-      <c r="T36" s="58">
+      <c r="J36" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="K36" s="27">
+        <v>205</v>
+      </c>
+      <c r="L36" s="27">
+        <v>140</v>
+      </c>
+      <c r="M36" s="27"/>
+      <c r="N36" s="27">
+        <v>140</v>
+      </c>
+      <c r="O36" s="27">
+        <v>20</v>
+      </c>
+      <c r="P36" s="27"/>
+      <c r="Q36" s="27"/>
+      <c r="R36" s="27"/>
+      <c r="S36" s="27"/>
+      <c r="T36" s="53">
         <f>K36+L36+M36+N36+O36+P36+Q36+R36+S36</f>
-        <v>530</v>
-      </c>
-      <c r="U36" s="64" t="s">
-        <v>366</v>
+        <v>505</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3787,16 +3767,33 @@
       <c r="E37" s="8">
         <v>10</v>
       </c>
-      <c r="J37" s="10"/>
-      <c r="K37" s="31"/>
-      <c r="L37" s="31"/>
-      <c r="R37" s="31"/>
-      <c r="T37" s="64">
-        <f>T35+T36</f>
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J37" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="K37" s="33">
+        <v>110</v>
+      </c>
+      <c r="L37" s="33">
+        <v>145</v>
+      </c>
+      <c r="M37" s="33"/>
+      <c r="N37" s="33">
+        <v>170</v>
+      </c>
+      <c r="O37" s="33"/>
+      <c r="P37" s="33"/>
+      <c r="Q37" s="33"/>
+      <c r="R37" s="33"/>
+      <c r="S37" s="33"/>
+      <c r="T37" s="58">
+        <f>K37+L37+M37+N37+O37+P37+Q37+R37+S37</f>
+        <v>425</v>
+      </c>
+      <c r="U37" s="64" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>96</v>
       </c>
@@ -3812,10 +3809,13 @@
       <c r="E38" s="8">
         <v>10</v>
       </c>
-      <c r="O38" s="8"/>
-      <c r="P38" s="10"/>
-      <c r="Q38" s="8"/>
-      <c r="T38" s="4"/>
+      <c r="K38" s="31"/>
+      <c r="L38" s="31"/>
+      <c r="R38" s="31"/>
+      <c r="T38" s="64">
+        <f>T36+T37</f>
+        <v>930</v>
+      </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
@@ -3835,9 +3835,7 @@
       </c>
       <c r="O39" s="8"/>
       <c r="P39" s="10"/>
-      <c r="Q39" s="10"/>
-      <c r="R39" s="8"/>
-      <c r="S39" s="8"/>
+      <c r="Q39" s="8"/>
       <c r="T39" s="4"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
@@ -3857,7 +3855,7 @@
         <v>10</v>
       </c>
       <c r="O40" s="8"/>
-      <c r="P40" s="7"/>
+      <c r="P40" s="10"/>
       <c r="Q40" s="10"/>
       <c r="R40" s="8"/>
       <c r="S40" s="8"/>
@@ -3870,8 +3868,9 @@
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="O41" s="8"/>
-      <c r="P41" s="10"/>
+      <c r="P41" s="7"/>
       <c r="Q41" s="10"/>
+      <c r="R41" s="8"/>
       <c r="S41" s="8"/>
       <c r="T41" s="4"/>
     </row>
@@ -3892,9 +3891,8 @@
         <v>8</v>
       </c>
       <c r="O42" s="8"/>
-      <c r="P42" s="7"/>
+      <c r="P42" s="10"/>
       <c r="Q42" s="10"/>
-      <c r="R42" s="8"/>
       <c r="S42" s="8"/>
       <c r="T42" s="4"/>
     </row>
@@ -3915,10 +3913,10 @@
         <v>8</v>
       </c>
       <c r="O43" s="8"/>
-      <c r="P43" s="10"/>
+      <c r="P43" s="7"/>
       <c r="Q43" s="10"/>
       <c r="R43" s="8"/>
-      <c r="S43" s="17"/>
+      <c r="S43" s="8"/>
       <c r="T43" s="4"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
@@ -3937,8 +3935,8 @@
       <c r="E44" s="8">
         <v>8</v>
       </c>
-      <c r="N44" s="31"/>
       <c r="O44" s="8"/>
+      <c r="P44" s="10"/>
       <c r="Q44" s="10"/>
       <c r="R44" s="8"/>
       <c r="S44" s="17"/>
@@ -3960,7 +3958,7 @@
       <c r="E45" s="8">
         <v>8</v>
       </c>
-      <c r="N45" s="54"/>
+      <c r="N45" s="31"/>
       <c r="O45" s="8"/>
       <c r="Q45" s="10"/>
       <c r="R45" s="8"/>
@@ -3983,7 +3981,7 @@
       <c r="E46" s="8">
         <v>8</v>
       </c>
-      <c r="N46" s="31"/>
+      <c r="N46" s="54"/>
       <c r="O46" s="8"/>
       <c r="Q46" s="10"/>
       <c r="R46" s="8"/>
@@ -4008,7 +4006,7 @@
       </c>
       <c r="N47" s="31"/>
       <c r="O47" s="8"/>
-      <c r="Q47" s="7"/>
+      <c r="Q47" s="10"/>
       <c r="R47" s="8"/>
       <c r="S47" s="17"/>
       <c r="T47" s="4"/>
@@ -4029,7 +4027,7 @@
       <c r="E48" s="8">
         <v>8</v>
       </c>
-      <c r="N48" s="15"/>
+      <c r="N48" s="31"/>
       <c r="O48" s="8"/>
       <c r="Q48" s="7"/>
       <c r="R48" s="8"/>
@@ -4042,7 +4040,7 @@
       <c r="C49" s="7"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
-      <c r="N49" s="14"/>
+      <c r="N49" s="15"/>
       <c r="O49" s="8"/>
       <c r="Q49" s="7"/>
       <c r="R49" s="8"/>
@@ -4066,6 +4064,7 @@
         <v>7</v>
       </c>
       <c r="N50" s="14"/>
+      <c r="O50" s="8"/>
       <c r="Q50" s="7"/>
       <c r="R50" s="8"/>
       <c r="S50" s="17"/>
@@ -4088,7 +4087,7 @@
         <v>7</v>
       </c>
       <c r="N51" s="14"/>
-      <c r="Q51" s="10"/>
+      <c r="Q51" s="7"/>
       <c r="R51" s="8"/>
       <c r="S51" s="17"/>
       <c r="T51" s="4"/>
@@ -4153,7 +4152,7 @@
       <c r="E54" s="8">
         <v>7</v>
       </c>
-      <c r="N54" s="15"/>
+      <c r="N54" s="14"/>
       <c r="Q54" s="10"/>
       <c r="R54" s="8"/>
       <c r="S54" s="17"/>
@@ -4175,7 +4174,7 @@
       <c r="E55" s="8">
         <v>7</v>
       </c>
-      <c r="N55" s="31"/>
+      <c r="N55" s="15"/>
       <c r="Q55" s="10"/>
       <c r="R55" s="8"/>
       <c r="S55" s="17"/>
@@ -4208,7 +4207,7 @@
       <c r="C57" s="7"/>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
-      <c r="N57" s="15"/>
+      <c r="N57" s="31"/>
       <c r="Q57" s="10"/>
       <c r="R57" s="8"/>
       <c r="S57" s="17"/>
@@ -4252,7 +4251,7 @@
       <c r="E59" s="8">
         <v>10</v>
       </c>
-      <c r="N59" s="7"/>
+      <c r="N59" s="15"/>
       <c r="Q59" s="10"/>
       <c r="R59" s="8"/>
       <c r="S59" s="17"/>
@@ -4274,6 +4273,7 @@
       <c r="E60" s="8">
         <v>10</v>
       </c>
+      <c r="N60" s="7"/>
       <c r="Q60" s="10"/>
       <c r="R60" s="8"/>
       <c r="S60" s="17"/>
@@ -4337,7 +4337,7 @@
       <c r="E63" s="8">
         <v>10</v>
       </c>
-      <c r="Q63" s="7"/>
+      <c r="Q63" s="10"/>
       <c r="R63" s="8"/>
       <c r="S63" s="17"/>
       <c r="T63" s="4"/>
@@ -4411,7 +4411,7 @@
       <c r="E67" s="8">
         <v>10</v>
       </c>
-      <c r="Q67" s="10"/>
+      <c r="Q67" s="7"/>
       <c r="R67" s="8"/>
       <c r="S67" s="17"/>
       <c r="T67" s="4"/>
@@ -4740,7 +4740,7 @@
       </c>
       <c r="Q83" s="10"/>
       <c r="R83" s="8"/>
-      <c r="S83" s="8"/>
+      <c r="S83" s="17"/>
       <c r="T83" s="4"/>
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.25">
@@ -4970,7 +4970,7 @@
       <c r="E95" s="8">
         <v>7</v>
       </c>
-      <c r="Q95" s="7"/>
+      <c r="Q95" s="10"/>
       <c r="R95" s="8"/>
       <c r="S95" s="8"/>
       <c r="T95" s="4"/>
@@ -5054,7 +5054,7 @@
       <c r="E99" s="8">
         <v>7</v>
       </c>
-      <c r="Q99" s="10"/>
+      <c r="Q99" s="7"/>
       <c r="R99" s="8"/>
       <c r="S99" s="8"/>
       <c r="T99" s="4"/>
@@ -5128,7 +5128,7 @@
       <c r="E103" s="8">
         <v>6</v>
       </c>
-      <c r="Q103" s="7"/>
+      <c r="Q103" s="10"/>
       <c r="R103" s="8"/>
       <c r="S103" s="8"/>
       <c r="T103" s="4"/>
@@ -5212,6 +5212,8 @@
       <c r="E107" s="8">
         <v>6</v>
       </c>
+      <c r="Q107" s="7"/>
+      <c r="R107" s="8"/>
       <c r="S107" s="8"/>
       <c r="T107" s="4"/>
     </row>
@@ -5420,6 +5422,7 @@
       <c r="E119" s="8">
         <v>10</v>
       </c>
+      <c r="S119" s="8"/>
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
@@ -5505,9 +5508,6 @@
       <c r="E124" s="8">
         <v>10</v>
       </c>
-      <c r="K124" s="31"/>
-      <c r="L124" s="31"/>
-      <c r="M124" s="31"/>
     </row>
     <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
@@ -5675,8 +5675,8 @@
       <c r="E133" s="8">
         <v>8</v>
       </c>
-      <c r="K133" s="54"/>
-      <c r="L133" s="54"/>
+      <c r="K133" s="31"/>
+      <c r="L133" s="31"/>
       <c r="M133" s="31"/>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
@@ -5696,8 +5696,8 @@
         <v>8</v>
       </c>
       <c r="I134" s="14"/>
-      <c r="K134" s="31"/>
-      <c r="L134" s="31"/>
+      <c r="K134" s="54"/>
+      <c r="L134" s="54"/>
       <c r="M134" s="31"/>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
@@ -5728,8 +5728,8 @@
         <v>10</v>
       </c>
       <c r="I136" s="15"/>
-      <c r="K136" s="14"/>
-      <c r="L136" s="14"/>
+      <c r="K136" s="31"/>
+      <c r="L136" s="31"/>
       <c r="M136" s="31"/>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
@@ -5808,8 +5808,8 @@
       <c r="E140" s="8">
         <v>10</v>
       </c>
-      <c r="K140" s="15"/>
-      <c r="L140" s="15"/>
+      <c r="K140" s="14"/>
+      <c r="L140" s="14"/>
       <c r="M140" s="31"/>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.25">
@@ -5868,8 +5868,8 @@
       <c r="E143" s="8">
         <v>10</v>
       </c>
-      <c r="K143" s="31"/>
-      <c r="L143" s="31"/>
+      <c r="K143" s="15"/>
+      <c r="L143" s="15"/>
       <c r="M143" s="31"/>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
@@ -5898,8 +5898,8 @@
       <c r="E145" s="8">
         <v>9</v>
       </c>
-      <c r="K145" s="15"/>
-      <c r="L145" s="15"/>
+      <c r="K145" s="31"/>
+      <c r="L145" s="31"/>
       <c r="M145" s="31"/>
     </row>
     <row r="146" spans="1:18" x14ac:dyDescent="0.25">
@@ -5958,8 +5958,8 @@
       <c r="E148" s="8">
         <v>9</v>
       </c>
-      <c r="K148" s="31"/>
-      <c r="L148" s="31"/>
+      <c r="K148" s="15"/>
+      <c r="L148" s="15"/>
       <c r="M148" s="31"/>
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.25">
@@ -5968,6 +5968,9 @@
       <c r="C149" s="7"/>
       <c r="D149" s="8"/>
       <c r="E149" s="8"/>
+      <c r="K149" s="31"/>
+      <c r="L149" s="31"/>
+      <c r="M149" s="31"/>
     </row>
     <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
@@ -6060,7 +6063,6 @@
       <c r="E155" s="8">
         <v>8</v>
       </c>
-      <c r="R155" s="31"/>
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
@@ -6158,7 +6160,7 @@
       <c r="E161" s="8">
         <v>4</v>
       </c>
-      <c r="R161" s="54"/>
+      <c r="R161" s="31"/>
     </row>
     <row r="162" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
@@ -6176,7 +6178,7 @@
       <c r="E162" s="8">
         <v>4</v>
       </c>
-      <c r="R162" s="31"/>
+      <c r="R162" s="54"/>
     </row>
     <row r="163" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
@@ -6202,7 +6204,7 @@
       <c r="C164" s="7"/>
       <c r="D164" s="8"/>
       <c r="E164" s="8"/>
-      <c r="R164" s="14"/>
+      <c r="R164" s="31"/>
     </row>
     <row r="165" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
@@ -6238,7 +6240,7 @@
       <c r="E166" s="8">
         <v>8</v>
       </c>
-      <c r="R166" s="15"/>
+      <c r="R166" s="14"/>
     </row>
     <row r="167" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
@@ -6256,7 +6258,7 @@
       <c r="E167" s="8">
         <v>8</v>
       </c>
-      <c r="R167" s="14"/>
+      <c r="R167" s="15"/>
     </row>
     <row r="168" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
@@ -6318,7 +6320,7 @@
       <c r="E171" s="8">
         <v>5</v>
       </c>
-      <c r="R171" s="31"/>
+      <c r="R171" s="14"/>
     </row>
     <row r="172" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A172" s="24" t="s">
@@ -6354,7 +6356,7 @@
       <c r="E173" s="8">
         <v>5</v>
       </c>
-      <c r="R173" s="14"/>
+      <c r="R173" s="31"/>
     </row>
     <row r="174" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A174" s="24"/>
@@ -6362,7 +6364,7 @@
       <c r="C174" s="7"/>
       <c r="D174" s="8"/>
       <c r="E174" s="8"/>
-      <c r="R174" s="7"/>
+      <c r="R174" s="14"/>
     </row>
     <row r="175" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
@@ -6398,6 +6400,7 @@
       <c r="E176" s="8">
         <v>7</v>
       </c>
+      <c r="R176" s="7"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
@@ -7098,8 +7101,6 @@
       </c>
       <c r="I222" s="66"/>
       <c r="J222" s="31"/>
-      <c r="K222" s="31"/>
-      <c r="L222" s="31"/>
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A223" s="24" t="s">
@@ -7174,7 +7175,6 @@
       <c r="J226" s="31"/>
       <c r="K226" s="31"/>
       <c r="L226" s="31"/>
-      <c r="S226" s="31"/>
     </row>
     <row r="227" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A227" s="5" t="s">
@@ -7490,6 +7490,7 @@
       <c r="J242" s="55"/>
       <c r="K242" s="31"/>
       <c r="L242" s="31"/>
+      <c r="S242" s="31"/>
     </row>
     <row r="243" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A243" s="5" t="s">
@@ -7516,6 +7517,8 @@
       <c r="B244" s="7"/>
       <c r="C244" s="7"/>
       <c r="J244" s="36"/>
+      <c r="K244" s="31"/>
+      <c r="L244" s="31"/>
     </row>
     <row r="245" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A245" s="24" t="s">
@@ -12662,19 +12665,19 @@
       <c r="H586" s="4"/>
     </row>
     <row r="587" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A587" s="77" t="s">
+      <c r="A587" s="74" t="s">
         <v>53</v>
       </c>
       <c r="B587" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C587" s="78" t="s">
+      <c r="C587" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="D587" s="79">
+      <c r="D587" s="76">
         <v>20</v>
       </c>
-      <c r="E587" s="79">
+      <c r="E587" s="76">
         <v>7</v>
       </c>
       <c r="H587" s="4"/>
@@ -13360,19 +13363,19 @@
       </c>
     </row>
     <row r="631" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A631" s="77" t="s">
+      <c r="A631" s="74" t="s">
         <v>81</v>
       </c>
       <c r="B631" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C631" s="78" t="s">
+      <c r="C631" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="D631" s="79">
+      <c r="D631" s="76">
         <v>60</v>
       </c>
-      <c r="E631" s="79">
+      <c r="E631" s="76">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update UML remove harpoon uren registratie
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1846" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="409">
   <si>
     <t>ID Code</t>
   </si>
@@ -791,9 +791,6 @@
   </si>
   <si>
     <t>Weapons_Pistol (60)</t>
-  </si>
-  <si>
-    <t>Weapons_HarpoonGun (50)</t>
   </si>
   <si>
     <t>Weapons_StunGrenades (70)</t>
@@ -2129,7 +2126,7 @@
   <dimension ref="A1:U1029"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P43" sqref="P43"/>
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2300,31 +2297,31 @@
       </c>
       <c r="J3" s="10"/>
       <c r="K3" s="79" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L3" s="79" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="M3" s="79" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="N3" s="61" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="P3" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="R3" s="41" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="S3" s="61" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -2357,31 +2354,31 @@
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="72" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L4" s="72" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="M4" s="72" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N4" s="42" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="O4" s="70" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="P4" s="40" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="R4" s="40" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="S4" s="42" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -2414,31 +2411,31 @@
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="72" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L5" s="56" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="N5" s="42" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="O5" s="15" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="P5" s="65" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="Q5" s="10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="R5" s="42" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="S5" s="40" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -2471,31 +2468,31 @@
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="78" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L6" s="72" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N6" s="42" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="O6" s="15" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="P6" s="40" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="R6" s="40" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="S6" s="40" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -2528,31 +2525,31 @@
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="72" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L7" s="56" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="N7" s="42" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="O7" s="56" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="P7" s="42" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="R7" s="40" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="S7" s="40" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -2585,31 +2582,31 @@
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="72" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L8" s="72" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="M8" s="13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N8" s="65" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O8" s="56" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="P8" s="40" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="R8" s="40" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="S8" s="65" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -2630,31 +2627,31 @@
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="72" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L9" s="72" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="N9" s="46" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="O9" s="56" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="P9" s="40" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Q9" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="R9" s="40" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="S9" s="40" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -2685,31 +2682,31 @@
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="72" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="L10" s="72" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="M10" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="N10" s="46" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="O10" s="13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="P10" s="40" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="Q10" s="56" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="R10" s="40" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="S10" s="40" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -2739,28 +2736,28 @@
       <c r="J11" s="1"/>
       <c r="K11" s="56"/>
       <c r="L11" s="72" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="M11" s="78" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N11" s="42" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O11" s="13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P11" s="40" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Q11" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="R11" s="40" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="S11" s="40" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -2784,33 +2781,33 @@
         <v>41</v>
       </c>
       <c r="I12" s="62" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="56"/>
       <c r="L12" s="13" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M12" s="72" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="N12" s="46" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="O12" s="56" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="P12" s="42" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Q12" s="13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="R12" s="65" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="S12" s="42" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -2834,33 +2831,33 @@
         <v>41</v>
       </c>
       <c r="I13" s="62" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="56"/>
       <c r="L13" s="72" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="M13" s="72" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N13" s="42" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="O13" s="13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="P13" s="65" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q13" s="13" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="R13" s="40" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="S13" s="42" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -2884,31 +2881,31 @@
         <v>215</v>
       </c>
       <c r="I14" s="62" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="56"/>
       <c r="L14" s="56"/>
       <c r="M14" s="56" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="N14" s="42" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O14" s="56" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="P14" s="65" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Q14" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="R14" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="S14" s="40" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -2938,19 +2935,19 @@
       <c r="K15" s="56"/>
       <c r="L15" s="56"/>
       <c r="M15" s="72" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="N15" s="40" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O15" s="7"/>
       <c r="P15" s="42"/>
       <c r="Q15" s="7"/>
       <c r="R15" s="65" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="S15" s="40" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -2980,14 +2977,14 @@
       <c r="K16" s="56"/>
       <c r="L16" s="56"/>
       <c r="M16" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="N16" s="42"/>
       <c r="O16" s="7"/>
       <c r="P16" s="42"/>
       <c r="Q16" s="7"/>
       <c r="R16" s="65" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="S16" s="30"/>
     </row>
@@ -3013,7 +3010,7 @@
       <c r="P17" s="42"/>
       <c r="Q17" s="14"/>
       <c r="R17" s="65" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="S17" s="30"/>
     </row>
@@ -3151,7 +3148,7 @@
         <v>221</v>
       </c>
       <c r="I21" s="62" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="J21" s="50" t="s">
         <v>17</v>
@@ -3235,7 +3232,7 @@
         <v>6</v>
       </c>
       <c r="U23" s="64" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3359,7 +3356,7 @@
       <c r="G27" s="9"/>
       <c r="J27" s="10"/>
       <c r="K27" s="71" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L27" s="69" t="s">
         <v>236</v>
@@ -3371,19 +3368,19 @@
         <v>245</v>
       </c>
       <c r="O27" s="44" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="P27" s="67" t="s">
         <v>254</v>
       </c>
       <c r="Q27" s="44" t="s">
+        <v>264</v>
+      </c>
+      <c r="R27" s="67" t="s">
         <v>265</v>
       </c>
-      <c r="R27" s="67" t="s">
-        <v>266</v>
-      </c>
       <c r="S27" s="44" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="T27" s="52"/>
     </row>
@@ -3406,7 +3403,7 @@
       <c r="G28" s="9"/>
       <c r="H28" s="5"/>
       <c r="K28" s="65" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="L28" s="70" t="s">
         <v>238</v>
@@ -3421,16 +3418,16 @@
         <v>256</v>
       </c>
       <c r="P28" s="68" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Q28" s="42" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="R28" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="S28" s="40" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="T28" s="52"/>
     </row>
@@ -3452,7 +3449,7 @@
       </c>
       <c r="J29" s="10"/>
       <c r="K29" s="65" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="L29" s="70" t="s">
         <v>239</v>
@@ -3467,16 +3464,16 @@
         <v>257</v>
       </c>
       <c r="P29" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q29" s="46" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="R29" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="S29" s="40" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="T29" s="52"/>
     </row>
@@ -3498,31 +3495,31 @@
       </c>
       <c r="J30" s="10"/>
       <c r="K30" s="65" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="L30" s="70" t="s">
         <v>240</v>
       </c>
       <c r="M30" s="65" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="N30" s="70" t="s">
         <v>251</v>
       </c>
-      <c r="O30" s="40" t="s">
-        <v>258</v>
+      <c r="O30" s="65" t="s">
+        <v>255</v>
       </c>
       <c r="P30" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q30" s="40" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="R30" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="S30" s="40" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T30" s="52"/>
     </row>
@@ -3550,23 +3547,23 @@
         <v>242</v>
       </c>
       <c r="M31" s="65" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="N31" s="80" t="s">
-        <v>408</v>
-      </c>
-      <c r="O31" s="65" t="s">
-        <v>255</v>
+        <v>407</v>
+      </c>
+      <c r="O31" s="42" t="s">
+        <v>396</v>
       </c>
       <c r="P31" s="15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Q31" s="42"/>
       <c r="R31" s="14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="S31" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="T31" s="52"/>
     </row>
@@ -3599,18 +3596,16 @@
       <c r="N32" s="70" t="s">
         <v>252</v>
       </c>
-      <c r="O32" s="42" t="s">
-        <v>397</v>
-      </c>
+      <c r="O32" s="30"/>
       <c r="P32" s="15" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="Q32" s="42"/>
       <c r="R32" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="S32" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="T32" s="52"/>
     </row>
@@ -3622,13 +3617,13 @@
       <c r="E33" s="8"/>
       <c r="J33" s="10"/>
       <c r="K33" s="65" t="s">
+        <v>395</v>
+      </c>
+      <c r="L33" s="70" t="s">
         <v>396</v>
       </c>
-      <c r="L33" s="70" t="s">
-        <v>397</v>
-      </c>
       <c r="M33" s="65" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="N33" s="70" t="s">
         <v>253</v>
@@ -3638,7 +3633,7 @@
       <c r="Q33" s="42"/>
       <c r="R33" s="14"/>
       <c r="S33" s="42" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -3659,16 +3654,16 @@
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="65" t="s">
+        <v>398</v>
+      </c>
+      <c r="L34" s="70" t="s">
         <v>399</v>
       </c>
-      <c r="L34" s="70" t="s">
-        <v>400</v>
-      </c>
       <c r="M34" s="65" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="N34" s="70" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="O34" s="42"/>
       <c r="P34" s="15"/>
@@ -3696,7 +3691,7 @@
       <c r="L35" s="14"/>
       <c r="M35" s="45"/>
       <c r="N35" s="70" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="O35" s="43"/>
       <c r="P35" s="15"/>
@@ -3791,7 +3786,7 @@
         <v>530</v>
       </c>
       <c r="U37" s="64" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="38" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12721,7 +12716,7 @@
     </row>
     <row r="590" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A590" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B590" s="23" t="s">
         <v>11</v>
@@ -13484,7 +13479,7 @@
     </row>
     <row r="638" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A638" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B638" s="23" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Asset list update & fix bulletholes en flechette
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="410">
   <si>
     <t>ID Code</t>
   </si>
@@ -1244,6 +1244,9 @@
   </si>
   <si>
     <t>Weapons_AbstractGrenades (30)</t>
+  </si>
+  <si>
+    <t>Weapins_Harpoongun (50)</t>
   </si>
 </sst>
 </file>
@@ -1572,7 +1575,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1806,6 +1809,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2126,7 +2132,7 @@
   <dimension ref="A1:U1029"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P42" sqref="P42"/>
+      <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3506,8 +3512,8 @@
       <c r="N30" s="70" t="s">
         <v>251</v>
       </c>
-      <c r="O30" s="65" t="s">
-        <v>255</v>
+      <c r="O30" s="81" t="s">
+        <v>409</v>
       </c>
       <c r="P30" s="14" t="s">
         <v>262</v>
@@ -3552,8 +3558,8 @@
       <c r="N31" s="80" t="s">
         <v>407</v>
       </c>
-      <c r="O31" s="42" t="s">
-        <v>396</v>
+      <c r="O31" s="65" t="s">
+        <v>255</v>
       </c>
       <c r="P31" s="15" t="s">
         <v>268</v>
@@ -3596,7 +3602,7 @@
       <c r="N32" s="70" t="s">
         <v>252</v>
       </c>
-      <c r="O32" s="30"/>
+      <c r="O32" s="42"/>
       <c r="P32" s="15" t="s">
         <v>396</v>
       </c>

</xml_diff>

<commit_message>
Update Imports and Stuff namen etc
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -2132,7 +2132,7 @@
   <dimension ref="A1:U1029"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2371,7 +2371,7 @@
       <c r="N4" s="42" t="s">
         <v>304</v>
       </c>
-      <c r="O4" s="70" t="s">
+      <c r="O4" s="14" t="s">
         <v>321</v>
       </c>
       <c r="P4" s="40" t="s">
@@ -2431,7 +2431,7 @@
       <c r="O5" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="P5" s="65" t="s">
+      <c r="P5" s="40" t="s">
         <v>330</v>
       </c>
       <c r="Q5" s="10" t="s">
@@ -2479,7 +2479,7 @@
       <c r="L6" s="72" t="s">
         <v>292</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="M6" s="72" t="s">
         <v>296</v>
       </c>
       <c r="N6" s="42" t="s">
@@ -2536,7 +2536,7 @@
       <c r="L7" s="56" t="s">
         <v>293</v>
       </c>
-      <c r="M7" s="13" t="s">
+      <c r="M7" s="72" t="s">
         <v>297</v>
       </c>
       <c r="N7" s="42" t="s">
@@ -2596,7 +2596,7 @@
       <c r="M8" s="13" t="s">
         <v>353</v>
       </c>
-      <c r="N8" s="65" t="s">
+      <c r="N8" s="40" t="s">
         <v>309</v>
       </c>
       <c r="O8" s="56" t="s">
@@ -2611,7 +2611,7 @@
       <c r="R8" s="40" t="s">
         <v>362</v>
       </c>
-      <c r="S8" s="65" t="s">
+      <c r="S8" s="40" t="s">
         <v>378</v>
       </c>
     </row>
@@ -2794,7 +2794,7 @@
       <c r="L12" s="13" t="s">
         <v>392</v>
       </c>
-      <c r="M12" s="72" t="s">
+      <c r="M12" s="13" t="s">
         <v>301</v>
       </c>
       <c r="N12" s="46" t="s">
@@ -2809,7 +2809,7 @@
       <c r="Q12" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="R12" s="65" t="s">
+      <c r="R12" s="40" t="s">
         <v>336</v>
       </c>
       <c r="S12" s="42" t="s">
@@ -2844,7 +2844,7 @@
       <c r="L13" s="72" t="s">
         <v>284</v>
       </c>
-      <c r="M13" s="72" t="s">
+      <c r="M13" s="13" t="s">
         <v>302</v>
       </c>
       <c r="N13" s="42" t="s">
@@ -2853,7 +2853,7 @@
       <c r="O13" s="13" t="s">
         <v>327</v>
       </c>
-      <c r="P13" s="65" t="s">
+      <c r="P13" s="40" t="s">
         <v>335</v>
       </c>
       <c r="Q13" s="13" t="s">
@@ -2901,7 +2901,7 @@
       <c r="O14" s="56" t="s">
         <v>338</v>
       </c>
-      <c r="P14" s="65" t="s">
+      <c r="P14" s="40" t="s">
         <v>337</v>
       </c>
       <c r="Q14" s="13" t="s">
@@ -2940,7 +2940,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="56"/>
       <c r="L15" s="56"/>
-      <c r="M15" s="72" t="s">
+      <c r="M15" s="13" t="s">
         <v>352</v>
       </c>
       <c r="N15" s="40" t="s">
@@ -2949,7 +2949,7 @@
       <c r="O15" s="7"/>
       <c r="P15" s="42"/>
       <c r="Q15" s="7"/>
-      <c r="R15" s="65" t="s">
+      <c r="R15" s="40" t="s">
         <v>371</v>
       </c>
       <c r="S15" s="40" t="s">
@@ -2989,7 +2989,7 @@
       <c r="O16" s="7"/>
       <c r="P16" s="42"/>
       <c r="Q16" s="7"/>
-      <c r="R16" s="65" t="s">
+      <c r="R16" s="40" t="s">
         <v>372</v>
       </c>
       <c r="S16" s="30"/>
@@ -3015,7 +3015,7 @@
       <c r="O17" s="7"/>
       <c r="P17" s="42"/>
       <c r="Q17" s="14"/>
-      <c r="R17" s="65" t="s">
+      <c r="R17" s="40" t="s">
         <v>373</v>
       </c>
       <c r="S17" s="30"/>

</xml_diff>

<commit_message>
Sprint 3 alle imports en name changes
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -1575,7 +1575,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1800,9 +1800,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2132,7 +2129,7 @@
   <dimension ref="A1:U1029"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2302,13 +2299,13 @@
         <v>228</v>
       </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="79" t="s">
+      <c r="K3" s="78" t="s">
         <v>281</v>
       </c>
-      <c r="L3" s="79" t="s">
+      <c r="L3" s="78" t="s">
         <v>289</v>
       </c>
-      <c r="M3" s="79" t="s">
+      <c r="M3" s="78" t="s">
         <v>390</v>
       </c>
       <c r="N3" s="61" t="s">
@@ -2536,7 +2533,7 @@
       <c r="L7" s="56" t="s">
         <v>293</v>
       </c>
-      <c r="M7" s="72" t="s">
+      <c r="M7" s="13" t="s">
         <v>297</v>
       </c>
       <c r="N7" s="42" t="s">
@@ -2638,7 +2635,7 @@
       <c r="L9" s="72" t="s">
         <v>388</v>
       </c>
-      <c r="M9" s="13" t="s">
+      <c r="M9" s="72" t="s">
         <v>298</v>
       </c>
       <c r="N9" s="46" t="s">
@@ -2693,7 +2690,7 @@
       <c r="L10" s="72" t="s">
         <v>389</v>
       </c>
-      <c r="M10" s="13" t="s">
+      <c r="M10" s="72" t="s">
         <v>299</v>
       </c>
       <c r="N10" s="46" t="s">
@@ -2744,7 +2741,7 @@
       <c r="L11" s="72" t="s">
         <v>391</v>
       </c>
-      <c r="M11" s="78" t="s">
+      <c r="M11" s="72" t="s">
         <v>300</v>
       </c>
       <c r="N11" s="42" t="s">
@@ -2794,7 +2791,7 @@
       <c r="L12" s="13" t="s">
         <v>392</v>
       </c>
-      <c r="M12" s="13" t="s">
+      <c r="M12" s="72" t="s">
         <v>301</v>
       </c>
       <c r="N12" s="46" t="s">
@@ -2844,7 +2841,7 @@
       <c r="L13" s="72" t="s">
         <v>284</v>
       </c>
-      <c r="M13" s="13" t="s">
+      <c r="M13" s="72" t="s">
         <v>302</v>
       </c>
       <c r="N13" s="42" t="s">
@@ -2892,7 +2889,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="56"/>
       <c r="L14" s="56"/>
-      <c r="M14" s="56" t="s">
+      <c r="M14" s="72" t="s">
         <v>306</v>
       </c>
       <c r="N14" s="42" t="s">
@@ -2940,7 +2937,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="56"/>
       <c r="L15" s="56"/>
-      <c r="M15" s="13" t="s">
+      <c r="M15" s="72" t="s">
         <v>352</v>
       </c>
       <c r="N15" s="40" t="s">
@@ -3512,7 +3509,7 @@
       <c r="N30" s="70" t="s">
         <v>251</v>
       </c>
-      <c r="O30" s="81" t="s">
+      <c r="O30" s="80" t="s">
         <v>409</v>
       </c>
       <c r="P30" s="14" t="s">
@@ -3555,7 +3552,7 @@
       <c r="M31" s="65" t="s">
         <v>400</v>
       </c>
-      <c r="N31" s="80" t="s">
+      <c r="N31" s="79" t="s">
         <v>407</v>
       </c>
       <c r="O31" s="65" t="s">

</xml_diff>

<commit_message>
Sprint 4 Exports en rename
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -2129,7 +2129,7 @@
   <dimension ref="A1:U1029"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2422,7 +2422,7 @@
       <c r="M5" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="N5" s="42" t="s">
+      <c r="N5" s="65" t="s">
         <v>305</v>
       </c>
       <c r="O5" s="15" t="s">
@@ -2479,7 +2479,7 @@
       <c r="M6" s="72" t="s">
         <v>296</v>
       </c>
-      <c r="N6" s="42" t="s">
+      <c r="N6" s="65" t="s">
         <v>307</v>
       </c>
       <c r="O6" s="15" t="s">
@@ -2536,7 +2536,7 @@
       <c r="M7" s="13" t="s">
         <v>297</v>
       </c>
-      <c r="N7" s="42" t="s">
+      <c r="N7" s="65" t="s">
         <v>308</v>
       </c>
       <c r="O7" s="56" t="s">
@@ -2638,7 +2638,7 @@
       <c r="M9" s="72" t="s">
         <v>298</v>
       </c>
-      <c r="N9" s="46" t="s">
+      <c r="N9" s="65" t="s">
         <v>310</v>
       </c>
       <c r="O9" s="56" t="s">
@@ -2693,7 +2693,7 @@
       <c r="M10" s="72" t="s">
         <v>299</v>
       </c>
-      <c r="N10" s="46" t="s">
+      <c r="N10" s="65" t="s">
         <v>311</v>
       </c>
       <c r="O10" s="13" t="s">
@@ -2744,7 +2744,7 @@
       <c r="M11" s="72" t="s">
         <v>300</v>
       </c>
-      <c r="N11" s="42" t="s">
+      <c r="N11" s="65" t="s">
         <v>313</v>
       </c>
       <c r="O11" s="13" t="s">
@@ -2892,7 +2892,7 @@
       <c r="M14" s="72" t="s">
         <v>306</v>
       </c>
-      <c r="N14" s="42" t="s">
+      <c r="N14" s="65" t="s">
         <v>319</v>
       </c>
       <c r="O14" s="56" t="s">

</xml_diff>

<commit_message>
Sprint 5 Alle assets import en rename
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -2129,7 +2129,7 @@
   <dimension ref="A1:U1029"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2311,7 +2311,7 @@
       <c r="N3" s="61" t="s">
         <v>303</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="79" t="s">
         <v>320</v>
       </c>
       <c r="P3" s="41" t="s">
@@ -2368,7 +2368,7 @@
       <c r="N4" s="42" t="s">
         <v>304</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="O4" s="70" t="s">
         <v>321</v>
       </c>
       <c r="P4" s="40" t="s">
@@ -2641,7 +2641,7 @@
       <c r="N9" s="65" t="s">
         <v>310</v>
       </c>
-      <c r="O9" s="56" t="s">
+      <c r="O9" s="72" t="s">
         <v>312</v>
       </c>
       <c r="P9" s="40" t="s">
@@ -2797,7 +2797,7 @@
       <c r="N12" s="46" t="s">
         <v>318</v>
       </c>
-      <c r="O12" s="56" t="s">
+      <c r="O12" s="72" t="s">
         <v>326</v>
       </c>
       <c r="P12" s="42" t="s">
@@ -2847,7 +2847,7 @@
       <c r="N13" s="42" t="s">
         <v>317</v>
       </c>
-      <c r="O13" s="13" t="s">
+      <c r="O13" s="72" t="s">
         <v>327</v>
       </c>
       <c r="P13" s="40" t="s">

</xml_diff>

<commit_message>
Sprint 6 Alle Assets tot nu import en rename in unity
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -2128,8 +2128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,7 +2314,7 @@
       <c r="O3" s="79" t="s">
         <v>320</v>
       </c>
-      <c r="P3" s="41" t="s">
+      <c r="P3" s="71" t="s">
         <v>328</v>
       </c>
       <c r="Q3" s="10" t="s">
@@ -2428,7 +2428,7 @@
       <c r="O5" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="P5" s="40" t="s">
+      <c r="P5" s="65" t="s">
         <v>330</v>
       </c>
       <c r="Q5" s="10" t="s">
@@ -2485,7 +2485,7 @@
       <c r="O6" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="P6" s="40" t="s">
+      <c r="P6" s="65" t="s">
         <v>331</v>
       </c>
       <c r="Q6" s="7" t="s">
@@ -2850,7 +2850,7 @@
       <c r="O13" s="72" t="s">
         <v>327</v>
       </c>
-      <c r="P13" s="40" t="s">
+      <c r="P13" s="65" t="s">
         <v>335</v>
       </c>
       <c r="Q13" s="13" t="s">

</xml_diff>

<commit_message>
Imports eindelijk done wat we tot nu toe hebben
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -2126,7 +2126,7 @@
   <dimension ref="A1:U1029"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2596,7 +2596,7 @@
       <c r="O8" s="55" t="s">
         <v>315</v>
       </c>
-      <c r="P8" s="40" t="s">
+      <c r="P8" s="64" t="s">
         <v>348</v>
       </c>
       <c r="Q8" s="78" t="s">

</xml_diff>

<commit_message>
Import Assets Ruben en kevin
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -1811,7 +1811,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2131,8 +2131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2377,7 +2377,7 @@
       <c r="P4" s="40" t="s">
         <v>329</v>
       </c>
-      <c r="Q4" s="81" t="s">
+      <c r="Q4" s="78" t="s">
         <v>342</v>
       </c>
       <c r="R4" s="64" t="s">
@@ -2422,7 +2422,7 @@
       <c r="L5" s="71" t="s">
         <v>291</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="M5" s="71" t="s">
         <v>295</v>
       </c>
       <c r="N5" s="64" t="s">
@@ -2708,7 +2708,7 @@
       <c r="Q10" s="71" t="s">
         <v>354</v>
       </c>
-      <c r="R10" s="40" t="s">
+      <c r="R10" s="81" t="s">
         <v>367</v>
       </c>
       <c r="S10" s="40" t="s">

</xml_diff>

<commit_message>
Imports en namechanges porject opschonen
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -1575,7 +1575,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1811,7 +1811,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2132,7 +2135,7 @@
   <dimension ref="A1:U1029"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2368,7 +2371,7 @@
       <c r="M4" s="71" t="s">
         <v>294</v>
       </c>
-      <c r="N4" s="41" t="s">
+      <c r="N4" s="81" t="s">
         <v>304</v>
       </c>
       <c r="O4" s="69" t="s">
@@ -2428,7 +2431,7 @@
       <c r="N5" s="64" t="s">
         <v>305</v>
       </c>
-      <c r="O5" s="15" t="s">
+      <c r="O5" s="82" t="s">
         <v>322</v>
       </c>
       <c r="P5" s="64" t="s">

</xml_diff>

<commit_message>
Imports af maar trello doet het niet dus moet nog sprint 6,7,8,9 controleren
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -1575,7 +1575,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1809,12 +1809,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2134,8 +2128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2371,7 +2365,7 @@
       <c r="M4" s="71" t="s">
         <v>294</v>
       </c>
-      <c r="N4" s="81" t="s">
+      <c r="N4" s="64" t="s">
         <v>304</v>
       </c>
       <c r="O4" s="69" t="s">
@@ -2431,7 +2425,7 @@
       <c r="N5" s="64" t="s">
         <v>305</v>
       </c>
-      <c r="O5" s="82" t="s">
+      <c r="O5" s="69" t="s">
         <v>322</v>
       </c>
       <c r="P5" s="64" t="s">
@@ -2494,7 +2488,7 @@
       <c r="P6" s="64" t="s">
         <v>331</v>
       </c>
-      <c r="Q6" s="7" t="s">
+      <c r="Q6" s="78" t="s">
         <v>344</v>
       </c>
       <c r="R6" s="40" t="s">
@@ -2605,7 +2599,7 @@
       <c r="O8" s="55" t="s">
         <v>315</v>
       </c>
-      <c r="P8" s="64" t="s">
+      <c r="P8" s="40" t="s">
         <v>348</v>
       </c>
       <c r="Q8" s="78" t="s">
@@ -2711,7 +2705,7 @@
       <c r="Q10" s="71" t="s">
         <v>354</v>
       </c>
-      <c r="R10" s="81" t="s">
+      <c r="R10" s="64" t="s">
         <v>367</v>
       </c>
       <c r="S10" s="40" t="s">
@@ -3376,7 +3370,7 @@
       <c r="N27" s="68" t="s">
         <v>245</v>
       </c>
-      <c r="O27" s="43" t="s">
+      <c r="O27" s="70" t="s">
         <v>259</v>
       </c>
       <c r="P27" s="66" t="s">
@@ -3423,7 +3417,7 @@
       <c r="N28" s="69" t="s">
         <v>248</v>
       </c>
-      <c r="O28" s="45" t="s">
+      <c r="O28" s="64" t="s">
         <v>256</v>
       </c>
       <c r="P28" s="67" t="s">
@@ -3469,7 +3463,7 @@
       <c r="N29" s="69" t="s">
         <v>249</v>
       </c>
-      <c r="O29" s="45" t="s">
+      <c r="O29" s="64" t="s">
         <v>257</v>
       </c>
       <c r="P29" s="14" t="s">

</xml_diff>

<commit_message>
Import Teleporter en update asset list
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$A$1:$E$674</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -1912,6 +1912,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1947,6 +1964,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -2126,7 +2160,7 @@
   <dimension ref="A1:U1029"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2428,7 +2462,7 @@
       <c r="P5" s="64" t="s">
         <v>330</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="Q5" s="77" t="s">
         <v>343</v>
       </c>
       <c r="R5" s="41" t="s">

</xml_diff>

<commit_message>
Import Ai Room & Import MedBay
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -2159,8 +2159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2402,7 +2402,7 @@
       <c r="O4" s="68" t="s">
         <v>321</v>
       </c>
-      <c r="P4" s="40" t="s">
+      <c r="P4" s="64" t="s">
         <v>329</v>
       </c>
       <c r="Q4" s="77" t="s">
@@ -2561,7 +2561,7 @@
       <c r="K7" s="70" t="s">
         <v>285</v>
       </c>
-      <c r="L7" s="55" t="s">
+      <c r="L7" s="70" t="s">
         <v>293</v>
       </c>
       <c r="M7" s="70" t="s">
@@ -2630,7 +2630,7 @@
       <c r="O8" s="55" t="s">
         <v>315</v>
       </c>
-      <c r="P8" s="40" t="s">
+      <c r="P8" s="64" t="s">
         <v>348</v>
       </c>
       <c r="Q8" s="77" t="s">

</xml_diff>

<commit_message>
Import Water purification & Plants
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -2159,8 +2159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2579,7 +2579,7 @@
       <c r="Q7" s="77" t="s">
         <v>345</v>
       </c>
-      <c r="R7" s="40" t="s">
+      <c r="R7" s="64" t="s">
         <v>361</v>
       </c>
       <c r="S7" s="40" t="s">
@@ -2727,7 +2727,7 @@
       <c r="N10" s="64" t="s">
         <v>311</v>
       </c>
-      <c r="O10" s="13" t="s">
+      <c r="O10" s="70" t="s">
         <v>324</v>
       </c>
       <c r="P10" s="40" t="s">

</xml_diff>

<commit_message>
Asset list en Presentatie start
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
+++ b/Algemeen/Asset List/Asset List Game-Lab-2.1.xlsx
@@ -2159,8 +2159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3146,19 +3146,35 @@
         <v>19</v>
       </c>
       <c r="K20" s="28">
-        <v>6</v>
-      </c>
-      <c r="L20" s="30"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="29"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="30"/>
-      <c r="S20" s="32"/>
+        <v>63</v>
+      </c>
+      <c r="L20" s="30">
+        <v>98</v>
+      </c>
+      <c r="M20" s="31">
+        <v>86</v>
+      </c>
+      <c r="N20" s="30">
+        <v>89</v>
+      </c>
+      <c r="O20" s="29">
+        <v>146</v>
+      </c>
+      <c r="P20" s="27">
+        <v>76</v>
+      </c>
+      <c r="Q20" s="29">
+        <v>128</v>
+      </c>
+      <c r="R20" s="30">
+        <v>100</v>
+      </c>
+      <c r="S20" s="32">
+        <v>30</v>
+      </c>
       <c r="T20" s="48">
         <f>K20+L20+M20+N20+O20+P20+Q20+R20+S20</f>
-        <v>6</v>
+        <v>816</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -3187,18 +3203,36 @@
       <c r="J21" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="K21" s="21"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="31"/>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="31"/>
-      <c r="R21" s="30"/>
-      <c r="S21" s="32"/>
+      <c r="K21" s="21">
+        <v>98</v>
+      </c>
+      <c r="L21" s="30">
+        <v>35</v>
+      </c>
+      <c r="M21" s="31">
+        <v>20</v>
+      </c>
+      <c r="N21" s="30">
+        <v>0</v>
+      </c>
+      <c r="O21" s="31">
+        <v>0</v>
+      </c>
+      <c r="P21" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="31">
+        <v>0</v>
+      </c>
+      <c r="R21" s="30">
+        <v>22</v>
+      </c>
+      <c r="S21" s="32">
+        <v>0</v>
+      </c>
       <c r="T21" s="49">
         <f>K21+L21+M21+N21+O21+P21+Q21+R21+S21</f>
-        <v>0</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3221,18 +3255,36 @@
       <c r="J22" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="K22" s="25"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="34"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="34"/>
-      <c r="R22" s="33"/>
-      <c r="S22" s="35"/>
+      <c r="K22" s="25">
+        <v>48</v>
+      </c>
+      <c r="L22" s="33">
+        <v>81</v>
+      </c>
+      <c r="M22" s="34">
+        <v>106</v>
+      </c>
+      <c r="N22" s="33">
+        <v>50</v>
+      </c>
+      <c r="O22" s="34">
+        <v>20</v>
+      </c>
+      <c r="P22" s="33">
+        <v>50</v>
+      </c>
+      <c r="Q22" s="34">
+        <v>0</v>
+      </c>
+      <c r="R22" s="33">
+        <v>0</v>
+      </c>
+      <c r="S22" s="35">
+        <v>0</v>
+      </c>
       <c r="T22" s="49">
         <f>K22+L22+M22+N22+O22+P22+Q22+R22+S22</f>
-        <v>0</v>
+        <v>355</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3263,7 +3315,7 @@
       <c r="R23" s="31"/>
       <c r="T23" s="62">
         <f>T20+T21+T22</f>
-        <v>6</v>
+        <v>1346</v>
       </c>
       <c r="U23" s="63" t="s">
         <v>364</v>
@@ -3497,7 +3549,7 @@
       <c r="O29" s="64" t="s">
         <v>257</v>
       </c>
-      <c r="P29" s="14" t="s">
+      <c r="P29" s="68" t="s">
         <v>261</v>
       </c>
       <c r="Q29" s="45" t="s">
@@ -3543,7 +3595,7 @@
       <c r="O30" s="78" t="s">
         <v>409</v>
       </c>
-      <c r="P30" s="14" t="s">
+      <c r="P30" s="68" t="s">
         <v>262</v>
       </c>
       <c r="Q30" s="40" t="s">
@@ -3770,7 +3822,9 @@
       <c r="O36" s="27">
         <v>20</v>
       </c>
-      <c r="P36" s="27"/>
+      <c r="P36" s="27">
+        <v>0</v>
+      </c>
       <c r="Q36" s="27"/>
       <c r="R36" s="27"/>
       <c r="S36" s="27"/>
@@ -3810,14 +3864,18 @@
       <c r="N37" s="33">
         <v>170</v>
       </c>
-      <c r="O37" s="33"/>
-      <c r="P37" s="33"/>
+      <c r="O37" s="33">
+        <v>190</v>
+      </c>
+      <c r="P37" s="33">
+        <v>100</v>
+      </c>
       <c r="Q37" s="33"/>
       <c r="R37" s="33"/>
       <c r="S37" s="33"/>
       <c r="T37" s="57">
         <f>K37+L37+M37+N37+O37+P37+Q37+R37+S37</f>
-        <v>530</v>
+        <v>820</v>
       </c>
       <c r="U37" s="63" t="s">
         <v>365</v>
@@ -3844,7 +3902,7 @@
       <c r="R38" s="31"/>
       <c r="T38" s="63">
         <f>T36+T37</f>
-        <v>1135</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>